<commit_message>
updated checklist and few commands
</commit_message>
<xml_diff>
--- a/Checklist.xlsx
+++ b/Checklist.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Prashant\AziraPowershellscript\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MO\Powershell\Project\AziraPowershellscript2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82232A58-B879-445F-81AF-9BC45BBC20E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Application" sheetId="1" r:id="rId1"/>
@@ -30,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="274">
   <si>
     <t xml:space="preserve"> Last Updated</t>
   </si>
@@ -923,12 +922,6 @@
     <t>C:\DB\MSSQL11.MSSQLSERVER\MSSQL\DATA\ReportServerTempDB.mdf</t>
   </si>
   <si>
-    <t>ReportServerDatabase TempDB PhysicalLogfile</t>
-  </si>
-  <si>
-    <t>Path</t>
-  </si>
-  <si>
     <t>C:\DB\MSSQL11.MSSQLSERVER\MSSQL\DATA\ReportServerTempDB_log.ldf</t>
   </si>
   <si>
@@ -1011,13 +1004,29 @@
   </si>
   <si>
     <t>DONE</t>
+  </si>
+  <si>
+    <t>ReportServerDatabase TempDB PhysicalLogfile Path</t>
+  </si>
+  <si>
+    <t>Remarks</t>
+  </si>
+  <si>
+    <t>Partial Done</t>
+  </si>
+  <si>
+    <t>Got the commands but haven't comitted the script</t>
+  </si>
+  <si>
+    <t>Partially 
+Done</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1065,6 +1074,14 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -1097,7 +1114,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -1288,12 +1305,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFDBDBDE"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1411,6 +1437,18 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
@@ -1476,6 +1514,13 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1515,7 +1560,7 @@
         <xdr:cNvPr id="14" name="Picture 92361">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000E000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1562,13 +1607,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>4</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>4</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1576,7 +1621,7 @@
         <xdr:cNvPr id="15" name="Picture 92362">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000F000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1884,47 +1929,48 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:F42"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E11" sqref="E11"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="51" customWidth="1"/>
-    <col min="4" max="4" width="74.44140625" customWidth="1"/>
-    <col min="6" max="6" width="11.44140625" customWidth="1"/>
+    <col min="4" max="4" width="74.42578125" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="41"/>
+    <col min="6" max="6" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="40" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C1" s="40" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D1" s="40" t="s">
-        <v>267</v>
-      </c>
-      <c r="E1" s="40" t="s">
+        <v>265</v>
+      </c>
+      <c r="E1" s="42" t="s">
         <v>48</v>
       </c>
       <c r="F1" s="40" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="41" t="s">
+    <row r="2" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-    </row>
-    <row r="3" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+    </row>
+    <row r="3" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="13">
         <v>1</v>
       </c>
@@ -1935,7 +1981,7 @@
         <v>44102</v>
       </c>
     </row>
-    <row r="4" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="11">
         <v>2</v>
       </c>
@@ -1946,396 +1992,424 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="6" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="50" t="s">
+    <row r="5" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="51"/>
-      <c r="D6" s="51"/>
-    </row>
-    <row r="7" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B7" s="14">
+      <c r="C5" s="55"/>
+      <c r="D5" s="55"/>
+    </row>
+    <row r="6" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B6" s="14">
         <v>3</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C6" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="48" t="s">
+      <c r="D6" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="E7" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="1"/>
-      <c r="C8" s="7" t="s">
+      <c r="E6" s="44" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="1"/>
+      <c r="C7" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="46"/>
-    </row>
-    <row r="9" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B9" s="12">
+      <c r="D7" s="50"/>
+      <c r="E7" s="44"/>
+    </row>
+    <row r="8" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B8" s="12">
         <v>4</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C8" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="43" t="s">
+      <c r="D8" s="47" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="2:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="1"/>
-      <c r="C10" s="9" t="s">
+      <c r="E8" s="44"/>
+    </row>
+    <row r="9" spans="2:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="1"/>
+      <c r="C9" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="47"/>
-    </row>
-    <row r="11" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B11" s="14">
+      <c r="D9" s="51"/>
+      <c r="E9" s="44"/>
+    </row>
+    <row r="10" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B10" s="14">
         <v>5</v>
       </c>
-      <c r="C11" s="16" t="s">
+      <c r="C10" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="48" t="s">
+      <c r="D10" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="E11" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="5"/>
-      <c r="C12" s="17" t="s">
-        <v>265</v>
-      </c>
-      <c r="D12" s="49"/>
-    </row>
-    <row r="13" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B13" s="12">
+      <c r="E10" s="44" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="5"/>
+      <c r="C11" s="17" t="s">
+        <v>263</v>
+      </c>
+      <c r="D11" s="53"/>
+      <c r="E11" s="44"/>
+    </row>
+    <row r="12" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B12" s="12">
         <v>6</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C12" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="43" t="s">
+      <c r="D12" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="E13" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="5"/>
-      <c r="C14" s="18" t="s">
-        <v>265</v>
-      </c>
-      <c r="D14" s="44"/>
-    </row>
-    <row r="15" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B15" s="12">
+      <c r="E12" s="44" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="5"/>
+      <c r="C13" s="18" t="s">
+        <v>263</v>
+      </c>
+      <c r="D13" s="48"/>
+      <c r="E13" s="44"/>
+    </row>
+    <row r="14" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B14" s="12">
         <v>7</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C14" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D15" s="45" t="s">
+      <c r="D14" s="49" t="s">
         <v>14</v>
       </c>
-      <c r="E15" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="1"/>
-      <c r="C16" s="7" t="s">
+      <c r="E14" s="44" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="1"/>
+      <c r="C15" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="46"/>
-    </row>
-    <row r="17" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B17" s="12">
+      <c r="D15" s="50"/>
+      <c r="E15" s="44"/>
+    </row>
+    <row r="16" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B16" s="12">
         <v>8</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C16" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="43" t="s">
+      <c r="D16" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="E17" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="1"/>
-      <c r="C18" s="9" t="s">
+      <c r="E16" s="44" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="1"/>
+      <c r="C17" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D18" s="47"/>
-    </row>
-    <row r="19" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B19" s="12">
+      <c r="D17" s="51"/>
+      <c r="E17" s="44"/>
+    </row>
+    <row r="18" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B18" s="12">
         <v>9</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C18" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D19" s="45">
+      <c r="D18" s="49">
         <v>4</v>
       </c>
-    </row>
-    <row r="20" spans="2:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="1"/>
-      <c r="C20" s="7" t="s">
+      <c r="E18" s="44"/>
+    </row>
+    <row r="19" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="1"/>
+      <c r="C19" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D20" s="46"/>
-    </row>
-    <row r="21" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="1">
+      <c r="D19" s="50"/>
+      <c r="E19" s="44"/>
+    </row>
+    <row r="20" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="1">
         <v>10</v>
       </c>
-      <c r="C21" s="19" t="s">
+      <c r="C20" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="D20" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E21" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="22" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C22" s="20" t="s">
+      <c r="E20" s="44" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C21" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D21" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="2:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="12">
+      <c r="E21" s="44"/>
+    </row>
+    <row r="22" spans="2:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="12">
         <v>11</v>
       </c>
-      <c r="C23" s="8" t="s">
+      <c r="C22" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D23" s="43" t="s">
+      <c r="D22" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="E23" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="1"/>
-      <c r="C24" s="9" t="s">
+      <c r="E22" s="44" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="1"/>
+      <c r="C23" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="D24" s="47"/>
-    </row>
-    <row r="25" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B25" s="12">
+      <c r="D23" s="51"/>
+      <c r="E23" s="44"/>
+    </row>
+    <row r="24" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B24" s="12">
         <v>12</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="C24" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D25" s="45" t="s">
+      <c r="D24" s="49" t="s">
         <v>28</v>
       </c>
-      <c r="E25" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="26" spans="2:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B26" s="1"/>
-      <c r="C26" s="7" t="s">
+      <c r="E24" s="44" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="1"/>
+      <c r="C25" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="D26" s="46"/>
-    </row>
-    <row r="27" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B27" s="12">
+      <c r="D25" s="50"/>
+      <c r="E25" s="44"/>
+    </row>
+    <row r="26" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B26" s="12">
         <v>13</v>
       </c>
-      <c r="C27" s="8" t="s">
+      <c r="C26" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="D27" s="43" t="s">
+      <c r="D26" s="47" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="28" spans="2:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="1"/>
-      <c r="C28" s="9" t="s">
+      <c r="E26" s="44"/>
+    </row>
+    <row r="27" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="1"/>
+      <c r="C27" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D28" s="47"/>
-    </row>
-    <row r="29" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="12">
+      <c r="D27" s="51"/>
+      <c r="E27" s="44"/>
+    </row>
+    <row r="28" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="12">
         <v>14</v>
       </c>
-      <c r="C29" s="6" t="s">
+      <c r="C28" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="D29" s="45" t="s">
+      <c r="D28" s="49" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="30" spans="2:5" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B30" s="1"/>
-      <c r="C30" s="7" t="s">
+      <c r="E28" s="44"/>
+    </row>
+    <row r="29" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="1"/>
+      <c r="C29" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D30" s="46"/>
-    </row>
-    <row r="31" spans="2:5" ht="32.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B31" s="21">
+      <c r="D29" s="50"/>
+      <c r="E29" s="44"/>
+    </row>
+    <row r="30" spans="2:5" ht="31.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="21">
         <v>15</v>
       </c>
-      <c r="C31" s="23" t="s">
+      <c r="C30" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="D31" s="22" t="s">
+      <c r="D30" s="22" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="32" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="1">
+        <v>16</v>
+      </c>
+      <c r="C31" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="1">
-        <v>16</v>
-      </c>
-      <c r="C32" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="D32" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C32" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="D32" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="33" spans="2:4" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="1">
-        <v>17</v>
-      </c>
-      <c r="C33" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="D33" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C33" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="D33" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="34" spans="2:4" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B34" s="1">
-        <v>18</v>
-      </c>
-      <c r="C34" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="D34" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C34" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="D34" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="35" spans="2:4" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B35" s="1">
-        <v>19</v>
-      </c>
-      <c r="C35" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="D35" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C35" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="1">
+        <v>21</v>
+      </c>
+      <c r="C36" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="D36" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="36" spans="2:4" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B36" s="1">
-        <v>20</v>
-      </c>
-      <c r="C36" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="D36" s="2" t="s">
+    <row r="37" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="1">
+        <v>22</v>
+      </c>
+      <c r="C37" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="1">
+        <v>23</v>
+      </c>
+      <c r="C38" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="1">
+        <v>24</v>
+      </c>
+      <c r="C39" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="D39" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="37" spans="2:4" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B37" s="1">
-        <v>21</v>
-      </c>
-      <c r="C37" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="38" spans="2:4" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B38" s="1">
-        <v>22</v>
-      </c>
-      <c r="C38" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="39" spans="2:4" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B39" s="1">
-        <v>23</v>
-      </c>
-      <c r="C39" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="D39" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="40" spans="2:4" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B40" s="1">
-        <v>24</v>
-      </c>
-      <c r="C40" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="D40" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C40" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="D40" s="4" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="41" spans="2:4" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B41" s="1">
-        <v>25</v>
-      </c>
-      <c r="C41" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="D41" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="42" spans="2:4" s="27" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="C42" s="28" t="s">
+    <row r="41" spans="2:5" s="27" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="C41" s="28" t="s">
         <v>69</v>
       </c>
+      <c r="E41" s="43"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="D19:D20"/>
+  <mergeCells count="25">
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="D18:D19"/>
     <mergeCell ref="B2:D2"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="E14:E15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2344,29 +2418,31 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="3.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="47.44140625" customWidth="1"/>
-    <col min="4" max="4" width="93.33203125" customWidth="1"/>
+    <col min="2" max="2" width="3.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="47.42578125" customWidth="1"/>
+    <col min="4" max="4" width="93.28515625" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E1" t="s">
+    <row r="1" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E1" s="67" t="s">
         <v>48</v>
       </c>
-      <c r="F1" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="2" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F1" s="67" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="2" spans="2:6" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="26">
         <v>26</v>
       </c>
@@ -2376,8 +2452,14 @@
       <c r="D2" s="26" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E2" t="s">
+        <v>271</v>
+      </c>
+      <c r="F2" s="68" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="4">
         <v>27</v>
       </c>
@@ -2387,8 +2469,14 @@
       <c r="D3" s="4" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="4" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E3" t="s">
+        <v>271</v>
+      </c>
+      <c r="F3" s="68" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="2">
         <v>28</v>
       </c>
@@ -2398,8 +2486,14 @@
       <c r="D4" s="2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="5" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E4" t="s">
+        <v>271</v>
+      </c>
+      <c r="F4" s="68" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="4">
         <v>29</v>
       </c>
@@ -2409,8 +2503,14 @@
       <c r="D5" s="4" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="6" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E5" t="s">
+        <v>271</v>
+      </c>
+      <c r="F5" s="68" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="26">
         <v>30</v>
       </c>
@@ -2420,8 +2520,14 @@
       <c r="D6" s="26" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="7" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E6" t="s">
+        <v>271</v>
+      </c>
+      <c r="F6" s="68" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="4">
         <v>31</v>
       </c>
@@ -2431,8 +2537,14 @@
       <c r="D7" s="4" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="8" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E7" t="s">
+        <v>271</v>
+      </c>
+      <c r="F7" s="68" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="2">
         <v>32</v>
       </c>
@@ -2442,75 +2554,81 @@
       <c r="D8" s="2" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="9" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="E8" t="s">
+        <v>271</v>
+      </c>
+      <c r="F8" s="68" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B9" s="10">
         <v>33</v>
       </c>
-      <c r="C9" s="43" t="s">
+      <c r="C9" s="47" t="s">
         <v>61</v>
       </c>
       <c r="D9" s="8" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="10" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="11"/>
-      <c r="C10" s="47"/>
+      <c r="C10" s="51"/>
       <c r="D10" s="4" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="11" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B11" s="24">
         <v>34</v>
       </c>
-      <c r="C11" s="45" t="s">
+      <c r="C11" s="49" t="s">
         <v>64</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="12" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="13"/>
-      <c r="C12" s="46"/>
+      <c r="C12" s="50"/>
       <c r="D12" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B13" s="10">
         <v>35</v>
       </c>
-      <c r="C13" s="43" t="s">
+      <c r="C13" s="47" t="s">
         <v>66</v>
       </c>
       <c r="D13" s="8" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="14" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="11"/>
-      <c r="C14" s="47"/>
+      <c r="C14" s="51"/>
       <c r="D14" s="4" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="15" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B15" s="24">
         <v>36</v>
       </c>
-      <c r="C15" s="45" t="s">
+      <c r="C15" s="49" t="s">
         <v>68</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="13"/>
-      <c r="C16" s="46"/>
+      <c r="C16" s="50"/>
       <c r="D16" s="2" t="s">
         <v>67</v>
       </c>
@@ -2523,1053 +2641,1131 @@
     <mergeCell ref="C11:C12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="B2:F81"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:F80"/>
   <sheetViews>
-    <sheetView topLeftCell="A70" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D74" sqref="D74"/>
+    <sheetView tabSelected="1" topLeftCell="B11" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21:E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="56" customWidth="1"/>
-    <col min="4" max="4" width="108.33203125" customWidth="1"/>
+    <col min="4" max="4" width="108.28515625" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="41"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>177</v>
       </c>
-      <c r="E2" t="s">
-        <v>262</v>
+      <c r="E2" s="41" t="s">
+        <v>260</v>
       </c>
       <c r="F2" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="3" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B3" s="48">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B3" s="52">
         <v>37</v>
       </c>
       <c r="C3" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="48" t="s">
+      <c r="D3" s="52" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="4" spans="2:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="46"/>
+      <c r="E3" s="44" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="50"/>
       <c r="C4" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="D4" s="46"/>
-    </row>
-    <row r="5" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B5" s="43">
+      <c r="D4" s="50"/>
+      <c r="E4" s="44"/>
+    </row>
+    <row r="5" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B5" s="47">
         <v>38</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="43" t="s">
+      <c r="D5" s="47" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="6" spans="2:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="47"/>
+      <c r="E5" s="44" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="51"/>
       <c r="C6" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="D6" s="47"/>
-    </row>
-    <row r="7" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B7" s="45">
+      <c r="D6" s="51"/>
+      <c r="E6" s="44"/>
+    </row>
+    <row r="7" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B7" s="49">
         <v>39</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="45" t="s">
+      <c r="D7" s="49" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="8" spans="2:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="46"/>
+      <c r="E7" s="44"/>
+    </row>
+    <row r="8" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="50"/>
       <c r="C8" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="D8" s="46"/>
-    </row>
-    <row r="9" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B9" s="43">
+      <c r="D8" s="50"/>
+      <c r="E8" s="44"/>
+    </row>
+    <row r="9" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B9" s="47">
         <v>40</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="D9" s="43" t="s">
+      <c r="D9" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="E9" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="47"/>
+      <c r="E9" s="44" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="51"/>
       <c r="C10" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="D10" s="47"/>
-    </row>
-    <row r="11" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B11" s="45">
+      <c r="D10" s="51"/>
+      <c r="E10" s="44"/>
+    </row>
+    <row r="11" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B11" s="49">
         <v>41</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="D11" s="45" t="s">
+      <c r="D11" s="49" t="s">
         <v>80</v>
       </c>
-      <c r="E11" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="46"/>
+      <c r="E11" s="44" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="50"/>
       <c r="C12" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="D12" s="46"/>
-    </row>
-    <row r="13" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B13" s="43">
+      <c r="D12" s="50"/>
+      <c r="E12" s="44"/>
+    </row>
+    <row r="13" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B13" s="47">
         <v>42</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="D13" s="43" t="s">
+      <c r="D13" s="47" t="s">
         <v>83</v>
       </c>
-      <c r="E13" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="47"/>
+      <c r="E13" s="44" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="51"/>
       <c r="C14" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="D14" s="47"/>
-    </row>
-    <row r="15" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="16" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B16" s="58">
+      <c r="D14" s="51"/>
+      <c r="E14" s="44"/>
+    </row>
+    <row r="15" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B15" s="62">
         <v>43</v>
       </c>
-      <c r="C16" s="31" t="s">
+      <c r="C15" s="31" t="s">
         <v>84</v>
       </c>
-      <c r="D16" s="58" t="s">
+      <c r="D15" s="62" t="s">
         <v>86</v>
       </c>
-      <c r="E16" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="53"/>
-      <c r="C17" s="32" t="s">
+      <c r="E15" s="44" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="57"/>
+      <c r="C16" s="32" t="s">
         <v>85</v>
       </c>
-      <c r="D17" s="53"/>
-    </row>
-    <row r="18" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B18" s="54">
+      <c r="D16" s="57"/>
+      <c r="E16" s="44"/>
+    </row>
+    <row r="17" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B17" s="58">
         <v>44</v>
       </c>
-      <c r="C18" s="33" t="s">
+      <c r="C17" s="33" t="s">
         <v>87</v>
       </c>
-      <c r="D18" s="59">
+      <c r="D17" s="63">
         <v>987654321</v>
       </c>
-    </row>
-    <row r="19" spans="2:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="55"/>
-      <c r="C19" s="34" t="s">
+      <c r="E17" s="44"/>
+    </row>
+    <row r="18" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="59"/>
+      <c r="C18" s="34" t="s">
         <v>88</v>
       </c>
-      <c r="D19" s="60"/>
-    </row>
-    <row r="20" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B20" s="52">
+      <c r="D18" s="64"/>
+      <c r="E18" s="44"/>
+    </row>
+    <row r="19" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B19" s="56">
         <v>45</v>
       </c>
-      <c r="C20" s="35" t="s">
+      <c r="C19" s="35" t="s">
         <v>89</v>
       </c>
-      <c r="D20" s="52">
+      <c r="D19" s="56">
         <v>1433</v>
       </c>
-    </row>
-    <row r="21" spans="2:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="53"/>
-      <c r="C21" s="32" t="s">
+      <c r="E19" s="44"/>
+    </row>
+    <row r="20" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="57"/>
+      <c r="C20" s="32" t="s">
         <v>90</v>
       </c>
-      <c r="D21" s="53"/>
-    </row>
-    <row r="22" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B22" s="54">
+      <c r="D20" s="57"/>
+      <c r="E20" s="44"/>
+    </row>
+    <row r="21" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B21" s="58">
         <v>46</v>
       </c>
-      <c r="C22" s="33" t="s">
+      <c r="C21" s="33" t="s">
         <v>91</v>
       </c>
-      <c r="D22" s="56">
+      <c r="D21" s="60">
         <v>43925</v>
       </c>
-    </row>
-    <row r="23" spans="2:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="55"/>
-      <c r="C23" s="34" t="s">
+      <c r="E21" s="69" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="59"/>
+      <c r="C22" s="34" t="s">
         <v>92</v>
       </c>
-      <c r="D23" s="57"/>
-    </row>
-    <row r="24" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B24" s="52">
+      <c r="D22" s="61"/>
+      <c r="E22" s="44"/>
+    </row>
+    <row r="23" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B23" s="56">
         <v>47</v>
       </c>
-      <c r="C24" s="35" t="s">
+      <c r="C23" s="35" t="s">
         <v>93</v>
       </c>
-      <c r="D24" s="52" t="s">
+      <c r="D23" s="56" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="25" spans="2:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B25" s="53"/>
-      <c r="C25" s="32" t="s">
+      <c r="E23" s="69" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="57"/>
+      <c r="C24" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="D25" s="53"/>
-    </row>
-    <row r="26" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B26" s="54">
+      <c r="D24" s="57"/>
+      <c r="E24" s="44"/>
+    </row>
+    <row r="25" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B25" s="58">
         <v>48</v>
       </c>
-      <c r="C26" s="33" t="s">
+      <c r="C25" s="33" t="s">
         <v>94</v>
       </c>
-      <c r="D26" s="56">
+      <c r="D25" s="60">
         <v>43834</v>
       </c>
-    </row>
-    <row r="27" spans="2:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="55"/>
-      <c r="C27" s="34" t="s">
+      <c r="E25" s="69" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="59"/>
+      <c r="C26" s="34" t="s">
         <v>95</v>
       </c>
-      <c r="D27" s="57"/>
-    </row>
-    <row r="28" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B28" s="52">
+      <c r="D26" s="61"/>
+      <c r="E26" s="44"/>
+    </row>
+    <row r="27" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B27" s="56">
         <v>49</v>
       </c>
-      <c r="C28" s="35" t="s">
+      <c r="C27" s="35" t="s">
         <v>96</v>
       </c>
-      <c r="D28" s="52">
+      <c r="D27" s="56">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="2:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B29" s="53"/>
-      <c r="C29" s="32" t="s">
+      <c r="E27" s="69" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="57"/>
+      <c r="C28" s="32" t="s">
         <v>96</v>
       </c>
-      <c r="D29" s="53"/>
-    </row>
-    <row r="30" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B30" s="54">
+      <c r="D28" s="57"/>
+      <c r="E28" s="44"/>
+    </row>
+    <row r="29" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B29" s="58">
         <v>50</v>
       </c>
-      <c r="C30" s="33" t="s">
+      <c r="C29" s="33" t="s">
         <v>97</v>
       </c>
-      <c r="D30" s="54">
+      <c r="D29" s="58">
         <v>5</v>
       </c>
-    </row>
-    <row r="31" spans="2:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B31" s="55"/>
-      <c r="C31" s="34" t="s">
+      <c r="E29" s="44"/>
+    </row>
+    <row r="30" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="59"/>
+      <c r="C30" s="34" t="s">
         <v>98</v>
       </c>
-      <c r="D31" s="55"/>
-    </row>
-    <row r="32" spans="2:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="52">
+      <c r="D30" s="59"/>
+      <c r="E30" s="44"/>
+    </row>
+    <row r="31" spans="2:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="56">
         <v>51</v>
       </c>
-      <c r="C32" s="35" t="s">
+      <c r="C31" s="35" t="s">
         <v>99</v>
       </c>
-      <c r="D32" s="35" t="s">
+      <c r="D31" s="35" t="s">
         <v>101</v>
       </c>
-      <c r="E32" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="33" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B33" s="53"/>
-      <c r="C33" s="32" t="s">
+      <c r="E31" s="44" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="57"/>
+      <c r="C32" s="32" t="s">
         <v>100</v>
       </c>
-      <c r="D33" s="36" t="s">
+      <c r="D32" s="36" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="34" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B34" s="54">
+      <c r="E32" s="44"/>
+    </row>
+    <row r="33" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B33" s="58">
         <v>52</v>
       </c>
-      <c r="C34" s="33" t="s">
+      <c r="C33" s="33" t="s">
         <v>103</v>
       </c>
-      <c r="D34" s="54" t="s">
+      <c r="D33" s="58" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="35" spans="2:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B35" s="55"/>
-      <c r="C35" s="34" t="s">
+      <c r="E33" s="44"/>
+    </row>
+    <row r="34" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="59"/>
+      <c r="C34" s="34" t="s">
         <v>104</v>
       </c>
-      <c r="D35" s="55"/>
-    </row>
-    <row r="36" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B36" s="52">
+      <c r="D34" s="59"/>
+      <c r="E34" s="44"/>
+    </row>
+    <row r="35" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B35" s="56">
         <v>53</v>
       </c>
-      <c r="C36" s="35" t="s">
+      <c r="C35" s="35" t="s">
         <v>106</v>
       </c>
-      <c r="D36" s="52" t="s">
+      <c r="D35" s="56" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="37" spans="2:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B37" s="53"/>
-      <c r="C37" s="32" t="s">
+      <c r="E35" s="44"/>
+    </row>
+    <row r="36" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="57"/>
+      <c r="C36" s="32" t="s">
         <v>107</v>
       </c>
-      <c r="D37" s="53"/>
-    </row>
-    <row r="38" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B38" s="54">
+      <c r="D36" s="57"/>
+      <c r="E36" s="44"/>
+    </row>
+    <row r="37" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B37" s="58">
         <v>54</v>
       </c>
-      <c r="C38" s="33" t="s">
+      <c r="C37" s="33" t="s">
         <v>109</v>
       </c>
-      <c r="D38" s="54" t="s">
+      <c r="D37" s="58" t="s">
         <v>111</v>
       </c>
-      <c r="E38" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="39" spans="2:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B39" s="55"/>
-      <c r="C39" s="34" t="s">
+      <c r="E37" s="44" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="59"/>
+      <c r="C38" s="34" t="s">
         <v>110</v>
       </c>
-      <c r="D39" s="55"/>
-    </row>
-    <row r="40" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B40" s="36">
+      <c r="D38" s="59"/>
+      <c r="E38" s="44"/>
+    </row>
+    <row r="39" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="36">
         <v>55</v>
       </c>
-      <c r="C40" s="37" t="s">
+      <c r="C39" s="37" t="s">
         <v>112</v>
       </c>
-      <c r="D40" s="36" t="s">
+      <c r="D39" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="E40" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="41" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B41" s="38">
+      <c r="E39" s="41" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="38">
         <v>56</v>
       </c>
-      <c r="C41" s="38" t="s">
+      <c r="C40" s="38" t="s">
         <v>113</v>
       </c>
-      <c r="D41" s="38" t="s">
+      <c r="D40" s="38" t="s">
         <v>114</v>
       </c>
-      <c r="E41" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="42" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B42" s="36">
+      <c r="E40" s="41" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="36">
         <v>57</v>
       </c>
-      <c r="C42" s="36" t="s">
+      <c r="C41" s="36" t="s">
         <v>115</v>
       </c>
-      <c r="D42" s="36" t="s">
+      <c r="D41" s="36" t="s">
         <v>116</v>
       </c>
-      <c r="E42" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="43" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="61">
+      <c r="E41" s="41" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="65">
         <v>58</v>
       </c>
-      <c r="C43" s="39" t="s">
+      <c r="C42" s="39" t="s">
         <v>117</v>
       </c>
-      <c r="D43" s="61" t="s">
+      <c r="D42" s="65" t="s">
         <v>36</v>
       </c>
-      <c r="E43" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="44" spans="2:5" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B44" s="55"/>
-      <c r="C44" s="34" t="s">
+      <c r="E42" s="44" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B43" s="59"/>
+      <c r="C43" s="34" t="s">
         <v>118</v>
       </c>
-      <c r="D44" s="55"/>
-    </row>
-    <row r="45" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B45" s="52">
+      <c r="D43" s="59"/>
+      <c r="E43" s="44"/>
+    </row>
+    <row r="44" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B44" s="56">
         <v>59</v>
       </c>
-      <c r="C45" s="35" t="s">
+      <c r="C44" s="35" t="s">
         <v>119</v>
       </c>
-      <c r="D45" s="52" t="s">
+      <c r="D44" s="56" t="s">
         <v>36</v>
       </c>
-      <c r="E45" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="46" spans="2:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B46" s="53"/>
-      <c r="C46" s="32" t="s">
+      <c r="E44" s="44" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B45" s="57"/>
+      <c r="C45" s="32" t="s">
         <v>120</v>
       </c>
-      <c r="D46" s="53"/>
-    </row>
-    <row r="47" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B47" s="38">
+      <c r="D45" s="57"/>
+      <c r="E45" s="44"/>
+    </row>
+    <row r="46" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B46" s="38">
         <v>60</v>
       </c>
-      <c r="C47" s="38" t="s">
+      <c r="C46" s="38" t="s">
         <v>121</v>
       </c>
-      <c r="D47" s="38" t="s">
+      <c r="D46" s="38" t="s">
         <v>122</v>
       </c>
-      <c r="E47" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="48" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B48" s="36">
+      <c r="E46" s="41" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B47" s="36">
         <v>61</v>
       </c>
-      <c r="C48" s="36" t="s">
+      <c r="C47" s="36" t="s">
         <v>123</v>
       </c>
-      <c r="D48" s="36" t="s">
+      <c r="D47" s="36" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="49" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B49" s="38">
+    <row r="48" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B48" s="38">
         <v>62</v>
       </c>
-      <c r="C49" s="38" t="s">
+      <c r="C48" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="D49" s="38" t="s">
+      <c r="D48" s="38" t="s">
         <v>125</v>
       </c>
-      <c r="E49" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="50" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B50" s="52">
+      <c r="E48" s="41" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="49" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B49" s="56">
         <v>63</v>
       </c>
-      <c r="C50" s="35" t="s">
+      <c r="C49" s="35" t="s">
         <v>126</v>
       </c>
-      <c r="D50" s="52" t="s">
+      <c r="D49" s="56" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="51" spans="2:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B51" s="53"/>
-      <c r="C51" s="32" t="s">
+      <c r="E49" s="44"/>
+    </row>
+    <row r="50" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B50" s="57"/>
+      <c r="C50" s="32" t="s">
         <v>127</v>
       </c>
-      <c r="D51" s="53"/>
-    </row>
-    <row r="52" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B52" s="54">
+      <c r="D50" s="57"/>
+      <c r="E50" s="44"/>
+    </row>
+    <row r="51" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B51" s="58">
         <v>64</v>
       </c>
-      <c r="C52" s="33" t="s">
+      <c r="C51" s="33" t="s">
         <v>129</v>
       </c>
-      <c r="D52" s="54" t="s">
+      <c r="D51" s="58" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="53" spans="2:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B53" s="55"/>
-      <c r="C53" s="34" t="s">
+      <c r="E51" s="44"/>
+    </row>
+    <row r="52" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B52" s="59"/>
+      <c r="C52" s="34" t="s">
         <v>130</v>
       </c>
-      <c r="D53" s="55"/>
-    </row>
-    <row r="54" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B54" s="52">
+      <c r="D52" s="59"/>
+      <c r="E52" s="44"/>
+    </row>
+    <row r="53" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B53" s="56">
         <v>65</v>
       </c>
-      <c r="C54" s="35" t="s">
+      <c r="C53" s="35" t="s">
         <v>132</v>
       </c>
-      <c r="D54" s="52" t="s">
+      <c r="D53" s="56" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="55" spans="2:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B55" s="53"/>
-      <c r="C55" s="32" t="s">
+      <c r="E53" s="44"/>
+    </row>
+    <row r="54" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B54" s="57"/>
+      <c r="C54" s="32" t="s">
         <v>133</v>
       </c>
-      <c r="D55" s="53"/>
-    </row>
-    <row r="56" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B56" s="38">
+      <c r="D54" s="57"/>
+      <c r="E54" s="44"/>
+    </row>
+    <row r="55" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B55" s="38">
         <v>66</v>
       </c>
-      <c r="C56" s="38" t="s">
+      <c r="C55" s="38" t="s">
         <v>135</v>
       </c>
-      <c r="D56" s="38" t="s">
+      <c r="D55" s="38" t="s">
         <v>136</v>
       </c>
-      <c r="E56" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="57" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B57" s="36">
+      <c r="E55" s="41" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="56" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B56" s="36">
         <v>67</v>
       </c>
-      <c r="C57" s="36" t="s">
+      <c r="C56" s="36" t="s">
         <v>137</v>
       </c>
-      <c r="D57" s="36" t="s">
+      <c r="D56" s="36" t="s">
         <v>138</v>
       </c>
-      <c r="E57" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="58" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B58" s="38">
+      <c r="E56" s="41" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="57" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B57" s="38">
         <v>68</v>
       </c>
-      <c r="C58" s="38" t="s">
+      <c r="C57" s="38" t="s">
         <v>139</v>
       </c>
-      <c r="D58" s="38" t="s">
+      <c r="D57" s="38" t="s">
         <v>140</v>
       </c>
-      <c r="E58" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="59" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B59" s="36">
+      <c r="E57" s="41" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="58" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B58" s="36">
         <v>69</v>
       </c>
-      <c r="C59" s="36" t="s">
+      <c r="C58" s="36" t="s">
         <v>141</v>
       </c>
-      <c r="D59" s="36" t="s">
+      <c r="D58" s="36" t="s">
         <v>142</v>
       </c>
-      <c r="E59" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="60" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B60" s="38">
+      <c r="E58" s="41" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="59" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B59" s="38">
         <v>70</v>
       </c>
-      <c r="C60" s="38" t="s">
+      <c r="C59" s="38" t="s">
         <v>143</v>
       </c>
-      <c r="D60" s="38" t="s">
+      <c r="D59" s="38" t="s">
         <v>144</v>
       </c>
-      <c r="E60" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="61" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B61" s="36">
+      <c r="E59" s="41" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="60" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B60" s="36">
         <v>71</v>
       </c>
-      <c r="C61" s="36" t="s">
+      <c r="C60" s="36" t="s">
         <v>145</v>
       </c>
-      <c r="D61" s="36" t="s">
+      <c r="D60" s="36" t="s">
         <v>144</v>
       </c>
-      <c r="E61" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="62" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B62" s="38">
+      <c r="E60" s="41" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="61" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B61" s="38">
         <v>72</v>
       </c>
-      <c r="C62" s="38" t="s">
+      <c r="C61" s="38" t="s">
         <v>146</v>
       </c>
-      <c r="D62" s="38" t="s">
+      <c r="D61" s="38" t="s">
         <v>144</v>
       </c>
-      <c r="E62" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="63" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B63" s="36">
+      <c r="E61" s="41" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="62" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B62" s="36">
         <v>73</v>
       </c>
-      <c r="C63" s="36" t="s">
+      <c r="C62" s="36" t="s">
         <v>147</v>
       </c>
-      <c r="D63" s="36" t="s">
+      <c r="D62" s="36" t="s">
         <v>144</v>
       </c>
-      <c r="E63" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="64" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B64" s="38">
+      <c r="E62" s="41" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="63" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B63" s="38">
         <v>74</v>
       </c>
-      <c r="C64" s="38" t="s">
+      <c r="C63" s="38" t="s">
         <v>148</v>
       </c>
-      <c r="D64" s="38" t="s">
+      <c r="D63" s="38" t="s">
         <v>144</v>
       </c>
-      <c r="E64" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="65" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B65" s="26">
+      <c r="E63" s="41" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="64" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B64" s="26">
         <v>75</v>
       </c>
-      <c r="C65" s="26" t="s">
+      <c r="C64" s="26" t="s">
         <v>149</v>
       </c>
-      <c r="D65" s="26" t="s">
+      <c r="D64" s="26" t="s">
         <v>144</v>
       </c>
-      <c r="E65" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="66" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B66" s="4">
+      <c r="E64" s="41" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="65" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B65" s="4">
         <v>76</v>
       </c>
-      <c r="C66" s="4" t="s">
+      <c r="C65" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="D66" s="4" t="s">
+      <c r="D65" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="E66" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="67" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E65" s="41" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="66" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B66" s="2">
+        <v>77</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="E66" s="41" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="67" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B67" s="2">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="E67" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="68" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B68" s="2">
-        <v>78</v>
-      </c>
-      <c r="C68" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="D68" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="E68" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="69" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B69" s="4">
+      <c r="E67" s="41" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="68" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B68" s="4">
         <v>79</v>
       </c>
-      <c r="C69" s="4" t="s">
+      <c r="C68" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="D69" s="4" t="s">
+      <c r="D68" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="E69" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="70" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B70" s="2">
+      <c r="E68" s="41" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="69" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B69" s="2">
         <v>80</v>
       </c>
-      <c r="C70" s="2" t="s">
+      <c r="C69" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="D70" s="2" t="s">
+      <c r="D69" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="E70" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="71" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B71" s="4">
+      <c r="E69" s="41" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="70" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B70" s="4">
         <v>81</v>
       </c>
-      <c r="C71" s="4" t="s">
+      <c r="C70" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="D71" s="4" t="s">
+      <c r="D70" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="E71" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="72" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B72" s="2">
+      <c r="E70" s="41" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="71" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B71" s="2">
         <v>82</v>
       </c>
-      <c r="C72" s="2" t="s">
+      <c r="C71" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="D72" s="2">
+      <c r="D71" s="2">
         <v>110</v>
       </c>
-      <c r="E72" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="73" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B73" s="4">
+      <c r="E71" s="41" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="72" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B72" s="4">
         <v>83</v>
       </c>
-      <c r="C73" s="4" t="s">
+      <c r="C72" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="D73" s="4" t="s">
+      <c r="D72" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="E73" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="74" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B74" s="2">
+      <c r="E72" s="41" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="73" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B73" s="2">
         <v>84</v>
       </c>
-      <c r="C74" s="2" t="s">
+      <c r="C73" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="D74" s="2" t="s">
+      <c r="D73" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="E74" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="75" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B75" s="4">
+      <c r="E73" s="41" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="74" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B74" s="4">
         <v>85</v>
       </c>
-      <c r="C75" s="4" t="s">
+      <c r="C74" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="D75" s="4" t="s">
+      <c r="D74" s="4" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="76" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B76" s="2">
+    <row r="75" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B75" s="2">
         <v>86</v>
       </c>
-      <c r="C76" s="2" t="s">
+      <c r="C75" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="D76" s="2" t="s">
+      <c r="D75" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="E76" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="77" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B77" s="4">
+      <c r="E75" s="41" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="76" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B76" s="4">
         <v>87</v>
       </c>
-      <c r="C77" s="4" t="s">
+      <c r="C76" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="D77" s="4" t="s">
+      <c r="D76" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="E77" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="78" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B78" s="2">
+      <c r="E76" s="41" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="77" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B77" s="2">
         <v>88</v>
       </c>
-      <c r="C78" s="2" t="s">
+      <c r="C77" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="D78" s="2" t="s">
+      <c r="D77" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="E78" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="79" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B79" s="4">
+      <c r="E77" s="41" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="78" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B78" s="4">
         <v>89</v>
       </c>
-      <c r="C79" s="4" t="s">
+      <c r="C78" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="D79" s="30">
+      <c r="D78" s="30">
         <v>44088</v>
       </c>
-      <c r="E79" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="80" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B80" s="2">
+      <c r="E78" s="41" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="79" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B79" s="2">
         <v>90</v>
       </c>
-      <c r="C80" s="2" t="s">
+      <c r="C79" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="D80" s="3">
+      <c r="D79" s="3">
         <v>43178</v>
       </c>
     </row>
-    <row r="81" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B81" s="4">
+    <row r="80" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B80" s="4">
         <v>91</v>
       </c>
-      <c r="C81" s="4" t="s">
+      <c r="C80" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="D81" s="4" t="s">
+      <c r="D80" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="E81" t="s">
-        <v>270</v>
+      <c r="E80" s="41" t="s">
+        <v>268</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="45">
-    <mergeCell ref="B52:B53"/>
-    <mergeCell ref="D52:D53"/>
-    <mergeCell ref="B54:B55"/>
-    <mergeCell ref="D54:D55"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="D45:D46"/>
-    <mergeCell ref="B50:B51"/>
-    <mergeCell ref="D50:D51"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="D43:D44"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="D18:D19"/>
+  <mergeCells count="68">
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="D51:D52"/>
+    <mergeCell ref="B53:B54"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="D49:D50"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E33:E34"/>
+    <mergeCell ref="E35:E36"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="D11:D12"/>
     <mergeCell ref="B13:B14"/>
     <mergeCell ref="D13:D14"/>
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="D7:D8"/>
     <mergeCell ref="B9:B10"/>
     <mergeCell ref="D9:D10"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="E49:E50"/>
+    <mergeCell ref="E51:E52"/>
+    <mergeCell ref="E53:E54"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="E44:E45"/>
+    <mergeCell ref="E42:E43"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="E21:E22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F20"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView topLeftCell="B2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="7.88671875" customWidth="1"/>
-    <col min="3" max="3" width="56.88671875" customWidth="1"/>
+    <col min="2" max="2" width="7.85546875" customWidth="1"/>
+    <col min="3" max="3" width="56.85546875" customWidth="1"/>
     <col min="4" max="4" width="100" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="41"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E1" t="s">
-        <v>262</v>
+    <row r="1" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E1" s="41" t="s">
+        <v>260</v>
       </c>
       <c r="F1" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="2" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B2" s="48">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="2" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B2" s="52">
         <v>92</v>
       </c>
       <c r="C2" s="16" t="s">
         <v>178</v>
       </c>
-      <c r="D2" s="48" t="s">
+      <c r="D2" s="52" t="s">
         <v>36</v>
       </c>
-      <c r="E2" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="3" spans="2:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="46"/>
+      <c r="E2" s="44" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="50"/>
       <c r="C3" s="7" t="s">
         <v>179</v>
       </c>
-      <c r="D3" s="46"/>
-    </row>
-    <row r="4" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B4" s="43">
+      <c r="D3" s="50"/>
+      <c r="E3" s="44"/>
+    </row>
+    <row r="4" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B4" s="47">
         <v>93</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="43" t="s">
+      <c r="D4" s="47" t="s">
         <v>71</v>
       </c>
-      <c r="E4" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="47"/>
+      <c r="E4" s="44" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="51"/>
       <c r="C5" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="D5" s="47"/>
-    </row>
-    <row r="6" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B6" s="45">
+      <c r="D5" s="51"/>
+      <c r="E5" s="44"/>
+    </row>
+    <row r="6" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B6" s="49">
         <v>94</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="45" t="s">
+      <c r="D6" s="49" t="s">
         <v>182</v>
       </c>
-      <c r="E6" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="46"/>
+      <c r="E6" s="44" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="50"/>
       <c r="C7" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="D7" s="46"/>
-    </row>
-    <row r="8" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D7" s="50"/>
+      <c r="E7" s="44"/>
+    </row>
+    <row r="8" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="4">
         <v>95</v>
       </c>
@@ -3579,11 +3775,11 @@
       <c r="D8" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="E8" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E8" s="41" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="2">
         <v>96</v>
       </c>
@@ -3593,11 +3789,11 @@
       <c r="D9" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="E9" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E9" s="41" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="4">
         <v>97</v>
       </c>
@@ -3607,11 +3803,11 @@
       <c r="D10" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="E10" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E10" s="41" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="2">
         <v>98</v>
       </c>
@@ -3622,49 +3818,53 @@
         <v>189</v>
       </c>
     </row>
-    <row r="12" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B12" s="62">
+    <row r="12" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B12" s="66">
         <v>99</v>
       </c>
-      <c r="C12" s="62" t="s">
+      <c r="C12" s="66" t="s">
         <v>190</v>
       </c>
       <c r="D12" s="29" t="s">
         <v>191</v>
       </c>
-      <c r="E12" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B13" s="44"/>
-      <c r="C13" s="44"/>
+      <c r="E12" s="44" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B13" s="48"/>
+      <c r="C13" s="48"/>
       <c r="D13" s="8" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="14" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B14" s="44"/>
-      <c r="C14" s="44"/>
+      <c r="E13" s="44"/>
+    </row>
+    <row r="14" spans="2:6" ht="33" x14ac:dyDescent="0.25">
+      <c r="B14" s="48"/>
+      <c r="C14" s="48"/>
       <c r="D14" s="8" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="15" spans="2:6" ht="50.4" x14ac:dyDescent="0.3">
-      <c r="B15" s="44"/>
-      <c r="C15" s="44"/>
+      <c r="E14" s="44"/>
+    </row>
+    <row r="15" spans="2:6" ht="49.5" x14ac:dyDescent="0.25">
+      <c r="B15" s="48"/>
+      <c r="C15" s="48"/>
       <c r="D15" s="8" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="16" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="47"/>
-      <c r="C16" s="47"/>
+      <c r="E15" s="44"/>
+    </row>
+    <row r="16" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="51"/>
+      <c r="C16" s="51"/>
       <c r="D16" s="4" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="17" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E16" s="44"/>
+    </row>
+    <row r="17" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="2">
         <v>100</v>
       </c>
@@ -3674,40 +3874,42 @@
       <c r="D17" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="E17" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B18" s="43">
+      <c r="E17" s="41" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B18" s="47">
         <v>101</v>
       </c>
-      <c r="C18" s="43" t="s">
+      <c r="C18" s="47" t="s">
         <v>198</v>
       </c>
       <c r="D18" s="8" t="s">
         <v>199</v>
       </c>
-      <c r="E18" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B19" s="44"/>
-      <c r="C19" s="44"/>
+      <c r="E18" s="44" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B19" s="48"/>
+      <c r="C19" s="48"/>
       <c r="D19" s="8" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="20" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="47"/>
-      <c r="C20" s="47"/>
+      <c r="E19" s="44"/>
+    </row>
+    <row r="20" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="51"/>
+      <c r="C20" s="51"/>
       <c r="D20" s="4" t="s">
         <v>201</v>
       </c>
+      <c r="E20" s="44"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="15">
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="B4:B5"/>
@@ -3718,98 +3920,107 @@
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="B12:B16"/>
     <mergeCell ref="C12:C16"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="E12:E16"/>
+    <mergeCell ref="E18:E20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F31"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="4.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="59" customWidth="1"/>
-    <col min="4" max="4" width="52.6640625" customWidth="1"/>
+    <col min="4" max="4" width="52.7109375" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="41"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E1" t="s">
+    <row r="1" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E1" s="41" t="s">
         <v>48</v>
       </c>
       <c r="F1" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="2" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B2" s="48">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="2" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B2" s="52">
         <v>102</v>
       </c>
       <c r="C2" s="16" t="s">
         <v>178</v>
       </c>
-      <c r="D2" s="48" t="s">
+      <c r="D2" s="52" t="s">
         <v>36</v>
       </c>
-      <c r="E2" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="3" spans="2:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="46"/>
+      <c r="E2" s="44" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="50"/>
       <c r="C3" s="7" t="s">
         <v>179</v>
       </c>
-      <c r="D3" s="46"/>
-    </row>
-    <row r="4" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B4" s="43">
+      <c r="D3" s="50"/>
+      <c r="E3" s="44"/>
+    </row>
+    <row r="4" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B4" s="47">
         <v>103</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>202</v>
       </c>
-      <c r="D4" s="43" t="s">
+      <c r="D4" s="47" t="s">
         <v>71</v>
       </c>
-      <c r="E4" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="47"/>
+      <c r="E4" s="44" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="51"/>
       <c r="C5" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="D5" s="47"/>
-    </row>
-    <row r="6" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B6" s="45">
+      <c r="D5" s="51"/>
+      <c r="E5" s="44"/>
+    </row>
+    <row r="6" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B6" s="49">
         <v>104</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="45" t="s">
+      <c r="D6" s="49" t="s">
         <v>182</v>
       </c>
-      <c r="E6" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="46"/>
+      <c r="E6" s="44" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="50"/>
       <c r="C7" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="D7" s="46"/>
-    </row>
-    <row r="8" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D7" s="50"/>
+      <c r="E7" s="44"/>
+    </row>
+    <row r="8" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="4">
         <v>105</v>
       </c>
@@ -3820,7 +4031,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="9" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="2">
         <v>106</v>
       </c>
@@ -3830,11 +4041,11 @@
       <c r="D9" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="E9" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E9" s="41" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="4">
         <v>107</v>
       </c>
@@ -3844,11 +4055,11 @@
       <c r="D10" s="4" t="s">
         <v>208</v>
       </c>
-      <c r="E10" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E10" s="41" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="2">
         <v>108</v>
       </c>
@@ -3859,7 +4070,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="12" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="4">
         <v>109</v>
       </c>
@@ -3870,7 +4081,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="13" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="2">
         <v>110</v>
       </c>
@@ -3881,7 +4092,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="14" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="4">
         <v>111</v>
       </c>
@@ -3892,7 +4103,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="26">
         <v>112</v>
       </c>
@@ -3902,11 +4113,11 @@
       <c r="D15" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="E15" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E15" s="41" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="4">
         <v>113</v>
       </c>
@@ -3916,11 +4127,11 @@
       <c r="D16" s="4" t="s">
         <v>216</v>
       </c>
-      <c r="E16" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" ht="34.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E16" s="41" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="2">
         <v>114</v>
       </c>
@@ -3931,7 +4142,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="18" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="4">
         <v>115</v>
       </c>
@@ -3941,11 +4152,11 @@
       <c r="D18" s="4" t="s">
         <v>220</v>
       </c>
-      <c r="E18" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E18" s="41" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="2">
         <v>116</v>
       </c>
@@ -3956,25 +4167,25 @@
         <v>222</v>
       </c>
     </row>
-    <row r="20" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B20" s="43">
+    <row r="20" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B20" s="47">
         <v>117</v>
       </c>
       <c r="C20" s="8" t="s">
         <v>223</v>
       </c>
-      <c r="D20" s="43" t="s">
+      <c r="D20" s="47" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="21" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="47"/>
+    <row r="21" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="51"/>
       <c r="C21" s="4" t="s">
         <v>224</v>
       </c>
-      <c r="D21" s="47"/>
-    </row>
-    <row r="22" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D21" s="51"/>
+    </row>
+    <row r="22" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="2">
         <v>118</v>
       </c>
@@ -3985,7 +4196,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="23" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="4">
         <v>119</v>
       </c>
@@ -3995,11 +4206,11 @@
       <c r="D23" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="E23" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E23" s="41" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="2">
         <v>120</v>
       </c>
@@ -4009,11 +4220,11 @@
       <c r="D24" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="E24" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5" ht="34.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E24" s="41" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="4">
         <v>121</v>
       </c>
@@ -4023,11 +4234,11 @@
       <c r="D25" s="4" t="s">
         <v>232</v>
       </c>
-      <c r="E25" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="26" spans="2:5" ht="34.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E25" s="41" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="2">
         <v>122</v>
       </c>
@@ -4037,11 +4248,11 @@
       <c r="D26" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="E26" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="27" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E26" s="41" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="4">
         <v>123</v>
       </c>
@@ -4051,11 +4262,11 @@
       <c r="D27" s="4" t="s">
         <v>236</v>
       </c>
-      <c r="E27" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="28" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E27" s="41" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="2">
         <v>124</v>
       </c>
@@ -4065,11 +4276,11 @@
       <c r="D28" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="E28" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="29" spans="2:5" ht="34.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E28" s="41" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B29" s="4">
         <v>125</v>
       </c>
@@ -4079,219 +4290,220 @@
       <c r="D29" s="4" t="s">
         <v>240</v>
       </c>
-      <c r="E29" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="30" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B30" s="45">
+      <c r="E29" s="41" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B30" s="49">
         <v>126</v>
       </c>
       <c r="C30" s="6" t="s">
+        <v>269</v>
+      </c>
+      <c r="D30" s="49" t="s">
         <v>241</v>
       </c>
-      <c r="D30" s="45" t="s">
-        <v>243</v>
-      </c>
-      <c r="E30" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="31" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B31" s="46"/>
-      <c r="C31" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="D31" s="46"/>
+      <c r="E30" s="41" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="50"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="50"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="D4:D5"/>
+  <mergeCells count="13">
     <mergeCell ref="B30:B31"/>
     <mergeCell ref="D30:D31"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="B20:B21"/>
     <mergeCell ref="D20:D21"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="D4:D5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F12"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="42.44140625" customWidth="1"/>
-    <col min="4" max="4" width="74.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.42578125" customWidth="1"/>
+    <col min="4" max="4" width="74.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="F1" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="2" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="2" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="26">
         <v>127</v>
       </c>
       <c r="C2" s="26" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D2" s="26" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="3" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="4">
         <v>128</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E3" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="26">
         <v>129</v>
       </c>
       <c r="C4" s="26" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D4" s="26" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E4" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="4">
         <v>130</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E5" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="2">
         <v>131</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D6" s="3">
         <v>44088</v>
       </c>
       <c r="E6" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" ht="34.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="4">
         <v>132</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E7" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" ht="34.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="2">
         <v>133</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E8" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" ht="34.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="4">
         <v>134</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E9" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" ht="51" thickBot="1" x14ac:dyDescent="0.35">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" ht="50.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="2">
         <v>135</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="E10" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" ht="34.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="4">
         <v>136</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="E11" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" ht="34.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="2">
         <v>137</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="E12" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
IIsConfiguration and other new Scripts
</commit_message>
<xml_diff>
--- a/Checklist.xlsx
+++ b/Checklist.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MO\Powershell\Project\AziraPowershellscript2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Prashant\AziraPowershellscript\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E82581F-AED1-4F55-B769-BEFDD23316C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="2"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Application" sheetId="1" r:id="rId1"/>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="272">
   <si>
     <t xml:space="preserve"> Last Updated</t>
   </si>
@@ -1012,12 +1013,6 @@
     <t>Remarks</t>
   </si>
   <si>
-    <t>Partial Done</t>
-  </si>
-  <si>
-    <t>Got the commands but haven't comitted the script</t>
-  </si>
-  <si>
     <t>Partially 
 Done</t>
   </si>
@@ -1025,7 +1020,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1319,7 +1314,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1446,81 +1441,90 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="4" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="4" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="4" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="4" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1560,7 +1564,7 @@
         <xdr:cNvPr id="14" name="Picture 92361">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000E000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1621,7 +1625,7 @@
         <xdr:cNvPr id="15" name="Picture 92362">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000F000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1929,24 +1933,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:F41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C28" sqref="C28"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="3.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="51" customWidth="1"/>
-    <col min="4" max="4" width="74.42578125" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="41"/>
-    <col min="6" max="6" width="11.42578125" customWidth="1"/>
+    <col min="4" max="4" width="74.44140625" customWidth="1"/>
+    <col min="5" max="5" width="9.109375" style="41"/>
+    <col min="6" max="6" width="11.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1" s="40" t="s">
         <v>266</v>
       </c>
@@ -1963,14 +1967,14 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="45" t="s">
+    <row r="2" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-    </row>
-    <row r="3" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+    </row>
+    <row r="3" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="13">
         <v>1</v>
       </c>
@@ -1980,8 +1984,11 @@
       <c r="D3" s="15">
         <v>44102</v>
       </c>
-    </row>
-    <row r="4" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E3" s="41" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="11">
         <v>2</v>
       </c>
@@ -1991,165 +1998,170 @@
       <c r="D4" s="25" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="54" t="s">
+      <c r="E4" s="41" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="55"/>
-      <c r="D5" s="55"/>
-    </row>
-    <row r="6" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="C5" s="56"/>
+      <c r="D5" s="56"/>
+    </row>
+    <row r="6" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B6" s="14">
         <v>3</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="52" t="s">
+      <c r="D6" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="44" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E6" s="57" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="1"/>
       <c r="C7" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="50"/>
-      <c r="E7" s="44"/>
-    </row>
-    <row r="8" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="D7" s="49"/>
+      <c r="E7" s="57"/>
+    </row>
+    <row r="8" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B8" s="12">
         <v>4</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="47" t="s">
+      <c r="D8" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="44"/>
-    </row>
-    <row r="9" spans="2:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E8" s="57"/>
+    </row>
+    <row r="9" spans="2:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="1"/>
       <c r="C9" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="51"/>
-      <c r="E9" s="44"/>
-    </row>
-    <row r="10" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="D9" s="47"/>
+      <c r="E9" s="57"/>
+    </row>
+    <row r="10" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B10" s="14">
         <v>5</v>
       </c>
       <c r="C10" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="52" t="s">
+      <c r="D10" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="44" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E10" s="57" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" s="5"/>
       <c r="C11" s="17" t="s">
         <v>263</v>
       </c>
-      <c r="D11" s="53"/>
-      <c r="E11" s="44"/>
-    </row>
-    <row r="12" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="D11" s="54"/>
+      <c r="E11" s="57"/>
+    </row>
+    <row r="12" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B12" s="12">
         <v>6</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="47" t="s">
+      <c r="D12" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="44" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E12" s="57" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="5"/>
       <c r="C13" s="18" t="s">
         <v>263</v>
       </c>
-      <c r="D13" s="48"/>
-      <c r="E13" s="44"/>
-    </row>
-    <row r="14" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="D13" s="52"/>
+      <c r="E13" s="57"/>
+    </row>
+    <row r="14" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B14" s="12">
         <v>7</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="49" t="s">
+      <c r="D14" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="E14" s="44" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E14" s="57" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="1"/>
       <c r="C15" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="50"/>
-      <c r="E15" s="44"/>
-    </row>
-    <row r="16" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="D15" s="49"/>
+      <c r="E15" s="57"/>
+    </row>
+    <row r="16" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B16" s="12">
         <v>8</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="47" t="s">
+      <c r="D16" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="E16" s="44" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E16" s="57" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="1"/>
       <c r="C17" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="51"/>
-      <c r="E17" s="44"/>
-    </row>
-    <row r="18" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="D17" s="47"/>
+      <c r="E17" s="57"/>
+    </row>
+    <row r="18" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B18" s="12">
         <v>9</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D18" s="49">
+      <c r="D18" s="48">
         <v>4</v>
       </c>
-      <c r="E18" s="44"/>
-    </row>
-    <row r="19" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E18" s="57" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B19" s="1"/>
       <c r="C19" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D19" s="50"/>
-      <c r="E19" s="44"/>
-    </row>
-    <row r="20" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D19" s="49"/>
+      <c r="E19" s="57"/>
+    </row>
+    <row r="20" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B20" s="1">
         <v>10</v>
       </c>
@@ -2159,104 +2171,104 @@
       <c r="D20" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E20" s="44" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E20" s="57" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C21" s="20" t="s">
         <v>22</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E21" s="44"/>
-    </row>
-    <row r="22" spans="2:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E21" s="57"/>
+    </row>
+    <row r="22" spans="2:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="12">
         <v>11</v>
       </c>
       <c r="C22" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D22" s="47" t="s">
+      <c r="D22" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="E22" s="44" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="23" spans="2:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E22" s="57" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B23" s="1"/>
       <c r="C23" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="D23" s="51"/>
-      <c r="E23" s="44"/>
-    </row>
-    <row r="24" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="D23" s="47"/>
+      <c r="E23" s="57"/>
+    </row>
+    <row r="24" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B24" s="12">
         <v>12</v>
       </c>
       <c r="C24" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D24" s="49" t="s">
+      <c r="D24" s="48" t="s">
         <v>28</v>
       </c>
-      <c r="E24" s="44" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E24" s="57" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B25" s="1"/>
       <c r="C25" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="D25" s="50"/>
-      <c r="E25" s="44"/>
-    </row>
-    <row r="26" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="D25" s="49"/>
+      <c r="E25" s="57"/>
+    </row>
+    <row r="26" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B26" s="12">
         <v>13</v>
       </c>
       <c r="C26" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="D26" s="47" t="s">
+      <c r="D26" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="E26" s="44"/>
-    </row>
-    <row r="27" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E26" s="57"/>
+    </row>
+    <row r="27" spans="2:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B27" s="1"/>
       <c r="C27" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D27" s="51"/>
-      <c r="E27" s="44"/>
-    </row>
-    <row r="28" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D27" s="47"/>
+      <c r="E27" s="57"/>
+    </row>
+    <row r="28" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="12">
         <v>14</v>
       </c>
       <c r="C28" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="D28" s="49" t="s">
+      <c r="D28" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="E28" s="44"/>
-    </row>
-    <row r="29" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E28" s="57"/>
+    </row>
+    <row r="29" spans="2:5" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B29" s="1"/>
       <c r="C29" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D29" s="50"/>
-      <c r="E29" s="44"/>
-    </row>
-    <row r="30" spans="2:5" ht="31.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D29" s="49"/>
+      <c r="E29" s="57"/>
+    </row>
+    <row r="30" spans="2:5" ht="32.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B30" s="21">
         <v>15</v>
       </c>
@@ -2267,7 +2279,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="31" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B31" s="1">
         <v>16</v>
       </c>
@@ -2278,7 +2290,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="32" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B32" s="1">
         <v>17</v>
       </c>
@@ -2289,7 +2301,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="33" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B33" s="1">
         <v>18</v>
       </c>
@@ -2300,7 +2312,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="34" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B34" s="1">
         <v>19</v>
       </c>
@@ -2311,7 +2323,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="35" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B35" s="1">
         <v>20</v>
       </c>
@@ -2322,7 +2334,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="36" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B36" s="1">
         <v>21</v>
       </c>
@@ -2333,7 +2345,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="37" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B37" s="1">
         <v>22</v>
       </c>
@@ -2344,7 +2356,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="38" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B38" s="1">
         <v>23</v>
       </c>
@@ -2355,7 +2367,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="39" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B39" s="1">
         <v>24</v>
       </c>
@@ -2366,7 +2378,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="40" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B40" s="1">
         <v>25</v>
       </c>
@@ -2377,7 +2389,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="41" spans="2:5" s="27" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:5" s="27" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
       <c r="C41" s="28" t="s">
         <v>69</v>
       </c>
@@ -2385,19 +2397,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="D6:D7"/>
     <mergeCell ref="E26:E27"/>
     <mergeCell ref="E28:E29"/>
     <mergeCell ref="E12:E13"/>
@@ -2410,6 +2409,19 @@
     <mergeCell ref="E24:E25"/>
     <mergeCell ref="E16:E17"/>
     <mergeCell ref="E14:E15"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="D18:D19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2418,31 +2430,31 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:F16"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="3.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="47.42578125" customWidth="1"/>
-    <col min="4" max="4" width="93.28515625" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="35.7109375" customWidth="1"/>
+    <col min="2" max="2" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="47.44140625" customWidth="1"/>
+    <col min="4" max="4" width="93.33203125" customWidth="1"/>
+    <col min="5" max="5" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E1" s="67" t="s">
+    <row r="1" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E1" s="44" t="s">
         <v>48</v>
       </c>
-      <c r="F1" s="67" t="s">
+      <c r="F1" s="44" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="2" spans="2:6" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="26">
         <v>26</v>
       </c>
@@ -2453,13 +2465,11 @@
         <v>14</v>
       </c>
       <c r="E2" t="s">
-        <v>271</v>
-      </c>
-      <c r="F2" s="68" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="3" spans="2:6" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>268</v>
+      </c>
+      <c r="F2" s="45"/>
+    </row>
+    <row r="3" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="4">
         <v>27</v>
       </c>
@@ -2470,13 +2480,11 @@
         <v>52</v>
       </c>
       <c r="E3" t="s">
-        <v>271</v>
-      </c>
-      <c r="F3" s="68" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>268</v>
+      </c>
+      <c r="F3" s="45"/>
+    </row>
+    <row r="4" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="2">
         <v>28</v>
       </c>
@@ -2487,13 +2495,11 @@
         <v>54</v>
       </c>
       <c r="E4" t="s">
-        <v>271</v>
-      </c>
-      <c r="F4" s="68" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>268</v>
+      </c>
+      <c r="F4" s="45"/>
+    </row>
+    <row r="5" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="4">
         <v>29</v>
       </c>
@@ -2504,13 +2510,11 @@
         <v>56</v>
       </c>
       <c r="E5" t="s">
-        <v>271</v>
-      </c>
-      <c r="F5" s="68" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>268</v>
+      </c>
+      <c r="F5" s="45"/>
+    </row>
+    <row r="6" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="26">
         <v>30</v>
       </c>
@@ -2521,13 +2525,11 @@
         <v>56</v>
       </c>
       <c r="E6" t="s">
-        <v>271</v>
-      </c>
-      <c r="F6" s="68" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>268</v>
+      </c>
+      <c r="F6" s="45"/>
+    </row>
+    <row r="7" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="4">
         <v>31</v>
       </c>
@@ -2538,13 +2540,11 @@
         <v>56</v>
       </c>
       <c r="E7" t="s">
-        <v>271</v>
-      </c>
-      <c r="F7" s="68" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>268</v>
+      </c>
+      <c r="F7" s="45"/>
+    </row>
+    <row r="8" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="2">
         <v>32</v>
       </c>
@@ -2555,80 +2555,78 @@
         <v>60</v>
       </c>
       <c r="E8" t="s">
-        <v>271</v>
-      </c>
-      <c r="F8" s="68" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
+        <v>268</v>
+      </c>
+      <c r="F8" s="45"/>
+    </row>
+    <row r="9" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B9" s="10">
         <v>33</v>
       </c>
-      <c r="C9" s="47" t="s">
+      <c r="C9" s="46" t="s">
         <v>61</v>
       </c>
       <c r="D9" s="8" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="10" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="11"/>
-      <c r="C10" s="51"/>
+      <c r="C10" s="47"/>
       <c r="D10" s="4" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="11" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B11" s="24">
         <v>34</v>
       </c>
-      <c r="C11" s="49" t="s">
+      <c r="C11" s="48" t="s">
         <v>64</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="12" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="13"/>
-      <c r="C12" s="50"/>
+      <c r="C12" s="49"/>
       <c r="D12" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B13" s="10">
         <v>35</v>
       </c>
-      <c r="C13" s="47" t="s">
+      <c r="C13" s="46" t="s">
         <v>66</v>
       </c>
       <c r="D13" s="8" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="14" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="11"/>
-      <c r="C14" s="51"/>
+      <c r="C14" s="47"/>
       <c r="D14" s="4" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="15" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B15" s="24">
         <v>36</v>
       </c>
-      <c r="C15" s="49" t="s">
+      <c r="C15" s="48" t="s">
         <v>68</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="13"/>
-      <c r="C16" s="50"/>
+      <c r="C16" s="49"/>
       <c r="D16" s="2" t="s">
         <v>67</v>
       </c>
@@ -2646,21 +2644,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B2:F80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B11" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21:E22"/>
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19:E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="56" customWidth="1"/>
-    <col min="4" max="4" width="108.28515625" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="41"/>
+    <col min="4" max="4" width="108.33203125" customWidth="1"/>
+    <col min="5" max="5" width="9.109375" style="41"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>177</v>
       </c>
@@ -2671,287 +2669,291 @@
         <v>261</v>
       </c>
     </row>
-    <row r="3" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B3" s="52">
+    <row r="3" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="B3" s="53">
         <v>37</v>
       </c>
       <c r="C3" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="52" t="s">
+      <c r="D3" s="53" t="s">
         <v>71</v>
       </c>
-      <c r="E3" s="44" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="50"/>
+      <c r="E3" s="57" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="49"/>
       <c r="C4" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="D4" s="50"/>
-      <c r="E4" s="44"/>
-    </row>
-    <row r="5" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B5" s="47">
+      <c r="D4" s="49"/>
+      <c r="E4" s="57"/>
+    </row>
+    <row r="5" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="B5" s="46">
         <v>38</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="47" t="s">
+      <c r="D5" s="46" t="s">
         <v>73</v>
       </c>
-      <c r="E5" s="44" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="51"/>
+      <c r="E5" s="57" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="47"/>
       <c r="C6" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="D6" s="51"/>
-      <c r="E6" s="44"/>
-    </row>
-    <row r="7" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B7" s="49">
+      <c r="D6" s="47"/>
+      <c r="E6" s="57"/>
+    </row>
+    <row r="7" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="B7" s="48">
         <v>39</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="49" t="s">
+      <c r="D7" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="E7" s="44"/>
-    </row>
-    <row r="8" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="50"/>
+      <c r="E7" s="57" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="49"/>
       <c r="C8" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="D8" s="50"/>
-      <c r="E8" s="44"/>
-    </row>
-    <row r="9" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B9" s="47">
+      <c r="D8" s="49"/>
+      <c r="E8" s="57"/>
+    </row>
+    <row r="9" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="B9" s="46">
         <v>40</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="D9" s="47" t="s">
+      <c r="D9" s="46" t="s">
         <v>77</v>
       </c>
-      <c r="E9" s="44" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="51"/>
+      <c r="E9" s="57" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="47"/>
       <c r="C10" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="D10" s="51"/>
-      <c r="E10" s="44"/>
-    </row>
-    <row r="11" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B11" s="49">
+      <c r="D10" s="47"/>
+      <c r="E10" s="57"/>
+    </row>
+    <row r="11" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="B11" s="48">
         <v>41</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="D11" s="49" t="s">
+      <c r="D11" s="48" t="s">
         <v>80</v>
       </c>
-      <c r="E11" s="44" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="50"/>
+      <c r="E11" s="57" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="49"/>
       <c r="C12" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="D12" s="50"/>
-      <c r="E12" s="44"/>
-    </row>
-    <row r="13" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B13" s="47">
+      <c r="D12" s="49"/>
+      <c r="E12" s="57"/>
+    </row>
+    <row r="13" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="B13" s="46">
         <v>42</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="D13" s="47" t="s">
+      <c r="D13" s="46" t="s">
         <v>83</v>
       </c>
-      <c r="E13" s="44" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="51"/>
+      <c r="E13" s="57" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="47"/>
       <c r="C14" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="D14" s="51"/>
-      <c r="E14" s="44"/>
-    </row>
-    <row r="15" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B15" s="62">
+      <c r="D14" s="47"/>
+      <c r="E14" s="57"/>
+    </row>
+    <row r="15" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="B15" s="65">
         <v>43</v>
       </c>
       <c r="C15" s="31" t="s">
         <v>84</v>
       </c>
-      <c r="D15" s="62" t="s">
+      <c r="D15" s="65" t="s">
         <v>86</v>
       </c>
-      <c r="E15" s="44" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="57"/>
+      <c r="E15" s="57" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="61"/>
       <c r="C16" s="32" t="s">
         <v>85</v>
       </c>
-      <c r="D16" s="57"/>
-      <c r="E16" s="44"/>
-    </row>
-    <row r="17" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="D16" s="61"/>
+      <c r="E16" s="57"/>
+    </row>
+    <row r="17" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B17" s="58">
         <v>44</v>
       </c>
       <c r="C17" s="33" t="s">
         <v>87</v>
       </c>
-      <c r="D17" s="63">
+      <c r="D17" s="66">
         <v>987654321</v>
       </c>
-      <c r="E17" s="44"/>
-    </row>
-    <row r="18" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E17" s="57"/>
+    </row>
+    <row r="18" spans="2:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B18" s="59"/>
       <c r="C18" s="34" t="s">
         <v>88</v>
       </c>
-      <c r="D18" s="64"/>
-      <c r="E18" s="44"/>
-    </row>
-    <row r="19" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B19" s="56">
+      <c r="D18" s="67"/>
+      <c r="E18" s="57"/>
+    </row>
+    <row r="19" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="B19" s="60">
         <v>45</v>
       </c>
       <c r="C19" s="35" t="s">
         <v>89</v>
       </c>
-      <c r="D19" s="56">
+      <c r="D19" s="60">
         <v>1433</v>
       </c>
-      <c r="E19" s="44"/>
-    </row>
-    <row r="20" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="57"/>
+      <c r="E19" s="57" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="61"/>
       <c r="C20" s="32" t="s">
         <v>90</v>
       </c>
-      <c r="D20" s="57"/>
-      <c r="E20" s="44"/>
-    </row>
-    <row r="21" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="D20" s="61"/>
+      <c r="E20" s="57"/>
+    </row>
+    <row r="21" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B21" s="58">
         <v>46</v>
       </c>
       <c r="C21" s="33" t="s">
         <v>91</v>
       </c>
-      <c r="D21" s="60">
+      <c r="D21" s="63">
         <v>43925</v>
       </c>
-      <c r="E21" s="69" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="22" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E21" s="68" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B22" s="59"/>
       <c r="C22" s="34" t="s">
         <v>92</v>
       </c>
-      <c r="D22" s="61"/>
-      <c r="E22" s="44"/>
-    </row>
-    <row r="23" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B23" s="56">
+      <c r="D22" s="72"/>
+      <c r="E22" s="57"/>
+    </row>
+    <row r="23" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="B23" s="60">
         <v>47</v>
       </c>
       <c r="C23" s="35" t="s">
         <v>93</v>
       </c>
-      <c r="D23" s="56" t="s">
+      <c r="D23" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="E23" s="69" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="57"/>
+      <c r="E23" s="68" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B24" s="61"/>
       <c r="C24" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="D24" s="57"/>
-      <c r="E24" s="44"/>
-    </row>
-    <row r="25" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="D24" s="71"/>
+      <c r="E24" s="57"/>
+    </row>
+    <row r="25" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B25" s="58">
         <v>48</v>
       </c>
       <c r="C25" s="33" t="s">
         <v>94</v>
       </c>
-      <c r="D25" s="60">
+      <c r="D25" s="63">
         <v>43834</v>
       </c>
-      <c r="E25" s="69" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="26" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E25" s="68" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B26" s="59"/>
       <c r="C26" s="34" t="s">
         <v>95</v>
       </c>
-      <c r="D26" s="61"/>
-      <c r="E26" s="44"/>
-    </row>
-    <row r="27" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B27" s="56">
+      <c r="D26" s="64"/>
+      <c r="E26" s="57"/>
+    </row>
+    <row r="27" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="B27" s="60">
         <v>49</v>
       </c>
       <c r="C27" s="35" t="s">
         <v>96</v>
       </c>
-      <c r="D27" s="56">
+      <c r="D27" s="60">
         <v>0</v>
       </c>
-      <c r="E27" s="69" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="28" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="57"/>
+      <c r="E27" s="68" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B28" s="61"/>
       <c r="C28" s="32" t="s">
         <v>96</v>
       </c>
-      <c r="D28" s="57"/>
-      <c r="E28" s="44"/>
-    </row>
-    <row r="29" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="D28" s="61"/>
+      <c r="E28" s="57"/>
+    </row>
+    <row r="29" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B29" s="58">
         <v>50</v>
       </c>
@@ -2961,18 +2963,20 @@
       <c r="D29" s="58">
         <v>5</v>
       </c>
-      <c r="E29" s="44"/>
-    </row>
-    <row r="30" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E29" s="68" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B30" s="59"/>
       <c r="C30" s="34" t="s">
         <v>98</v>
       </c>
       <c r="D30" s="59"/>
-      <c r="E30" s="44"/>
-    </row>
-    <row r="31" spans="2:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="56">
+      <c r="E30" s="57"/>
+    </row>
+    <row r="31" spans="2:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="60">
         <v>51</v>
       </c>
       <c r="C31" s="35" t="s">
@@ -2981,21 +2985,21 @@
       <c r="D31" s="35" t="s">
         <v>101</v>
       </c>
-      <c r="E31" s="44" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="32" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="57"/>
+      <c r="E31" s="57" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B32" s="61"/>
       <c r="C32" s="32" t="s">
         <v>100</v>
       </c>
       <c r="D32" s="36" t="s">
         <v>102</v>
       </c>
-      <c r="E32" s="44"/>
-    </row>
-    <row r="33" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="E32" s="57"/>
+    </row>
+    <row r="33" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B33" s="58">
         <v>52</v>
       </c>
@@ -3005,37 +3009,39 @@
       <c r="D33" s="58" t="s">
         <v>105</v>
       </c>
-      <c r="E33" s="44"/>
-    </row>
-    <row r="34" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E33" s="57"/>
+    </row>
+    <row r="34" spans="2:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B34" s="59"/>
       <c r="C34" s="34" t="s">
         <v>104</v>
       </c>
       <c r="D34" s="59"/>
-      <c r="E34" s="44"/>
-    </row>
-    <row r="35" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B35" s="56">
+      <c r="E34" s="57"/>
+    </row>
+    <row r="35" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="B35" s="60">
         <v>53</v>
       </c>
       <c r="C35" s="35" t="s">
         <v>106</v>
       </c>
-      <c r="D35" s="56" t="s">
+      <c r="D35" s="60" t="s">
         <v>108</v>
       </c>
-      <c r="E35" s="44"/>
-    </row>
-    <row r="36" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="57"/>
+      <c r="E35" s="57" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B36" s="61"/>
       <c r="C36" s="32" t="s">
         <v>107</v>
       </c>
-      <c r="D36" s="57"/>
-      <c r="E36" s="44"/>
-    </row>
-    <row r="37" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="D36" s="61"/>
+      <c r="E36" s="57"/>
+    </row>
+    <row r="37" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B37" s="58">
         <v>54</v>
       </c>
@@ -3045,19 +3051,19 @@
       <c r="D37" s="58" t="s">
         <v>111</v>
       </c>
-      <c r="E37" s="44" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="38" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E37" s="57" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B38" s="59"/>
       <c r="C38" s="34" t="s">
         <v>110</v>
       </c>
       <c r="D38" s="59"/>
-      <c r="E38" s="44"/>
-    </row>
-    <row r="39" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E38" s="57"/>
+    </row>
+    <row r="39" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B39" s="36">
         <v>55</v>
       </c>
@@ -3071,7 +3077,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="40" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B40" s="38">
         <v>56</v>
       </c>
@@ -3085,7 +3091,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="41" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B41" s="36">
         <v>57</v>
       </c>
@@ -3099,51 +3105,51 @@
         <v>268</v>
       </c>
     </row>
-    <row r="42" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="65">
+    <row r="42" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B42" s="62">
         <v>58</v>
       </c>
       <c r="C42" s="39" t="s">
         <v>117</v>
       </c>
-      <c r="D42" s="65" t="s">
+      <c r="D42" s="62" t="s">
         <v>36</v>
       </c>
-      <c r="E42" s="44" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="43" spans="2:5" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E42" s="57" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B43" s="59"/>
       <c r="C43" s="34" t="s">
         <v>118</v>
       </c>
       <c r="D43" s="59"/>
-      <c r="E43" s="44"/>
-    </row>
-    <row r="44" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B44" s="56">
+      <c r="E43" s="57"/>
+    </row>
+    <row r="44" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="B44" s="60">
         <v>59</v>
       </c>
       <c r="C44" s="35" t="s">
         <v>119</v>
       </c>
-      <c r="D44" s="56" t="s">
+      <c r="D44" s="60" t="s">
         <v>36</v>
       </c>
-      <c r="E44" s="44" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="45" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="57"/>
+      <c r="E44" s="57" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B45" s="61"/>
       <c r="C45" s="32" t="s">
         <v>120</v>
       </c>
-      <c r="D45" s="57"/>
-      <c r="E45" s="44"/>
-    </row>
-    <row r="46" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D45" s="61"/>
+      <c r="E45" s="57"/>
+    </row>
+    <row r="46" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B46" s="38">
         <v>60</v>
       </c>
@@ -3157,7 +3163,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="47" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B47" s="36">
         <v>61</v>
       </c>
@@ -3168,7 +3174,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="48" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B48" s="38">
         <v>62</v>
       </c>
@@ -3182,27 +3188,27 @@
         <v>267</v>
       </c>
     </row>
-    <row r="49" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B49" s="56">
+    <row r="49" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="B49" s="60">
         <v>63</v>
       </c>
       <c r="C49" s="35" t="s">
         <v>126</v>
       </c>
-      <c r="D49" s="56" t="s">
+      <c r="D49" s="60" t="s">
         <v>128</v>
       </c>
-      <c r="E49" s="44"/>
-    </row>
-    <row r="50" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="57"/>
+      <c r="E49" s="57"/>
+    </row>
+    <row r="50" spans="2:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B50" s="61"/>
       <c r="C50" s="32" t="s">
         <v>127</v>
       </c>
-      <c r="D50" s="57"/>
-      <c r="E50" s="44"/>
-    </row>
-    <row r="51" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="D50" s="61"/>
+      <c r="E50" s="57"/>
+    </row>
+    <row r="51" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B51" s="58">
         <v>64</v>
       </c>
@@ -3212,37 +3218,37 @@
       <c r="D51" s="58" t="s">
         <v>131</v>
       </c>
-      <c r="E51" s="44"/>
-    </row>
-    <row r="52" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E51" s="57"/>
+    </row>
+    <row r="52" spans="2:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B52" s="59"/>
       <c r="C52" s="34" t="s">
         <v>130</v>
       </c>
       <c r="D52" s="59"/>
-      <c r="E52" s="44"/>
-    </row>
-    <row r="53" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B53" s="56">
+      <c r="E52" s="57"/>
+    </row>
+    <row r="53" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="B53" s="60">
         <v>65</v>
       </c>
       <c r="C53" s="35" t="s">
         <v>132</v>
       </c>
-      <c r="D53" s="56" t="s">
+      <c r="D53" s="60" t="s">
         <v>134</v>
       </c>
-      <c r="E53" s="44"/>
-    </row>
-    <row r="54" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="57"/>
+      <c r="E53" s="57"/>
+    </row>
+    <row r="54" spans="2:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B54" s="61"/>
       <c r="C54" s="32" t="s">
         <v>133</v>
       </c>
-      <c r="D54" s="57"/>
-      <c r="E54" s="44"/>
-    </row>
-    <row r="55" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D54" s="61"/>
+      <c r="E54" s="57"/>
+    </row>
+    <row r="55" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B55" s="38">
         <v>66</v>
       </c>
@@ -3256,7 +3262,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="56" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B56" s="36">
         <v>67</v>
       </c>
@@ -3270,7 +3276,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="57" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B57" s="38">
         <v>68</v>
       </c>
@@ -3284,7 +3290,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="58" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B58" s="36">
         <v>69</v>
       </c>
@@ -3298,7 +3304,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="59" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B59" s="38">
         <v>70</v>
       </c>
@@ -3312,7 +3318,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="60" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B60" s="36">
         <v>71</v>
       </c>
@@ -3326,7 +3332,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="61" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B61" s="38">
         <v>72</v>
       </c>
@@ -3340,7 +3346,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="62" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B62" s="36">
         <v>73</v>
       </c>
@@ -3354,7 +3360,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="63" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B63" s="38">
         <v>74</v>
       </c>
@@ -3368,7 +3374,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="64" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B64" s="26">
         <v>75</v>
       </c>
@@ -3382,7 +3388,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="65" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B65" s="4">
         <v>76</v>
       </c>
@@ -3396,7 +3402,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="66" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B66" s="2">
         <v>77</v>
       </c>
@@ -3410,7 +3416,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="67" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B67" s="2">
         <v>78</v>
       </c>
@@ -3424,7 +3430,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="68" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B68" s="4">
         <v>79</v>
       </c>
@@ -3438,7 +3444,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="69" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B69" s="2">
         <v>80</v>
       </c>
@@ -3452,7 +3458,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="70" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B70" s="4">
         <v>81</v>
       </c>
@@ -3466,7 +3472,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="71" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B71" s="2">
         <v>82</v>
       </c>
@@ -3480,7 +3486,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="72" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B72" s="4">
         <v>83</v>
       </c>
@@ -3494,7 +3500,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="73" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B73" s="2">
         <v>84</v>
       </c>
@@ -3508,7 +3514,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="74" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B74" s="4">
         <v>85</v>
       </c>
@@ -3519,7 +3525,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="75" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B75" s="2">
         <v>86</v>
       </c>
@@ -3533,7 +3539,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="76" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B76" s="4">
         <v>87</v>
       </c>
@@ -3547,7 +3553,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="77" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B77" s="2">
         <v>88</v>
       </c>
@@ -3561,7 +3567,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="78" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B78" s="4">
         <v>89</v>
       </c>
@@ -3575,7 +3581,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="79" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B79" s="2">
         <v>90</v>
       </c>
@@ -3586,7 +3592,7 @@
         <v>43178</v>
       </c>
     </row>
-    <row r="80" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B80" s="4">
         <v>91</v>
       </c>
@@ -3602,37 +3608,27 @@
     </row>
   </sheetData>
   <mergeCells count="68">
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="D51:D52"/>
-    <mergeCell ref="B53:B54"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="D44:D45"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="D49:D50"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="D42:D43"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E49:E50"/>
+    <mergeCell ref="E51:E52"/>
+    <mergeCell ref="E53:E54"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="E44:E45"/>
+    <mergeCell ref="E42:E43"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="E31:E32"/>
     <mergeCell ref="E33:E34"/>
     <mergeCell ref="E35:E36"/>
     <mergeCell ref="B3:B4"/>
@@ -3649,49 +3645,59 @@
     <mergeCell ref="D9:D10"/>
     <mergeCell ref="B19:B20"/>
     <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="E49:E50"/>
-    <mergeCell ref="E51:E52"/>
-    <mergeCell ref="E53:E54"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="E44:E45"/>
-    <mergeCell ref="E42:E43"/>
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="D51:D52"/>
+    <mergeCell ref="B53:B54"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="D49:D50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B1:F20"/>
   <sheetViews>
-    <sheetView topLeftCell="B2" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E2" sqref="E2:E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="7.85546875" customWidth="1"/>
-    <col min="3" max="3" width="56.85546875" customWidth="1"/>
+    <col min="2" max="2" width="7.88671875" customWidth="1"/>
+    <col min="3" max="3" width="56.88671875" customWidth="1"/>
     <col min="4" max="4" width="100" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="41"/>
+    <col min="5" max="5" width="9.109375" style="41"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E1" s="41" t="s">
         <v>260</v>
       </c>
@@ -3699,73 +3705,73 @@
         <v>259</v>
       </c>
     </row>
-    <row r="2" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B2" s="52">
+    <row r="2" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="B2" s="53">
         <v>92</v>
       </c>
       <c r="C2" s="16" t="s">
         <v>178</v>
       </c>
-      <c r="D2" s="52" t="s">
+      <c r="D2" s="53" t="s">
         <v>36</v>
       </c>
-      <c r="E2" s="44" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="3" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="50"/>
+      <c r="E2" s="57" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="49"/>
       <c r="C3" s="7" t="s">
         <v>179</v>
       </c>
-      <c r="D3" s="50"/>
-      <c r="E3" s="44"/>
-    </row>
-    <row r="4" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B4" s="47">
+      <c r="D3" s="49"/>
+      <c r="E3" s="57"/>
+    </row>
+    <row r="4" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="B4" s="46">
         <v>93</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="47" t="s">
+      <c r="D4" s="46" t="s">
         <v>71</v>
       </c>
-      <c r="E4" s="44" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="51"/>
+      <c r="E4" s="57" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="47"/>
       <c r="C5" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="D5" s="51"/>
-      <c r="E5" s="44"/>
-    </row>
-    <row r="6" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B6" s="49">
+      <c r="D5" s="47"/>
+      <c r="E5" s="57"/>
+    </row>
+    <row r="6" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="B6" s="48">
         <v>94</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="49" t="s">
+      <c r="D6" s="48" t="s">
         <v>182</v>
       </c>
-      <c r="E6" s="44" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="50"/>
+      <c r="E6" s="57" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="49"/>
       <c r="C7" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="D7" s="50"/>
-      <c r="E7" s="44"/>
-    </row>
-    <row r="8" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D7" s="49"/>
+      <c r="E7" s="57"/>
+    </row>
+    <row r="8" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="4">
         <v>95</v>
       </c>
@@ -3779,7 +3785,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="9" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="2">
         <v>96</v>
       </c>
@@ -3793,7 +3799,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="10" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="4">
         <v>97</v>
       </c>
@@ -3807,7 +3813,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="11" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" s="2">
         <v>98</v>
       </c>
@@ -3818,53 +3824,53 @@
         <v>189</v>
       </c>
     </row>
-    <row r="12" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B12" s="66">
+    <row r="12" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="B12" s="69">
         <v>99</v>
       </c>
-      <c r="C12" s="66" t="s">
+      <c r="C12" s="69" t="s">
         <v>190</v>
       </c>
       <c r="D12" s="29" t="s">
         <v>191</v>
       </c>
-      <c r="E12" s="44" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B13" s="48"/>
-      <c r="C13" s="48"/>
+      <c r="E12" s="57" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="B13" s="52"/>
+      <c r="C13" s="52"/>
       <c r="D13" s="8" t="s">
         <v>192</v>
       </c>
-      <c r="E13" s="44"/>
-    </row>
-    <row r="14" spans="2:6" ht="33" x14ac:dyDescent="0.25">
-      <c r="B14" s="48"/>
-      <c r="C14" s="48"/>
+      <c r="E13" s="57"/>
+    </row>
+    <row r="14" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="B14" s="52"/>
+      <c r="C14" s="52"/>
       <c r="D14" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="E14" s="44"/>
-    </row>
-    <row r="15" spans="2:6" ht="49.5" x14ac:dyDescent="0.25">
-      <c r="B15" s="48"/>
-      <c r="C15" s="48"/>
+      <c r="E14" s="57"/>
+    </row>
+    <row r="15" spans="2:6" ht="50.4" x14ac:dyDescent="0.3">
+      <c r="B15" s="52"/>
+      <c r="C15" s="52"/>
       <c r="D15" s="8" t="s">
         <v>194</v>
       </c>
-      <c r="E15" s="44"/>
-    </row>
-    <row r="16" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="51"/>
-      <c r="C16" s="51"/>
+      <c r="E15" s="57"/>
+    </row>
+    <row r="16" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="47"/>
+      <c r="C16" s="47"/>
       <c r="D16" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="E16" s="44"/>
-    </row>
-    <row r="17" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E16" s="57"/>
+    </row>
+    <row r="17" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="2">
         <v>100</v>
       </c>
@@ -3878,38 +3884,43 @@
         <v>268</v>
       </c>
     </row>
-    <row r="18" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B18" s="47">
+    <row r="18" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="B18" s="46">
         <v>101</v>
       </c>
-      <c r="C18" s="47" t="s">
+      <c r="C18" s="46" t="s">
         <v>198</v>
       </c>
       <c r="D18" s="8" t="s">
         <v>199</v>
       </c>
-      <c r="E18" s="44" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B19" s="48"/>
-      <c r="C19" s="48"/>
+      <c r="E18" s="57" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="B19" s="52"/>
+      <c r="C19" s="52"/>
       <c r="D19" s="8" t="s">
         <v>200</v>
       </c>
-      <c r="E19" s="44"/>
-    </row>
-    <row r="20" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="51"/>
-      <c r="C20" s="51"/>
+      <c r="E19" s="57"/>
+    </row>
+    <row r="20" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="47"/>
+      <c r="C20" s="47"/>
       <c r="D20" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="E20" s="44"/>
+      <c r="E20" s="57"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="E12:E16"/>
+    <mergeCell ref="E18:E20"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="B4:B5"/>
@@ -3920,33 +3931,28 @@
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="B12:B16"/>
     <mergeCell ref="C12:C16"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="E12:E16"/>
-    <mergeCell ref="E18:E20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B1:F31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E5"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="59" customWidth="1"/>
-    <col min="4" max="4" width="52.7109375" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="41"/>
+    <col min="4" max="4" width="52.6640625" customWidth="1"/>
+    <col min="5" max="5" width="9.109375" style="41"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E1" s="41" t="s">
         <v>48</v>
       </c>
@@ -3954,73 +3960,73 @@
         <v>262</v>
       </c>
     </row>
-    <row r="2" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B2" s="52">
+    <row r="2" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="B2" s="53">
         <v>102</v>
       </c>
       <c r="C2" s="16" t="s">
         <v>178</v>
       </c>
-      <c r="D2" s="52" t="s">
+      <c r="D2" s="53" t="s">
         <v>36</v>
       </c>
-      <c r="E2" s="44" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="3" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="50"/>
+      <c r="E2" s="57" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="49"/>
       <c r="C3" s="7" t="s">
         <v>179</v>
       </c>
-      <c r="D3" s="50"/>
-      <c r="E3" s="44"/>
-    </row>
-    <row r="4" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B4" s="47">
+      <c r="D3" s="49"/>
+      <c r="E3" s="57"/>
+    </row>
+    <row r="4" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="B4" s="46">
         <v>103</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>202</v>
       </c>
-      <c r="D4" s="47" t="s">
+      <c r="D4" s="46" t="s">
         <v>71</v>
       </c>
-      <c r="E4" s="44" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="51"/>
+      <c r="E4" s="57" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="47"/>
       <c r="C5" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="D5" s="51"/>
-      <c r="E5" s="44"/>
-    </row>
-    <row r="6" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B6" s="49">
+      <c r="D5" s="47"/>
+      <c r="E5" s="57"/>
+    </row>
+    <row r="6" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="B6" s="48">
         <v>104</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="49" t="s">
+      <c r="D6" s="48" t="s">
         <v>182</v>
       </c>
-      <c r="E6" s="44" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="50"/>
+      <c r="E6" s="57" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="49"/>
       <c r="C7" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="D7" s="50"/>
-      <c r="E7" s="44"/>
-    </row>
-    <row r="8" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D7" s="49"/>
+      <c r="E7" s="57"/>
+    </row>
+    <row r="8" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="4">
         <v>105</v>
       </c>
@@ -4030,8 +4036,11 @@
       <c r="D8" s="4" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="9" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E8" s="41" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="2">
         <v>106</v>
       </c>
@@ -4045,7 +4054,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="10" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="4">
         <v>107</v>
       </c>
@@ -4059,7 +4068,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="11" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" s="2">
         <v>108</v>
       </c>
@@ -4070,7 +4079,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="12" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="4">
         <v>109</v>
       </c>
@@ -4081,7 +4090,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="13" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="2">
         <v>110</v>
       </c>
@@ -4092,7 +4101,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="14" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="4">
         <v>111</v>
       </c>
@@ -4103,7 +4112,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="26">
         <v>112</v>
       </c>
@@ -4117,7 +4126,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="16" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="4">
         <v>113</v>
       </c>
@@ -4131,7 +4140,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="17" spans="2:5" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:5" ht="34.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="2">
         <v>114</v>
       </c>
@@ -4142,7 +4151,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="18" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B18" s="4">
         <v>115</v>
       </c>
@@ -4156,7 +4165,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="19" spans="2:5" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B19" s="2">
         <v>116</v>
       </c>
@@ -4167,25 +4176,25 @@
         <v>222</v>
       </c>
     </row>
-    <row r="20" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B20" s="47">
+    <row r="20" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="B20" s="46">
         <v>117</v>
       </c>
       <c r="C20" s="8" t="s">
         <v>223</v>
       </c>
-      <c r="D20" s="47" t="s">
+      <c r="D20" s="46" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="21" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="51"/>
+    <row r="21" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="47"/>
       <c r="C21" s="4" t="s">
         <v>224</v>
       </c>
-      <c r="D21" s="51"/>
-    </row>
-    <row r="22" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D21" s="47"/>
+    </row>
+    <row r="22" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B22" s="2">
         <v>118</v>
       </c>
@@ -4196,7 +4205,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="23" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B23" s="4">
         <v>119</v>
       </c>
@@ -4210,7 +4219,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="24" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B24" s="2">
         <v>120</v>
       </c>
@@ -4224,7 +4233,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="25" spans="2:5" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:5" ht="34.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B25" s="4">
         <v>121</v>
       </c>
@@ -4238,7 +4247,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="26" spans="2:5" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:5" ht="34.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B26" s="2">
         <v>122</v>
       </c>
@@ -4252,7 +4261,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="27" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B27" s="4">
         <v>123</v>
       </c>
@@ -4266,7 +4275,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="28" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B28" s="2">
         <v>124</v>
       </c>
@@ -4280,7 +4289,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="29" spans="2:5" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:5" ht="34.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B29" s="4">
         <v>125</v>
       </c>
@@ -4294,33 +4303,27 @@
         <v>268</v>
       </c>
     </row>
-    <row r="30" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B30" s="49">
+    <row r="30" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="B30" s="48">
         <v>126</v>
       </c>
       <c r="C30" s="6" t="s">
         <v>269</v>
       </c>
-      <c r="D30" s="49" t="s">
+      <c r="D30" s="48" t="s">
         <v>241</v>
       </c>
       <c r="E30" s="41" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="31" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="50"/>
+    <row r="31" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B31" s="49"/>
       <c r="C31" s="2"/>
-      <c r="D31" s="50"/>
+      <c r="D31" s="49"/>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="D20:D21"/>
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="E4:E5"/>
     <mergeCell ref="E6:E7"/>
@@ -4328,26 +4331,32 @@
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="D4:D5"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="D20:D21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="B1:F12"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="42.42578125" customWidth="1"/>
-    <col min="4" max="4" width="74.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.44140625" customWidth="1"/>
+    <col min="4" max="4" width="74.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E1" t="s">
         <v>260</v>
       </c>
@@ -4355,7 +4364,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="2" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="26">
         <v>127</v>
       </c>
@@ -4366,7 +4375,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="3" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="4">
         <v>128</v>
       </c>
@@ -4380,7 +4389,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="4" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="26">
         <v>129</v>
       </c>
@@ -4394,7 +4403,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="5" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="4">
         <v>130</v>
       </c>
@@ -4408,7 +4417,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="6" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="2">
         <v>131</v>
       </c>
@@ -4422,7 +4431,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="7" spans="2:6" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:6" ht="34.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="4">
         <v>132</v>
       </c>
@@ -4436,7 +4445,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="8" spans="2:6" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:6" ht="34.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="2">
         <v>133</v>
       </c>
@@ -4450,7 +4459,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="9" spans="2:6" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:6" ht="34.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="4">
         <v>134</v>
       </c>
@@ -4464,7 +4473,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="10" spans="2:6" ht="50.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:6" ht="51" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="2">
         <v>135</v>
       </c>
@@ -4478,7 +4487,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="11" spans="2:6" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:6" ht="34.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" s="4">
         <v>136</v>
       </c>
@@ -4492,7 +4501,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="12" spans="2:6" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:6" ht="34.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="2">
         <v>137</v>
       </c>

</xml_diff>

<commit_message>
SQL server Scripts added
</commit_message>
<xml_diff>
--- a/Checklist.xlsx
+++ b/Checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Prashant\AziraPowershellscript\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BA63D6D-6A52-4F99-BB5F-D95AA3E355BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B9C8DEC-CF7F-48FE-B2D3-AECD50E786E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Application" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="272">
   <si>
     <t xml:space="preserve"> Last Updated</t>
   </si>
@@ -1087,7 +1087,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1126,6 +1126,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1335,7 +1341,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1460,9 +1466,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1474,6 +1477,27 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1510,18 +1534,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1552,27 +1591,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Accent1" xfId="1" builtinId="29"/>
@@ -1981,11 +2015,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:F41"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D28" sqref="D28:D29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D8" sqref="D8:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1997,7 +2031,7 @@
     <col min="6" max="6" width="11.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1" s="38" t="s">
         <v>264</v>
       </c>
@@ -2014,14 +2048,14 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="54" t="s">
+    <row r="2" spans="1:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
-    </row>
-    <row r="3" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C2" s="61"/>
+      <c r="D2" s="61"/>
+    </row>
+    <row r="3" spans="1:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="12">
         <v>1</v>
       </c>
@@ -2035,7 +2069,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="4" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="10">
         <v>2</v>
       </c>
@@ -2049,132 +2083,134 @@
         <v>266</v>
       </c>
     </row>
-    <row r="5" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="59" t="s">
+    <row r="5" spans="1:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="65" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="60"/>
-      <c r="D5" s="60"/>
-    </row>
-    <row r="6" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="C5" s="66"/>
+      <c r="D5" s="66"/>
+    </row>
+    <row r="6" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B6" s="13">
         <v>3</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="57" t="s">
+      <c r="D6" s="63" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="61" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E6" s="67" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="1"/>
       <c r="C7" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="53"/>
-      <c r="E7" s="61"/>
-    </row>
-    <row r="8" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="D7" s="59"/>
+      <c r="E7" s="67"/>
+    </row>
+    <row r="8" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="92"/>
       <c r="B8" s="11">
         <v>4</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="50" t="s">
+      <c r="D8" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="61"/>
-    </row>
-    <row r="9" spans="2:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E8" s="67"/>
+    </row>
+    <row r="9" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="92"/>
       <c r="B9" s="1"/>
       <c r="C9" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="51"/>
-      <c r="E9" s="61"/>
-    </row>
-    <row r="10" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="D9" s="57"/>
+      <c r="E9" s="67"/>
+    </row>
+    <row r="10" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B10" s="13">
         <v>5</v>
       </c>
       <c r="C10" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="57" t="s">
+      <c r="D10" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="61" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E10" s="67" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" s="5"/>
       <c r="C11" s="16" t="s">
         <v>261</v>
       </c>
-      <c r="D11" s="58"/>
-      <c r="E11" s="61"/>
-    </row>
-    <row r="12" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="D11" s="64"/>
+      <c r="E11" s="67"/>
+    </row>
+    <row r="12" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B12" s="11">
         <v>6</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="50" t="s">
+      <c r="D12" s="56" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="61" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E12" s="67" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="5"/>
       <c r="C13" s="17" t="s">
         <v>261</v>
       </c>
-      <c r="D13" s="56"/>
-      <c r="E13" s="61"/>
-    </row>
-    <row r="14" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="D13" s="62"/>
+      <c r="E13" s="67"/>
+    </row>
+    <row r="14" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B14" s="11">
         <v>7</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="52" t="s">
+      <c r="D14" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="E14" s="61" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E14" s="67" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="1"/>
       <c r="C15" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="53"/>
-      <c r="E15" s="61"/>
-    </row>
-    <row r="16" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="D15" s="59"/>
+      <c r="E15" s="67"/>
+    </row>
+    <row r="16" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B16" s="11">
         <v>8</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="50" t="s">
+      <c r="D16" s="56" t="s">
         <v>17</v>
       </c>
-      <c r="E16" s="61" t="s">
+      <c r="E16" s="67" t="s">
         <v>266</v>
       </c>
     </row>
@@ -2183,8 +2219,8 @@
       <c r="C17" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="51"/>
-      <c r="E17" s="61"/>
+      <c r="D17" s="57"/>
+      <c r="E17" s="67"/>
     </row>
     <row r="18" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B18" s="11">
@@ -2193,10 +2229,10 @@
       <c r="C18" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D18" s="52">
+      <c r="D18" s="58">
         <v>4</v>
       </c>
-      <c r="E18" s="61" t="s">
+      <c r="E18" s="67" t="s">
         <v>266</v>
       </c>
     </row>
@@ -2205,8 +2241,8 @@
       <c r="C19" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D19" s="53"/>
-      <c r="E19" s="61"/>
+      <c r="D19" s="59"/>
+      <c r="E19" s="67"/>
     </row>
     <row r="20" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B20" s="1">
@@ -2218,7 +2254,7 @@
       <c r="D20" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E20" s="61" t="s">
+      <c r="E20" s="67" t="s">
         <v>266</v>
       </c>
     </row>
@@ -2229,7 +2265,7 @@
       <c r="D21" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E21" s="61"/>
+      <c r="E21" s="67"/>
     </row>
     <row r="22" spans="2:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="11">
@@ -2238,10 +2274,10 @@
       <c r="C22" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D22" s="50" t="s">
+      <c r="D22" s="56" t="s">
         <v>25</v>
       </c>
-      <c r="E22" s="61" t="s">
+      <c r="E22" s="67" t="s">
         <v>266</v>
       </c>
     </row>
@@ -2250,8 +2286,8 @@
       <c r="C23" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="D23" s="51"/>
-      <c r="E23" s="61"/>
+      <c r="D23" s="57"/>
+      <c r="E23" s="67"/>
     </row>
     <row r="24" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B24" s="11">
@@ -2260,10 +2296,10 @@
       <c r="C24" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D24" s="52" t="s">
+      <c r="D24" s="58" t="s">
         <v>28</v>
       </c>
-      <c r="E24" s="61" t="s">
+      <c r="E24" s="67" t="s">
         <v>266</v>
       </c>
     </row>
@@ -2272,8 +2308,8 @@
       <c r="C25" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="D25" s="53"/>
-      <c r="E25" s="61"/>
+      <c r="D25" s="59"/>
+      <c r="E25" s="67"/>
     </row>
     <row r="26" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B26" s="11">
@@ -2282,10 +2318,10 @@
       <c r="C26" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="D26" s="50" t="s">
+      <c r="D26" s="56" t="s">
         <v>31</v>
       </c>
-      <c r="E26" s="61" t="s">
+      <c r="E26" s="67" t="s">
         <v>266</v>
       </c>
     </row>
@@ -2294,8 +2330,8 @@
       <c r="C27" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D27" s="51"/>
-      <c r="E27" s="61"/>
+      <c r="D27" s="57"/>
+      <c r="E27" s="67"/>
     </row>
     <row r="28" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="11">
@@ -2304,18 +2340,18 @@
       <c r="C28" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="D28" s="52" t="s">
+      <c r="D28" s="58" t="s">
         <v>34</v>
       </c>
-      <c r="E28" s="61"/>
+      <c r="E28" s="67"/>
     </row>
     <row r="29" spans="2:5" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B29" s="1"/>
       <c r="C29" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D29" s="53"/>
-      <c r="E29" s="61"/>
+      <c r="D29" s="59"/>
+      <c r="E29" s="67"/>
     </row>
     <row r="30" spans="2:5" ht="32.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B30" s="20">
@@ -2328,15 +2364,18 @@
         <v>36</v>
       </c>
     </row>
-    <row r="31" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B31" s="1">
+    <row r="31" spans="2:5" s="44" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B31" s="89">
         <v>16</v>
       </c>
-      <c r="C31" s="19" t="s">
+      <c r="C31" s="90" t="s">
         <v>37</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="D31" s="91" t="s">
         <v>38</v>
+      </c>
+      <c r="E31" s="55" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="32" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
@@ -2350,15 +2389,18 @@
         <v>38</v>
       </c>
     </row>
-    <row r="33" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B33" s="1">
+    <row r="33" spans="2:5" s="44" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B33" s="89">
         <v>18</v>
       </c>
-      <c r="C33" s="19" t="s">
+      <c r="C33" s="90" t="s">
         <v>40</v>
       </c>
-      <c r="D33" s="2" t="s">
+      <c r="D33" s="91" t="s">
         <v>38</v>
+      </c>
+      <c r="E33" s="55" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="34" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
@@ -2372,15 +2414,18 @@
         <v>38</v>
       </c>
     </row>
-    <row r="35" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B35" s="1">
+    <row r="35" spans="2:5" s="44" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B35" s="89">
         <v>20</v>
       </c>
-      <c r="C35" s="19" t="s">
+      <c r="C35" s="90" t="s">
         <v>42</v>
       </c>
-      <c r="D35" s="2" t="s">
+      <c r="D35" s="91" t="s">
         <v>36</v>
+      </c>
+      <c r="E35" s="55" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="36" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
@@ -2394,15 +2439,18 @@
         <v>38</v>
       </c>
     </row>
-    <row r="37" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B37" s="1">
+    <row r="37" spans="2:5" s="44" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B37" s="89">
         <v>22</v>
       </c>
-      <c r="C37" s="19" t="s">
+      <c r="C37" s="90" t="s">
         <v>44</v>
       </c>
-      <c r="D37" s="2" t="s">
+      <c r="D37" s="91" t="s">
         <v>38</v>
+      </c>
+      <c r="E37" s="55" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="38" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
@@ -2416,15 +2464,18 @@
         <v>38</v>
       </c>
     </row>
-    <row r="39" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B39" s="1">
+    <row r="39" spans="2:5" s="44" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B39" s="89">
         <v>24</v>
       </c>
-      <c r="C39" s="19" t="s">
+      <c r="C39" s="90" t="s">
         <v>46</v>
       </c>
-      <c r="D39" s="2" t="s">
+      <c r="D39" s="91" t="s">
         <v>36</v>
+      </c>
+      <c r="E39" s="55" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="40" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
@@ -2482,8 +2533,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11:C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2608,93 +2659,93 @@
       </c>
       <c r="F8" s="43"/>
     </row>
-    <row r="9" spans="2:6" s="45" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B9" s="77">
+    <row r="9" spans="2:6" s="48" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="B9" s="49">
         <v>33</v>
       </c>
-      <c r="C9" s="78" t="s">
+      <c r="C9" s="68" t="s">
         <v>61</v>
       </c>
-      <c r="D9" s="79" t="s">
+      <c r="D9" s="50" t="s">
         <v>62</v>
       </c>
-      <c r="E9" s="80" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" s="45" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="81"/>
-      <c r="C10" s="82"/>
-      <c r="D10" s="44" t="s">
+      <c r="E9" s="70" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" s="48" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="51"/>
+      <c r="C10" s="69"/>
+      <c r="D10" s="45" t="s">
         <v>63</v>
       </c>
-      <c r="E10" s="80"/>
-    </row>
-    <row r="11" spans="2:6" s="45" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B11" s="77">
+      <c r="E10" s="70"/>
+    </row>
+    <row r="11" spans="2:6" s="48" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="B11" s="49">
         <v>34</v>
       </c>
-      <c r="C11" s="78" t="s">
+      <c r="C11" s="68" t="s">
         <v>64</v>
       </c>
-      <c r="D11" s="79" t="s">
+      <c r="D11" s="50" t="s">
         <v>65</v>
       </c>
-      <c r="E11" s="80" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" s="45" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="81"/>
-      <c r="C12" s="82"/>
-      <c r="D12" s="44" t="s">
+      <c r="E11" s="70" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" s="48" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="51"/>
+      <c r="C12" s="69"/>
+      <c r="D12" s="45" t="s">
         <v>63</v>
       </c>
-      <c r="E12" s="80"/>
-    </row>
-    <row r="13" spans="2:6" s="45" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B13" s="77">
+      <c r="E12" s="70"/>
+    </row>
+    <row r="13" spans="2:6" s="48" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="B13" s="49">
         <v>35</v>
       </c>
-      <c r="C13" s="78" t="s">
+      <c r="C13" s="68" t="s">
         <v>66</v>
       </c>
-      <c r="D13" s="79" t="s">
+      <c r="D13" s="50" t="s">
         <v>62</v>
       </c>
-      <c r="E13" s="80" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" s="45" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="81"/>
-      <c r="C14" s="82"/>
-      <c r="D14" s="44" t="s">
+      <c r="E13" s="70" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" s="48" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="51"/>
+      <c r="C14" s="69"/>
+      <c r="D14" s="45" t="s">
         <v>67</v>
       </c>
-      <c r="E14" s="80"/>
-    </row>
-    <row r="15" spans="2:6" s="45" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B15" s="77">
+      <c r="E14" s="70"/>
+    </row>
+    <row r="15" spans="2:6" s="48" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="B15" s="49">
         <v>36</v>
       </c>
-      <c r="C15" s="78" t="s">
+      <c r="C15" s="68" t="s">
         <v>68</v>
       </c>
-      <c r="D15" s="79" t="s">
+      <c r="D15" s="50" t="s">
         <v>65</v>
       </c>
-      <c r="E15" s="80" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6" s="45" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="81"/>
-      <c r="C16" s="82"/>
-      <c r="D16" s="44" t="s">
+      <c r="E15" s="70" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" s="48" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="51"/>
+      <c r="C16" s="69"/>
+      <c r="D16" s="45" t="s">
         <v>67</v>
       </c>
-      <c r="E16" s="80"/>
+      <c r="E16" s="70"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -2716,8 +2767,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B2:F80"/>
   <sheetViews>
-    <sheetView topLeftCell="B67" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C74" sqref="C74"/>
+    <sheetView topLeftCell="B40" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D53" sqref="D53:D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2739,313 +2790,313 @@
       </c>
     </row>
     <row r="3" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B3" s="57">
+      <c r="B3" s="63">
         <v>37</v>
       </c>
       <c r="C3" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="57" t="s">
+      <c r="D3" s="63" t="s">
         <v>71</v>
       </c>
-      <c r="E3" s="61" t="s">
+      <c r="E3" s="67" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="4" spans="2:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="53"/>
+      <c r="B4" s="59"/>
       <c r="C4" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="D4" s="53"/>
-      <c r="E4" s="61"/>
+      <c r="D4" s="59"/>
+      <c r="E4" s="67"/>
     </row>
     <row r="5" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B5" s="50">
+      <c r="B5" s="56">
         <v>38</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="50" t="s">
+      <c r="D5" s="56" t="s">
         <v>73</v>
       </c>
-      <c r="E5" s="61" t="s">
+      <c r="E5" s="67" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="6" spans="2:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="51"/>
+      <c r="B6" s="57"/>
       <c r="C6" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="D6" s="51"/>
-      <c r="E6" s="61"/>
+      <c r="D6" s="57"/>
+      <c r="E6" s="67"/>
     </row>
     <row r="7" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B7" s="52">
+      <c r="B7" s="58">
         <v>39</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="52" t="s">
+      <c r="D7" s="58" t="s">
         <v>31</v>
       </c>
-      <c r="E7" s="61" t="s">
+      <c r="E7" s="67" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="8" spans="2:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="53"/>
+      <c r="B8" s="59"/>
       <c r="C8" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="D8" s="53"/>
-      <c r="E8" s="61"/>
+      <c r="D8" s="59"/>
+      <c r="E8" s="67"/>
     </row>
     <row r="9" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B9" s="50">
+      <c r="B9" s="56">
         <v>40</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="D9" s="50" t="s">
+      <c r="D9" s="56" t="s">
         <v>77</v>
       </c>
-      <c r="E9" s="61" t="s">
+      <c r="E9" s="67" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="10" spans="2:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="51"/>
+      <c r="B10" s="57"/>
       <c r="C10" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="D10" s="51"/>
-      <c r="E10" s="61"/>
+      <c r="D10" s="57"/>
+      <c r="E10" s="67"/>
     </row>
     <row r="11" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B11" s="52">
+      <c r="B11" s="58">
         <v>41</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="D11" s="52" t="s">
+      <c r="D11" s="58" t="s">
         <v>80</v>
       </c>
-      <c r="E11" s="61" t="s">
+      <c r="E11" s="67" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="12" spans="2:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="53"/>
+      <c r="B12" s="59"/>
       <c r="C12" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="D12" s="53"/>
-      <c r="E12" s="61"/>
+      <c r="D12" s="59"/>
+      <c r="E12" s="67"/>
     </row>
     <row r="13" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B13" s="50">
+      <c r="B13" s="56">
         <v>42</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="D13" s="50" t="s">
+      <c r="D13" s="56" t="s">
         <v>83</v>
       </c>
-      <c r="E13" s="61" t="s">
+      <c r="E13" s="67" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="14" spans="2:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="51"/>
+      <c r="B14" s="57"/>
       <c r="C14" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="D14" s="51"/>
-      <c r="E14" s="61"/>
+      <c r="D14" s="57"/>
+      <c r="E14" s="67"/>
     </row>
     <row r="15" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B15" s="72">
+      <c r="B15" s="83">
         <v>43</v>
       </c>
       <c r="C15" s="29" t="s">
         <v>84</v>
       </c>
-      <c r="D15" s="72" t="s">
+      <c r="D15" s="83" t="s">
         <v>86</v>
       </c>
-      <c r="E15" s="61" t="s">
+      <c r="E15" s="67" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="16" spans="2:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="65"/>
+      <c r="B16" s="74"/>
       <c r="C16" s="30" t="s">
         <v>85</v>
       </c>
-      <c r="D16" s="65"/>
-      <c r="E16" s="61"/>
+      <c r="D16" s="74"/>
+      <c r="E16" s="67"/>
     </row>
     <row r="17" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B17" s="62">
+      <c r="B17" s="75">
         <v>44</v>
       </c>
       <c r="C17" s="31" t="s">
         <v>87</v>
       </c>
-      <c r="D17" s="73">
+      <c r="D17" s="84">
         <v>987654321</v>
       </c>
-      <c r="E17" s="61"/>
+      <c r="E17" s="67"/>
     </row>
     <row r="18" spans="2:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="63"/>
+      <c r="B18" s="76"/>
       <c r="C18" s="32" t="s">
         <v>88</v>
       </c>
-      <c r="D18" s="74"/>
-      <c r="E18" s="61"/>
+      <c r="D18" s="85"/>
+      <c r="E18" s="67"/>
     </row>
     <row r="19" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B19" s="64">
+      <c r="B19" s="73">
         <v>45</v>
       </c>
       <c r="C19" s="33" t="s">
         <v>89</v>
       </c>
-      <c r="D19" s="64">
+      <c r="D19" s="73">
         <v>1433</v>
       </c>
-      <c r="E19" s="61" t="s">
+      <c r="E19" s="67" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="20" spans="2:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="65"/>
+      <c r="B20" s="74"/>
       <c r="C20" s="30" t="s">
         <v>90</v>
       </c>
-      <c r="D20" s="65"/>
-      <c r="E20" s="61"/>
+      <c r="D20" s="74"/>
+      <c r="E20" s="67"/>
     </row>
     <row r="21" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B21" s="62">
+      <c r="B21" s="75">
         <v>46</v>
       </c>
       <c r="C21" s="31" t="s">
         <v>91</v>
       </c>
-      <c r="D21" s="69">
+      <c r="D21" s="80">
         <v>43925</v>
       </c>
-      <c r="E21" s="75" t="s">
+      <c r="E21" s="86" t="s">
         <v>269</v>
       </c>
     </row>
     <row r="22" spans="2:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="63"/>
+      <c r="B22" s="76"/>
       <c r="C22" s="32" t="s">
         <v>92</v>
       </c>
-      <c r="D22" s="71"/>
-      <c r="E22" s="61"/>
+      <c r="D22" s="82"/>
+      <c r="E22" s="67"/>
     </row>
     <row r="23" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B23" s="64">
+      <c r="B23" s="73">
         <v>47</v>
       </c>
       <c r="C23" s="33" t="s">
         <v>93</v>
       </c>
-      <c r="D23" s="67" t="s">
+      <c r="D23" s="78" t="s">
         <v>7</v>
       </c>
-      <c r="E23" s="75" t="s">
+      <c r="E23" s="86" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="24" spans="2:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="65"/>
+      <c r="B24" s="74"/>
       <c r="C24" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="D24" s="68"/>
-      <c r="E24" s="61"/>
+      <c r="D24" s="79"/>
+      <c r="E24" s="67"/>
     </row>
     <row r="25" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B25" s="62">
+      <c r="B25" s="75">
         <v>48</v>
       </c>
       <c r="C25" s="31" t="s">
         <v>94</v>
       </c>
-      <c r="D25" s="69">
+      <c r="D25" s="80">
         <v>43834</v>
       </c>
-      <c r="E25" s="75" t="s">
+      <c r="E25" s="86" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="26" spans="2:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B26" s="63"/>
+      <c r="B26" s="76"/>
       <c r="C26" s="32" t="s">
         <v>95</v>
       </c>
-      <c r="D26" s="70"/>
-      <c r="E26" s="61"/>
+      <c r="D26" s="81"/>
+      <c r="E26" s="67"/>
     </row>
     <row r="27" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B27" s="64">
+      <c r="B27" s="73">
         <v>49</v>
       </c>
       <c r="C27" s="33" t="s">
         <v>96</v>
       </c>
-      <c r="D27" s="64">
+      <c r="D27" s="73">
         <v>0</v>
       </c>
-      <c r="E27" s="75" t="s">
+      <c r="E27" s="86" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="28" spans="2:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="65"/>
+      <c r="B28" s="74"/>
       <c r="C28" s="30" t="s">
         <v>96</v>
       </c>
-      <c r="D28" s="65"/>
-      <c r="E28" s="61"/>
+      <c r="D28" s="74"/>
+      <c r="E28" s="67"/>
     </row>
     <row r="29" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B29" s="62">
+      <c r="B29" s="75">
         <v>50</v>
       </c>
       <c r="C29" s="31" t="s">
         <v>97</v>
       </c>
-      <c r="D29" s="62">
+      <c r="D29" s="75">
         <v>5</v>
       </c>
-      <c r="E29" s="75" t="s">
+      <c r="E29" s="86" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="30" spans="2:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B30" s="63"/>
+      <c r="B30" s="76"/>
       <c r="C30" s="32" t="s">
         <v>98</v>
       </c>
-      <c r="D30" s="63"/>
-      <c r="E30" s="61"/>
+      <c r="D30" s="76"/>
+      <c r="E30" s="67"/>
     </row>
     <row r="31" spans="2:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="64">
+      <c r="B31" s="73">
         <v>51</v>
       </c>
       <c r="C31" s="33" t="s">
@@ -3054,83 +3105,83 @@
       <c r="D31" s="33" t="s">
         <v>101</v>
       </c>
-      <c r="E31" s="61" t="s">
+      <c r="E31" s="67" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="32" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B32" s="65"/>
+      <c r="B32" s="74"/>
       <c r="C32" s="30" t="s">
         <v>100</v>
       </c>
       <c r="D32" s="34" t="s">
         <v>102</v>
       </c>
-      <c r="E32" s="61"/>
+      <c r="E32" s="67"/>
     </row>
     <row r="33" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B33" s="62">
+      <c r="B33" s="75">
         <v>52</v>
       </c>
       <c r="C33" s="31" t="s">
         <v>103</v>
       </c>
-      <c r="D33" s="62" t="s">
+      <c r="D33" s="75" t="s">
         <v>105</v>
       </c>
-      <c r="E33" s="61"/>
+      <c r="E33" s="67"/>
     </row>
     <row r="34" spans="2:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B34" s="63"/>
+      <c r="B34" s="76"/>
       <c r="C34" s="32" t="s">
         <v>104</v>
       </c>
-      <c r="D34" s="63"/>
-      <c r="E34" s="61"/>
+      <c r="D34" s="76"/>
+      <c r="E34" s="67"/>
     </row>
     <row r="35" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B35" s="64">
+      <c r="B35" s="73">
         <v>53</v>
       </c>
       <c r="C35" s="33" t="s">
         <v>106</v>
       </c>
-      <c r="D35" s="64" t="s">
+      <c r="D35" s="73" t="s">
         <v>108</v>
       </c>
-      <c r="E35" s="61" t="s">
+      <c r="E35" s="67" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="36" spans="2:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B36" s="65"/>
+      <c r="B36" s="74"/>
       <c r="C36" s="30" t="s">
         <v>107</v>
       </c>
-      <c r="D36" s="65"/>
-      <c r="E36" s="61"/>
+      <c r="D36" s="74"/>
+      <c r="E36" s="67"/>
     </row>
     <row r="37" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B37" s="62">
+      <c r="B37" s="75">
         <v>54</v>
       </c>
       <c r="C37" s="31" t="s">
         <v>109</v>
       </c>
-      <c r="D37" s="62" t="s">
+      <c r="D37" s="75" t="s">
         <v>111</v>
       </c>
-      <c r="E37" s="61" t="s">
+      <c r="E37" s="67" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="38" spans="2:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B38" s="63"/>
+      <c r="B38" s="76"/>
       <c r="C38" s="32" t="s">
         <v>110</v>
       </c>
-      <c r="D38" s="63"/>
-      <c r="E38" s="61"/>
+      <c r="D38" s="76"/>
+      <c r="E38" s="67"/>
     </row>
     <row r="39" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B39" s="34">
@@ -3175,48 +3226,48 @@
       </c>
     </row>
     <row r="42" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="66">
+      <c r="B42" s="77">
         <v>58</v>
       </c>
       <c r="C42" s="37" t="s">
         <v>117</v>
       </c>
-      <c r="D42" s="66" t="s">
+      <c r="D42" s="77" t="s">
         <v>36</v>
       </c>
-      <c r="E42" s="61" t="s">
+      <c r="E42" s="67" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="43" spans="2:5" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B43" s="63"/>
+      <c r="B43" s="76"/>
       <c r="C43" s="32" t="s">
         <v>118</v>
       </c>
-      <c r="D43" s="63"/>
-      <c r="E43" s="61"/>
+      <c r="D43" s="76"/>
+      <c r="E43" s="67"/>
     </row>
     <row r="44" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B44" s="64">
+      <c r="B44" s="73">
         <v>59</v>
       </c>
       <c r="C44" s="33" t="s">
         <v>119</v>
       </c>
-      <c r="D44" s="64" t="s">
+      <c r="D44" s="73" t="s">
         <v>36</v>
       </c>
-      <c r="E44" s="61" t="s">
+      <c r="E44" s="67" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="45" spans="2:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B45" s="65"/>
+      <c r="B45" s="74"/>
       <c r="C45" s="30" t="s">
         <v>120</v>
       </c>
-      <c r="D45" s="65"/>
-      <c r="E45" s="61"/>
+      <c r="D45" s="74"/>
+      <c r="E45" s="67"/>
     </row>
     <row r="46" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B46" s="36">
@@ -3232,15 +3283,18 @@
         <v>266</v>
       </c>
     </row>
-    <row r="47" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B47" s="34">
+    <row r="47" spans="2:5" s="44" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B47" s="54">
         <v>61</v>
       </c>
-      <c r="C47" s="34" t="s">
+      <c r="C47" s="54" t="s">
         <v>123</v>
       </c>
-      <c r="D47" s="34" t="s">
+      <c r="D47" s="54" t="s">
         <v>124</v>
+      </c>
+      <c r="E47" s="55" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="48" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
@@ -3257,65 +3311,71 @@
         <v>265</v>
       </c>
     </row>
-    <row r="49" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B49" s="64">
+    <row r="49" spans="2:5" s="44" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="B49" s="71">
         <v>63</v>
       </c>
-      <c r="C49" s="33" t="s">
+      <c r="C49" s="52" t="s">
         <v>126</v>
       </c>
-      <c r="D49" s="64" t="s">
+      <c r="D49" s="71" t="s">
         <v>128</v>
       </c>
-      <c r="E49" s="61"/>
-    </row>
-    <row r="50" spans="2:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B50" s="65"/>
-      <c r="C50" s="30" t="s">
+      <c r="E49" s="87" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="50" spans="2:5" s="44" customFormat="1" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B50" s="72"/>
+      <c r="C50" s="53" t="s">
         <v>127</v>
       </c>
-      <c r="D50" s="65"/>
-      <c r="E50" s="61"/>
-    </row>
-    <row r="51" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B51" s="62">
+      <c r="D50" s="72"/>
+      <c r="E50" s="87"/>
+    </row>
+    <row r="51" spans="2:5" s="44" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="B51" s="71">
         <v>64</v>
       </c>
-      <c r="C51" s="31" t="s">
+      <c r="C51" s="52" t="s">
         <v>129</v>
       </c>
-      <c r="D51" s="62" t="s">
+      <c r="D51" s="71" t="s">
         <v>131</v>
       </c>
-      <c r="E51" s="61"/>
-    </row>
-    <row r="52" spans="2:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B52" s="63"/>
-      <c r="C52" s="32" t="s">
+      <c r="E51" s="87" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="52" spans="2:5" s="44" customFormat="1" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B52" s="72"/>
+      <c r="C52" s="53" t="s">
         <v>130</v>
       </c>
-      <c r="D52" s="63"/>
-      <c r="E52" s="61"/>
-    </row>
-    <row r="53" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B53" s="64">
+      <c r="D52" s="72"/>
+      <c r="E52" s="87"/>
+    </row>
+    <row r="53" spans="2:5" s="44" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="B53" s="71">
         <v>65</v>
       </c>
-      <c r="C53" s="33" t="s">
+      <c r="C53" s="52" t="s">
         <v>132</v>
       </c>
-      <c r="D53" s="64" t="s">
+      <c r="D53" s="71" t="s">
         <v>134</v>
       </c>
-      <c r="E53" s="61"/>
-    </row>
-    <row r="54" spans="2:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B54" s="65"/>
-      <c r="C54" s="30" t="s">
+      <c r="E53" s="87" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="54" spans="2:5" s="44" customFormat="1" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B54" s="72"/>
+      <c r="C54" s="53" t="s">
         <v>133</v>
       </c>
-      <c r="D54" s="65"/>
-      <c r="E54" s="61"/>
+      <c r="D54" s="72"/>
+      <c r="E54" s="87"/>
     </row>
     <row r="55" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B55" s="36">
@@ -3775,70 +3835,70 @@
       </c>
     </row>
     <row r="2" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B2" s="57">
+      <c r="B2" s="63">
         <v>92</v>
       </c>
       <c r="C2" s="15" t="s">
         <v>178</v>
       </c>
-      <c r="D2" s="57" t="s">
+      <c r="D2" s="63" t="s">
         <v>36</v>
       </c>
-      <c r="E2" s="61" t="s">
+      <c r="E2" s="67" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="3" spans="2:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="53"/>
+      <c r="B3" s="59"/>
       <c r="C3" s="7" t="s">
         <v>179</v>
       </c>
-      <c r="D3" s="53"/>
-      <c r="E3" s="61"/>
+      <c r="D3" s="59"/>
+      <c r="E3" s="67"/>
     </row>
     <row r="4" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B4" s="50">
+      <c r="B4" s="56">
         <v>93</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="50" t="s">
+      <c r="D4" s="56" t="s">
         <v>71</v>
       </c>
-      <c r="E4" s="61" t="s">
+      <c r="E4" s="67" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="5" spans="2:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="51"/>
+      <c r="B5" s="57"/>
       <c r="C5" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="D5" s="51"/>
-      <c r="E5" s="61"/>
+      <c r="D5" s="57"/>
+      <c r="E5" s="67"/>
     </row>
     <row r="6" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B6" s="52">
+      <c r="B6" s="58">
         <v>94</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="52" t="s">
+      <c r="D6" s="58" t="s">
         <v>182</v>
       </c>
-      <c r="E6" s="61" t="s">
+      <c r="E6" s="67" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="7" spans="2:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="53"/>
+      <c r="B7" s="59"/>
       <c r="C7" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="D7" s="53"/>
-      <c r="E7" s="61"/>
+      <c r="D7" s="59"/>
+      <c r="E7" s="67"/>
     </row>
     <row r="8" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="4">
@@ -3882,66 +3942,66 @@
         <v>266</v>
       </c>
     </row>
-    <row r="11" spans="2:6" s="49" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="46">
+    <row r="11" spans="2:6" s="48" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="45">
         <v>98</v>
       </c>
-      <c r="C11" s="46" t="s">
+      <c r="C11" s="45" t="s">
         <v>188</v>
       </c>
-      <c r="D11" s="46" t="s">
+      <c r="D11" s="45" t="s">
         <v>189</v>
       </c>
-      <c r="E11" s="47" t="s">
-        <v>266</v>
-      </c>
-      <c r="F11" s="48"/>
+      <c r="E11" s="46" t="s">
+        <v>266</v>
+      </c>
+      <c r="F11" s="47"/>
     </row>
     <row r="12" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B12" s="76">
+      <c r="B12" s="88">
         <v>99</v>
       </c>
-      <c r="C12" s="76" t="s">
+      <c r="C12" s="88" t="s">
         <v>190</v>
       </c>
       <c r="D12" s="27" t="s">
         <v>191</v>
       </c>
-      <c r="E12" s="61" t="s">
+      <c r="E12" s="67" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="13" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B13" s="56"/>
-      <c r="C13" s="56"/>
+      <c r="B13" s="62"/>
+      <c r="C13" s="62"/>
       <c r="D13" s="8" t="s">
         <v>192</v>
       </c>
-      <c r="E13" s="61"/>
+      <c r="E13" s="67"/>
     </row>
     <row r="14" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B14" s="56"/>
-      <c r="C14" s="56"/>
+      <c r="B14" s="62"/>
+      <c r="C14" s="62"/>
       <c r="D14" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="E14" s="61"/>
+      <c r="E14" s="67"/>
     </row>
     <row r="15" spans="2:6" ht="50.4" x14ac:dyDescent="0.3">
-      <c r="B15" s="56"/>
-      <c r="C15" s="56"/>
+      <c r="B15" s="62"/>
+      <c r="C15" s="62"/>
       <c r="D15" s="8" t="s">
         <v>194</v>
       </c>
-      <c r="E15" s="61"/>
+      <c r="E15" s="67"/>
     </row>
     <row r="16" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="51"/>
-      <c r="C16" s="51"/>
+      <c r="B16" s="57"/>
+      <c r="C16" s="57"/>
       <c r="D16" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="E16" s="61"/>
+      <c r="E16" s="67"/>
     </row>
     <row r="17" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="2">
@@ -3958,34 +4018,34 @@
       </c>
     </row>
     <row r="18" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B18" s="50">
+      <c r="B18" s="56">
         <v>101</v>
       </c>
-      <c r="C18" s="50" t="s">
+      <c r="C18" s="56" t="s">
         <v>198</v>
       </c>
       <c r="D18" s="8" t="s">
         <v>199</v>
       </c>
-      <c r="E18" s="61" t="s">
+      <c r="E18" s="67" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="19" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B19" s="56"/>
-      <c r="C19" s="56"/>
+      <c r="B19" s="62"/>
+      <c r="C19" s="62"/>
       <c r="D19" s="8" t="s">
         <v>200</v>
       </c>
-      <c r="E19" s="61"/>
+      <c r="E19" s="67"/>
     </row>
     <row r="20" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="51"/>
-      <c r="C20" s="51"/>
+      <c r="B20" s="57"/>
+      <c r="C20" s="57"/>
       <c r="D20" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="E20" s="61"/>
+      <c r="E20" s="67"/>
     </row>
   </sheetData>
   <mergeCells count="15">
@@ -4013,7 +4073,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B1:F31"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E20" sqref="E20:E21"/>
     </sheetView>
   </sheetViews>
@@ -4034,70 +4094,70 @@
       </c>
     </row>
     <row r="2" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B2" s="57">
+      <c r="B2" s="63">
         <v>102</v>
       </c>
       <c r="C2" s="15" t="s">
         <v>178</v>
       </c>
-      <c r="D2" s="57" t="s">
+      <c r="D2" s="63" t="s">
         <v>36</v>
       </c>
-      <c r="E2" s="61" t="s">
+      <c r="E2" s="67" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="3" spans="2:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="53"/>
+      <c r="B3" s="59"/>
       <c r="C3" s="7" t="s">
         <v>179</v>
       </c>
-      <c r="D3" s="53"/>
-      <c r="E3" s="61"/>
+      <c r="D3" s="59"/>
+      <c r="E3" s="67"/>
     </row>
     <row r="4" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B4" s="50">
+      <c r="B4" s="56">
         <v>103</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>202</v>
       </c>
-      <c r="D4" s="50" t="s">
+      <c r="D4" s="56" t="s">
         <v>71</v>
       </c>
-      <c r="E4" s="61" t="s">
+      <c r="E4" s="67" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="5" spans="2:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="51"/>
+      <c r="B5" s="57"/>
       <c r="C5" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="D5" s="51"/>
-      <c r="E5" s="61"/>
+      <c r="D5" s="57"/>
+      <c r="E5" s="67"/>
     </row>
     <row r="6" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B6" s="52">
+      <c r="B6" s="58">
         <v>104</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="52" t="s">
+      <c r="D6" s="58" t="s">
         <v>182</v>
       </c>
-      <c r="E6" s="61" t="s">
+      <c r="E6" s="67" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="7" spans="2:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="53"/>
+      <c r="B7" s="59"/>
       <c r="C7" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="D7" s="53"/>
-      <c r="E7" s="61"/>
+      <c r="D7" s="59"/>
+      <c r="E7" s="67"/>
     </row>
     <row r="8" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="4">
@@ -4155,45 +4215,45 @@
         <v>271</v>
       </c>
     </row>
-    <row r="12" spans="2:6" s="49" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="46">
+    <row r="12" spans="2:6" s="48" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="45">
         <v>109</v>
       </c>
-      <c r="C12" s="46" t="s">
+      <c r="C12" s="45" t="s">
         <v>210</v>
       </c>
-      <c r="D12" s="46" t="s">
+      <c r="D12" s="45" t="s">
         <v>211</v>
       </c>
-      <c r="E12" s="47" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" s="49" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="46">
+      <c r="E12" s="46" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" s="48" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="45">
         <v>110</v>
       </c>
-      <c r="C13" s="46" t="s">
+      <c r="C13" s="45" t="s">
         <v>212</v>
       </c>
-      <c r="D13" s="46" t="s">
+      <c r="D13" s="45" t="s">
         <v>213</v>
       </c>
-      <c r="E13" s="47" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" s="49" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="46">
+      <c r="E13" s="46" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" s="48" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="45">
         <v>111</v>
       </c>
-      <c r="C14" s="46" t="s">
+      <c r="C14" s="45" t="s">
         <v>214</v>
       </c>
-      <c r="D14" s="46">
+      <c r="D14" s="45">
         <v>0</v>
       </c>
-      <c r="E14" s="47" t="s">
+      <c r="E14" s="46" t="s">
         <v>266</v>
       </c>
     </row>
@@ -4225,17 +4285,17 @@
         <v>266</v>
       </c>
     </row>
-    <row r="17" spans="2:5" s="49" customFormat="1" ht="34.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="46">
+    <row r="17" spans="2:5" s="48" customFormat="1" ht="34.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="45">
         <v>114</v>
       </c>
-      <c r="C17" s="46" t="s">
+      <c r="C17" s="45" t="s">
         <v>217</v>
       </c>
-      <c r="D17" s="46" t="s">
+      <c r="D17" s="45" t="s">
         <v>218</v>
       </c>
-      <c r="E17" s="47" t="s">
+      <c r="E17" s="46" t="s">
         <v>266</v>
       </c>
     </row>
@@ -4253,39 +4313,39 @@
         <v>266</v>
       </c>
     </row>
-    <row r="19" spans="2:5" s="49" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="46">
+    <row r="19" spans="2:5" s="48" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B19" s="45">
         <v>116</v>
       </c>
-      <c r="C19" s="46" t="s">
+      <c r="C19" s="45" t="s">
         <v>221</v>
       </c>
-      <c r="D19" s="46" t="s">
+      <c r="D19" s="45" t="s">
         <v>222</v>
       </c>
-      <c r="E19" s="47" t="s">
+      <c r="E19" s="46" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="20" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B20" s="50">
+      <c r="B20" s="56">
         <v>117</v>
       </c>
       <c r="C20" s="8" t="s">
         <v>223</v>
       </c>
-      <c r="D20" s="50" t="s">
+      <c r="D20" s="56" t="s">
         <v>56</v>
       </c>
-      <c r="E20" s="61"/>
+      <c r="E20" s="67"/>
     </row>
     <row r="21" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="51"/>
+      <c r="B21" s="57"/>
       <c r="C21" s="4" t="s">
         <v>224</v>
       </c>
-      <c r="D21" s="51"/>
-      <c r="E21" s="61"/>
+      <c r="D21" s="57"/>
+      <c r="E21" s="67"/>
     </row>
     <row r="22" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B22" s="2">
@@ -4397,13 +4457,13 @@
       </c>
     </row>
     <row r="30" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B30" s="52">
+      <c r="B30" s="58">
         <v>126</v>
       </c>
       <c r="C30" s="6" t="s">
         <v>267</v>
       </c>
-      <c r="D30" s="52" t="s">
+      <c r="D30" s="58" t="s">
         <v>241</v>
       </c>
       <c r="E30" s="39" t="s">
@@ -4411,9 +4471,9 @@
       </c>
     </row>
     <row r="31" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B31" s="53"/>
+      <c r="B31" s="59"/>
       <c r="C31" s="2"/>
-      <c r="D31" s="53"/>
+      <c r="D31" s="59"/>
     </row>
   </sheetData>
   <mergeCells count="14">

</xml_diff>

<commit_message>
Prereq Init & Server SSL
</commit_message>
<xml_diff>
--- a/Checklist.xlsx
+++ b/Checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Prashant\AziraPowershellscript\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B9C8DEC-CF7F-48FE-B2D3-AECD50E786E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9433CB5C-0B1E-48A8-BEAA-516010EE31C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="272">
   <si>
     <t xml:space="preserve"> Last Updated</t>
   </si>
@@ -1341,7 +1341,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1492,33 +1492,31 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1531,9 +1529,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1543,70 +1538,81 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="4" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="4" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="4" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="4" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Accent1" xfId="1" builtinId="29"/>
@@ -2019,7 +2025,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D8" sqref="D8:D9"/>
+      <selection pane="bottomLeft" activeCell="A39" sqref="A39:XFD39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2049,11 +2055,11 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="60" t="s">
+      <c r="B2" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="61"/>
-      <c r="D2" s="61"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
     </row>
     <row r="3" spans="1:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="12">
@@ -2100,7 +2106,7 @@
       <c r="D6" s="63" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="67" t="s">
+      <c r="E6" s="55" t="s">
         <v>266</v>
       </c>
     </row>
@@ -2109,30 +2115,30 @@
       <c r="C7" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="59"/>
-      <c r="E7" s="67"/>
+      <c r="D7" s="61"/>
+      <c r="E7" s="55"/>
     </row>
     <row r="8" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="92"/>
+      <c r="A8" s="54"/>
       <c r="B8" s="11">
         <v>4</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="56" t="s">
+      <c r="D8" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="67"/>
+      <c r="E8" s="55"/>
     </row>
     <row r="9" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="92"/>
+      <c r="A9" s="54"/>
       <c r="B9" s="1"/>
       <c r="C9" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="57"/>
-      <c r="E9" s="67"/>
+      <c r="D9" s="62"/>
+      <c r="E9" s="55"/>
     </row>
     <row r="10" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B10" s="13">
@@ -2144,7 +2150,7 @@
       <c r="D10" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="67" t="s">
+      <c r="E10" s="55" t="s">
         <v>266</v>
       </c>
     </row>
@@ -2154,7 +2160,7 @@
         <v>261</v>
       </c>
       <c r="D11" s="64"/>
-      <c r="E11" s="67"/>
+      <c r="E11" s="55"/>
     </row>
     <row r="12" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B12" s="11">
@@ -2163,10 +2169,10 @@
       <c r="C12" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="56" t="s">
+      <c r="D12" s="58" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="67" t="s">
+      <c r="E12" s="55" t="s">
         <v>266</v>
       </c>
     </row>
@@ -2175,8 +2181,8 @@
       <c r="C13" s="17" t="s">
         <v>261</v>
       </c>
-      <c r="D13" s="62"/>
-      <c r="E13" s="67"/>
+      <c r="D13" s="59"/>
+      <c r="E13" s="55"/>
     </row>
     <row r="14" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B14" s="11">
@@ -2185,10 +2191,10 @@
       <c r="C14" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="58" t="s">
+      <c r="D14" s="60" t="s">
         <v>14</v>
       </c>
-      <c r="E14" s="67" t="s">
+      <c r="E14" s="55" t="s">
         <v>266</v>
       </c>
     </row>
@@ -2197,8 +2203,8 @@
       <c r="C15" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="59"/>
-      <c r="E15" s="67"/>
+      <c r="D15" s="61"/>
+      <c r="E15" s="55"/>
     </row>
     <row r="16" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B16" s="11">
@@ -2207,10 +2213,10 @@
       <c r="C16" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="56" t="s">
+      <c r="D16" s="58" t="s">
         <v>17</v>
       </c>
-      <c r="E16" s="67" t="s">
+      <c r="E16" s="55" t="s">
         <v>266</v>
       </c>
     </row>
@@ -2219,8 +2225,8 @@
       <c r="C17" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="57"/>
-      <c r="E17" s="67"/>
+      <c r="D17" s="62"/>
+      <c r="E17" s="55"/>
     </row>
     <row r="18" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B18" s="11">
@@ -2229,10 +2235,10 @@
       <c r="C18" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D18" s="58">
+      <c r="D18" s="60">
         <v>4</v>
       </c>
-      <c r="E18" s="67" t="s">
+      <c r="E18" s="55" t="s">
         <v>266</v>
       </c>
     </row>
@@ -2241,8 +2247,8 @@
       <c r="C19" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D19" s="59"/>
-      <c r="E19" s="67"/>
+      <c r="D19" s="61"/>
+      <c r="E19" s="55"/>
     </row>
     <row r="20" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B20" s="1">
@@ -2254,7 +2260,7 @@
       <c r="D20" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E20" s="67" t="s">
+      <c r="E20" s="55" t="s">
         <v>266</v>
       </c>
     </row>
@@ -2265,7 +2271,7 @@
       <c r="D21" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E21" s="67"/>
+      <c r="E21" s="55"/>
     </row>
     <row r="22" spans="2:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="11">
@@ -2274,10 +2280,10 @@
       <c r="C22" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D22" s="56" t="s">
+      <c r="D22" s="58" t="s">
         <v>25</v>
       </c>
-      <c r="E22" s="67" t="s">
+      <c r="E22" s="55" t="s">
         <v>266</v>
       </c>
     </row>
@@ -2286,8 +2292,8 @@
       <c r="C23" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="D23" s="57"/>
-      <c r="E23" s="67"/>
+      <c r="D23" s="62"/>
+      <c r="E23" s="55"/>
     </row>
     <row r="24" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B24" s="11">
@@ -2296,10 +2302,10 @@
       <c r="C24" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D24" s="58" t="s">
+      <c r="D24" s="60" t="s">
         <v>28</v>
       </c>
-      <c r="E24" s="67" t="s">
+      <c r="E24" s="55" t="s">
         <v>266</v>
       </c>
     </row>
@@ -2308,8 +2314,8 @@
       <c r="C25" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="D25" s="59"/>
-      <c r="E25" s="67"/>
+      <c r="D25" s="61"/>
+      <c r="E25" s="55"/>
     </row>
     <row r="26" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B26" s="11">
@@ -2318,10 +2324,10 @@
       <c r="C26" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="D26" s="56" t="s">
+      <c r="D26" s="58" t="s">
         <v>31</v>
       </c>
-      <c r="E26" s="67" t="s">
+      <c r="E26" s="55" t="s">
         <v>266</v>
       </c>
     </row>
@@ -2330,8 +2336,8 @@
       <c r="C27" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D27" s="57"/>
-      <c r="E27" s="67"/>
+      <c r="D27" s="62"/>
+      <c r="E27" s="55"/>
     </row>
     <row r="28" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="11">
@@ -2340,18 +2346,18 @@
       <c r="C28" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="D28" s="58" t="s">
+      <c r="D28" s="60" t="s">
         <v>34</v>
       </c>
-      <c r="E28" s="67"/>
+      <c r="E28" s="55"/>
     </row>
     <row r="29" spans="2:5" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B29" s="1"/>
       <c r="C29" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D29" s="59"/>
-      <c r="E29" s="67"/>
+      <c r="D29" s="61"/>
+      <c r="E29" s="55"/>
     </row>
     <row r="30" spans="2:5" ht="32.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B30" s="20">
@@ -2364,17 +2370,17 @@
         <v>36</v>
       </c>
     </row>
-    <row r="31" spans="2:5" s="44" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B31" s="89">
+    <row r="31" spans="2:5" s="48" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B31" s="93">
         <v>16</v>
       </c>
-      <c r="C31" s="90" t="s">
+      <c r="C31" s="94" t="s">
         <v>37</v>
       </c>
-      <c r="D31" s="91" t="s">
+      <c r="D31" s="45" t="s">
         <v>38</v>
       </c>
-      <c r="E31" s="55" t="s">
+      <c r="E31" s="46" t="s">
         <v>265</v>
       </c>
     </row>
@@ -2389,17 +2395,17 @@
         <v>38</v>
       </c>
     </row>
-    <row r="33" spans="2:5" s="44" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B33" s="89">
+    <row r="33" spans="2:5" s="48" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B33" s="93">
         <v>18</v>
       </c>
-      <c r="C33" s="90" t="s">
+      <c r="C33" s="94" t="s">
         <v>40</v>
       </c>
-      <c r="D33" s="91" t="s">
+      <c r="D33" s="45" t="s">
         <v>38</v>
       </c>
-      <c r="E33" s="55" t="s">
+      <c r="E33" s="46" t="s">
         <v>265</v>
       </c>
     </row>
@@ -2414,17 +2420,17 @@
         <v>38</v>
       </c>
     </row>
-    <row r="35" spans="2:5" s="44" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B35" s="89">
+    <row r="35" spans="2:5" s="48" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B35" s="93">
         <v>20</v>
       </c>
-      <c r="C35" s="90" t="s">
+      <c r="C35" s="94" t="s">
         <v>42</v>
       </c>
-      <c r="D35" s="91" t="s">
+      <c r="D35" s="45" t="s">
         <v>36</v>
       </c>
-      <c r="E35" s="55" t="s">
+      <c r="E35" s="46" t="s">
         <v>265</v>
       </c>
     </row>
@@ -2439,17 +2445,17 @@
         <v>38</v>
       </c>
     </row>
-    <row r="37" spans="2:5" s="44" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B37" s="89">
+    <row r="37" spans="2:5" s="48" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B37" s="93">
         <v>22</v>
       </c>
-      <c r="C37" s="90" t="s">
+      <c r="C37" s="94" t="s">
         <v>44</v>
       </c>
-      <c r="D37" s="91" t="s">
+      <c r="D37" s="45" t="s">
         <v>38</v>
       </c>
-      <c r="E37" s="55" t="s">
+      <c r="E37" s="46" t="s">
         <v>265</v>
       </c>
     </row>
@@ -2464,17 +2470,17 @@
         <v>38</v>
       </c>
     </row>
-    <row r="39" spans="2:5" s="44" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B39" s="89">
+    <row r="39" spans="2:5" s="48" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B39" s="93">
         <v>24</v>
       </c>
-      <c r="C39" s="90" t="s">
+      <c r="C39" s="94" t="s">
         <v>46</v>
       </c>
-      <c r="D39" s="91" t="s">
+      <c r="D39" s="45" t="s">
         <v>36</v>
       </c>
-      <c r="E39" s="55" t="s">
+      <c r="E39" s="46" t="s">
         <v>265</v>
       </c>
     </row>
@@ -2497,6 +2503,19 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="D6:D7"/>
     <mergeCell ref="E26:E27"/>
     <mergeCell ref="E28:E29"/>
     <mergeCell ref="E12:E13"/>
@@ -2509,19 +2528,6 @@
     <mergeCell ref="E24:E25"/>
     <mergeCell ref="E16:E17"/>
     <mergeCell ref="E14:E15"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="D18:D19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2663,89 +2669,89 @@
       <c r="B9" s="49">
         <v>33</v>
       </c>
-      <c r="C9" s="68" t="s">
+      <c r="C9" s="67" t="s">
         <v>61</v>
       </c>
       <c r="D9" s="50" t="s">
         <v>62</v>
       </c>
-      <c r="E9" s="70" t="s">
+      <c r="E9" s="69" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="10" spans="2:6" s="48" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="51"/>
-      <c r="C10" s="69"/>
+      <c r="C10" s="68"/>
       <c r="D10" s="45" t="s">
         <v>63</v>
       </c>
-      <c r="E10" s="70"/>
+      <c r="E10" s="69"/>
     </row>
     <row r="11" spans="2:6" s="48" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B11" s="49">
         <v>34</v>
       </c>
-      <c r="C11" s="68" t="s">
+      <c r="C11" s="67" t="s">
         <v>64</v>
       </c>
       <c r="D11" s="50" t="s">
         <v>65</v>
       </c>
-      <c r="E11" s="70" t="s">
+      <c r="E11" s="69" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="12" spans="2:6" s="48" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="51"/>
-      <c r="C12" s="69"/>
+      <c r="C12" s="68"/>
       <c r="D12" s="45" t="s">
         <v>63</v>
       </c>
-      <c r="E12" s="70"/>
+      <c r="E12" s="69"/>
     </row>
     <row r="13" spans="2:6" s="48" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B13" s="49">
         <v>35</v>
       </c>
-      <c r="C13" s="68" t="s">
+      <c r="C13" s="67" t="s">
         <v>66</v>
       </c>
       <c r="D13" s="50" t="s">
         <v>62</v>
       </c>
-      <c r="E13" s="70" t="s">
+      <c r="E13" s="69" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="14" spans="2:6" s="48" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="51"/>
-      <c r="C14" s="69"/>
+      <c r="C14" s="68"/>
       <c r="D14" s="45" t="s">
         <v>67</v>
       </c>
-      <c r="E14" s="70"/>
+      <c r="E14" s="69"/>
     </row>
     <row r="15" spans="2:6" s="48" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B15" s="49">
         <v>36</v>
       </c>
-      <c r="C15" s="68" t="s">
+      <c r="C15" s="67" t="s">
         <v>68</v>
       </c>
       <c r="D15" s="50" t="s">
         <v>65</v>
       </c>
-      <c r="E15" s="70" t="s">
+      <c r="E15" s="69" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="16" spans="2:6" s="48" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="51"/>
-      <c r="C16" s="69"/>
+      <c r="C16" s="68"/>
       <c r="D16" s="45" t="s">
         <v>67</v>
       </c>
-      <c r="E16" s="70"/>
+      <c r="E16" s="69"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -2767,8 +2773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B2:F80"/>
   <sheetViews>
-    <sheetView topLeftCell="B40" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D53" sqref="D53:D54"/>
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C49" sqref="A49:XFD54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2799,304 +2805,304 @@
       <c r="D3" s="63" t="s">
         <v>71</v>
       </c>
-      <c r="E3" s="67" t="s">
+      <c r="E3" s="55" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="4" spans="2:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="59"/>
+      <c r="B4" s="61"/>
       <c r="C4" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="D4" s="59"/>
-      <c r="E4" s="67"/>
+      <c r="D4" s="61"/>
+      <c r="E4" s="55"/>
     </row>
     <row r="5" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B5" s="56">
+      <c r="B5" s="58">
         <v>38</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="56" t="s">
+      <c r="D5" s="58" t="s">
         <v>73</v>
       </c>
-      <c r="E5" s="67" t="s">
+      <c r="E5" s="55" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="6" spans="2:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="57"/>
+      <c r="B6" s="62"/>
       <c r="C6" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="D6" s="57"/>
-      <c r="E6" s="67"/>
+      <c r="D6" s="62"/>
+      <c r="E6" s="55"/>
     </row>
     <row r="7" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B7" s="58">
+      <c r="B7" s="60">
         <v>39</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="58" t="s">
+      <c r="D7" s="60" t="s">
         <v>31</v>
       </c>
-      <c r="E7" s="67" t="s">
+      <c r="E7" s="55" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="8" spans="2:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="59"/>
+      <c r="B8" s="61"/>
       <c r="C8" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="D8" s="59"/>
-      <c r="E8" s="67"/>
+      <c r="D8" s="61"/>
+      <c r="E8" s="55"/>
     </row>
     <row r="9" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B9" s="56">
+      <c r="B9" s="58">
         <v>40</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="D9" s="56" t="s">
+      <c r="D9" s="58" t="s">
         <v>77</v>
       </c>
-      <c r="E9" s="67" t="s">
+      <c r="E9" s="55" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="10" spans="2:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="57"/>
+      <c r="B10" s="62"/>
       <c r="C10" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="D10" s="57"/>
-      <c r="E10" s="67"/>
+      <c r="D10" s="62"/>
+      <c r="E10" s="55"/>
     </row>
     <row r="11" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B11" s="58">
+      <c r="B11" s="60">
         <v>41</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="D11" s="58" t="s">
+      <c r="D11" s="60" t="s">
         <v>80</v>
       </c>
-      <c r="E11" s="67" t="s">
+      <c r="E11" s="55" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="12" spans="2:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="59"/>
+      <c r="B12" s="61"/>
       <c r="C12" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="D12" s="59"/>
-      <c r="E12" s="67"/>
+      <c r="D12" s="61"/>
+      <c r="E12" s="55"/>
     </row>
     <row r="13" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B13" s="56">
+      <c r="B13" s="58">
         <v>42</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="D13" s="56" t="s">
+      <c r="D13" s="58" t="s">
         <v>83</v>
       </c>
-      <c r="E13" s="67" t="s">
+      <c r="E13" s="55" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="14" spans="2:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="57"/>
+      <c r="B14" s="62"/>
       <c r="C14" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="D14" s="57"/>
-      <c r="E14" s="67"/>
+      <c r="D14" s="62"/>
+      <c r="E14" s="55"/>
     </row>
     <row r="15" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B15" s="83">
+      <c r="B15" s="78">
         <v>43</v>
       </c>
       <c r="C15" s="29" t="s">
         <v>84</v>
       </c>
-      <c r="D15" s="83" t="s">
+      <c r="D15" s="78" t="s">
         <v>86</v>
       </c>
-      <c r="E15" s="67" t="s">
+      <c r="E15" s="55" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="16" spans="2:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="74"/>
+      <c r="B16" s="73"/>
       <c r="C16" s="30" t="s">
         <v>85</v>
       </c>
-      <c r="D16" s="74"/>
-      <c r="E16" s="67"/>
+      <c r="D16" s="73"/>
+      <c r="E16" s="55"/>
     </row>
     <row r="17" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B17" s="75">
+      <c r="B17" s="74">
         <v>44</v>
       </c>
       <c r="C17" s="31" t="s">
         <v>87</v>
       </c>
-      <c r="D17" s="84">
+      <c r="D17" s="79">
         <v>987654321</v>
       </c>
-      <c r="E17" s="67"/>
+      <c r="E17" s="55"/>
     </row>
     <row r="18" spans="2:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="76"/>
+      <c r="B18" s="75"/>
       <c r="C18" s="32" t="s">
         <v>88</v>
       </c>
-      <c r="D18" s="85"/>
-      <c r="E18" s="67"/>
+      <c r="D18" s="80"/>
+      <c r="E18" s="55"/>
     </row>
     <row r="19" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B19" s="73">
+      <c r="B19" s="72">
         <v>45</v>
       </c>
       <c r="C19" s="33" t="s">
         <v>89</v>
       </c>
-      <c r="D19" s="73">
+      <c r="D19" s="72">
         <v>1433</v>
       </c>
-      <c r="E19" s="67" t="s">
+      <c r="E19" s="55" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="20" spans="2:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="74"/>
+      <c r="B20" s="73"/>
       <c r="C20" s="30" t="s">
         <v>90</v>
       </c>
-      <c r="D20" s="74"/>
-      <c r="E20" s="67"/>
+      <c r="D20" s="73"/>
+      <c r="E20" s="55"/>
     </row>
     <row r="21" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B21" s="75">
+      <c r="B21" s="74">
         <v>46</v>
       </c>
       <c r="C21" s="31" t="s">
         <v>91</v>
       </c>
-      <c r="D21" s="80">
+      <c r="D21" s="76">
         <v>43925</v>
       </c>
-      <c r="E21" s="86" t="s">
+      <c r="E21" s="71" t="s">
         <v>269</v>
       </c>
     </row>
     <row r="22" spans="2:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="76"/>
+      <c r="B22" s="75"/>
       <c r="C22" s="32" t="s">
         <v>92</v>
       </c>
-      <c r="D22" s="82"/>
-      <c r="E22" s="67"/>
+      <c r="D22" s="77"/>
+      <c r="E22" s="55"/>
     </row>
     <row r="23" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B23" s="73">
+      <c r="B23" s="72">
         <v>47</v>
       </c>
       <c r="C23" s="33" t="s">
         <v>93</v>
       </c>
-      <c r="D23" s="78" t="s">
+      <c r="D23" s="81" t="s">
         <v>7</v>
       </c>
-      <c r="E23" s="86" t="s">
+      <c r="E23" s="71" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="24" spans="2:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="74"/>
+      <c r="B24" s="73"/>
       <c r="C24" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="D24" s="79"/>
-      <c r="E24" s="67"/>
+      <c r="D24" s="82"/>
+      <c r="E24" s="55"/>
     </row>
     <row r="25" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B25" s="75">
+      <c r="B25" s="74">
         <v>48</v>
       </c>
       <c r="C25" s="31" t="s">
         <v>94</v>
       </c>
-      <c r="D25" s="80">
+      <c r="D25" s="76">
         <v>43834</v>
       </c>
-      <c r="E25" s="86" t="s">
+      <c r="E25" s="71" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="26" spans="2:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B26" s="76"/>
+      <c r="B26" s="75"/>
       <c r="C26" s="32" t="s">
         <v>95</v>
       </c>
-      <c r="D26" s="81"/>
-      <c r="E26" s="67"/>
+      <c r="D26" s="83"/>
+      <c r="E26" s="55"/>
     </row>
     <row r="27" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B27" s="73">
+      <c r="B27" s="72">
         <v>49</v>
       </c>
       <c r="C27" s="33" t="s">
         <v>96</v>
       </c>
-      <c r="D27" s="73">
+      <c r="D27" s="72">
         <v>0</v>
       </c>
-      <c r="E27" s="86" t="s">
+      <c r="E27" s="71" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="28" spans="2:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="74"/>
+      <c r="B28" s="73"/>
       <c r="C28" s="30" t="s">
         <v>96</v>
       </c>
-      <c r="D28" s="74"/>
-      <c r="E28" s="67"/>
+      <c r="D28" s="73"/>
+      <c r="E28" s="55"/>
     </row>
     <row r="29" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B29" s="75">
+      <c r="B29" s="74">
         <v>50</v>
       </c>
       <c r="C29" s="31" t="s">
         <v>97</v>
       </c>
-      <c r="D29" s="75">
+      <c r="D29" s="74">
         <v>5</v>
       </c>
-      <c r="E29" s="86" t="s">
+      <c r="E29" s="71" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="30" spans="2:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B30" s="76"/>
+      <c r="B30" s="75"/>
       <c r="C30" s="32" t="s">
         <v>98</v>
       </c>
-      <c r="D30" s="76"/>
-      <c r="E30" s="67"/>
+      <c r="D30" s="75"/>
+      <c r="E30" s="55"/>
     </row>
     <row r="31" spans="2:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="73">
+      <c r="B31" s="72">
         <v>51</v>
       </c>
       <c r="C31" s="33" t="s">
@@ -3105,83 +3111,85 @@
       <c r="D31" s="33" t="s">
         <v>101</v>
       </c>
-      <c r="E31" s="67" t="s">
+      <c r="E31" s="55" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="32" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B32" s="74"/>
+      <c r="B32" s="73"/>
       <c r="C32" s="30" t="s">
         <v>100</v>
       </c>
       <c r="D32" s="34" t="s">
         <v>102</v>
       </c>
-      <c r="E32" s="67"/>
-    </row>
-    <row r="33" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B33" s="75">
+      <c r="E32" s="55"/>
+    </row>
+    <row r="33" spans="2:5" s="44" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="B33" s="85">
         <v>52</v>
       </c>
-      <c r="C33" s="31" t="s">
+      <c r="C33" s="52" t="s">
         <v>103</v>
       </c>
-      <c r="D33" s="75" t="s">
+      <c r="D33" s="85" t="s">
         <v>105</v>
       </c>
-      <c r="E33" s="67"/>
-    </row>
-    <row r="34" spans="2:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B34" s="76"/>
-      <c r="C34" s="32" t="s">
+      <c r="E33" s="70" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" s="44" customFormat="1" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B34" s="86"/>
+      <c r="C34" s="53" t="s">
         <v>104</v>
       </c>
-      <c r="D34" s="76"/>
-      <c r="E34" s="67"/>
+      <c r="D34" s="86"/>
+      <c r="E34" s="70"/>
     </row>
     <row r="35" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B35" s="73">
+      <c r="B35" s="72">
         <v>53</v>
       </c>
       <c r="C35" s="33" t="s">
         <v>106</v>
       </c>
-      <c r="D35" s="73" t="s">
+      <c r="D35" s="72" t="s">
         <v>108</v>
       </c>
-      <c r="E35" s="67" t="s">
+      <c r="E35" s="55" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="36" spans="2:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B36" s="74"/>
+      <c r="B36" s="73"/>
       <c r="C36" s="30" t="s">
         <v>107</v>
       </c>
-      <c r="D36" s="74"/>
-      <c r="E36" s="67"/>
+      <c r="D36" s="73"/>
+      <c r="E36" s="55"/>
     </row>
     <row r="37" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B37" s="75">
+      <c r="B37" s="74">
         <v>54</v>
       </c>
       <c r="C37" s="31" t="s">
         <v>109</v>
       </c>
-      <c r="D37" s="75" t="s">
+      <c r="D37" s="74" t="s">
         <v>111</v>
       </c>
-      <c r="E37" s="67" t="s">
+      <c r="E37" s="55" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="38" spans="2:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B38" s="76"/>
+      <c r="B38" s="75"/>
       <c r="C38" s="32" t="s">
         <v>110</v>
       </c>
-      <c r="D38" s="76"/>
-      <c r="E38" s="67"/>
+      <c r="D38" s="75"/>
+      <c r="E38" s="55"/>
     </row>
     <row r="39" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B39" s="34">
@@ -3226,48 +3234,48 @@
       </c>
     </row>
     <row r="42" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="77">
+      <c r="B42" s="84">
         <v>58</v>
       </c>
       <c r="C42" s="37" t="s">
         <v>117</v>
       </c>
-      <c r="D42" s="77" t="s">
+      <c r="D42" s="84" t="s">
         <v>36</v>
       </c>
-      <c r="E42" s="67" t="s">
+      <c r="E42" s="55" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="43" spans="2:5" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B43" s="76"/>
+      <c r="B43" s="75"/>
       <c r="C43" s="32" t="s">
         <v>118</v>
       </c>
-      <c r="D43" s="76"/>
-      <c r="E43" s="67"/>
+      <c r="D43" s="75"/>
+      <c r="E43" s="55"/>
     </row>
     <row r="44" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B44" s="73">
+      <c r="B44" s="72">
         <v>59</v>
       </c>
       <c r="C44" s="33" t="s">
         <v>119</v>
       </c>
-      <c r="D44" s="73" t="s">
+      <c r="D44" s="72" t="s">
         <v>36</v>
       </c>
-      <c r="E44" s="67" t="s">
+      <c r="E44" s="55" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="45" spans="2:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B45" s="74"/>
+      <c r="B45" s="73"/>
       <c r="C45" s="30" t="s">
         <v>120</v>
       </c>
-      <c r="D45" s="74"/>
-      <c r="E45" s="67"/>
+      <c r="D45" s="73"/>
+      <c r="E45" s="55"/>
     </row>
     <row r="46" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B46" s="36">
@@ -3283,17 +3291,17 @@
         <v>266</v>
       </c>
     </row>
-    <row r="47" spans="2:5" s="44" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B47" s="54">
+    <row r="47" spans="2:5" s="48" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B47" s="88">
         <v>61</v>
       </c>
-      <c r="C47" s="54" t="s">
+      <c r="C47" s="88" t="s">
         <v>123</v>
       </c>
-      <c r="D47" s="54" t="s">
+      <c r="D47" s="88" t="s">
         <v>124</v>
       </c>
-      <c r="E47" s="55" t="s">
+      <c r="E47" s="46" t="s">
         <v>266</v>
       </c>
     </row>
@@ -3311,71 +3319,71 @@
         <v>265</v>
       </c>
     </row>
-    <row r="49" spans="2:5" s="44" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B49" s="71">
+    <row r="49" spans="2:5" s="48" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="B49" s="89">
         <v>63</v>
       </c>
-      <c r="C49" s="52" t="s">
+      <c r="C49" s="90" t="s">
         <v>126</v>
       </c>
-      <c r="D49" s="71" t="s">
+      <c r="D49" s="89" t="s">
         <v>128</v>
       </c>
-      <c r="E49" s="87" t="s">
+      <c r="E49" s="69" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="50" spans="2:5" s="44" customFormat="1" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B50" s="72"/>
-      <c r="C50" s="53" t="s">
+    <row r="50" spans="2:5" s="48" customFormat="1" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B50" s="91"/>
+      <c r="C50" s="92" t="s">
         <v>127</v>
       </c>
-      <c r="D50" s="72"/>
-      <c r="E50" s="87"/>
-    </row>
-    <row r="51" spans="2:5" s="44" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B51" s="71">
+      <c r="D50" s="91"/>
+      <c r="E50" s="69"/>
+    </row>
+    <row r="51" spans="2:5" s="48" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="B51" s="89">
         <v>64</v>
       </c>
-      <c r="C51" s="52" t="s">
+      <c r="C51" s="90" t="s">
         <v>129</v>
       </c>
-      <c r="D51" s="71" t="s">
+      <c r="D51" s="89" t="s">
         <v>131</v>
       </c>
-      <c r="E51" s="87" t="s">
+      <c r="E51" s="69" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="52" spans="2:5" s="44" customFormat="1" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B52" s="72"/>
-      <c r="C52" s="53" t="s">
+    <row r="52" spans="2:5" s="48" customFormat="1" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B52" s="91"/>
+      <c r="C52" s="92" t="s">
         <v>130</v>
       </c>
-      <c r="D52" s="72"/>
-      <c r="E52" s="87"/>
-    </row>
-    <row r="53" spans="2:5" s="44" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B53" s="71">
+      <c r="D52" s="91"/>
+      <c r="E52" s="69"/>
+    </row>
+    <row r="53" spans="2:5" s="48" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="B53" s="89">
         <v>65</v>
       </c>
-      <c r="C53" s="52" t="s">
+      <c r="C53" s="90" t="s">
         <v>132</v>
       </c>
-      <c r="D53" s="71" t="s">
+      <c r="D53" s="89" t="s">
         <v>134</v>
       </c>
-      <c r="E53" s="87" t="s">
+      <c r="E53" s="69" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="54" spans="2:5" s="44" customFormat="1" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B54" s="72"/>
-      <c r="C54" s="53" t="s">
+    <row r="54" spans="2:5" s="48" customFormat="1" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B54" s="91"/>
+      <c r="C54" s="92" t="s">
         <v>133</v>
       </c>
-      <c r="D54" s="72"/>
-      <c r="E54" s="87"/>
+      <c r="D54" s="91"/>
+      <c r="E54" s="69"/>
     </row>
     <row r="55" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B55" s="36">
@@ -3737,6 +3745,58 @@
     </row>
   </sheetData>
   <mergeCells count="68">
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="D51:D52"/>
+    <mergeCell ref="B53:B54"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="D49:D50"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E33:E34"/>
+    <mergeCell ref="E35:E36"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="E31:E32"/>
     <mergeCell ref="E49:E50"/>
     <mergeCell ref="E51:E52"/>
     <mergeCell ref="E53:E54"/>
@@ -3753,58 +3813,6 @@
     <mergeCell ref="E13:E14"/>
     <mergeCell ref="E15:E16"/>
     <mergeCell ref="E21:E22"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="E33:E34"/>
-    <mergeCell ref="E35:E36"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="D42:D43"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="D51:D52"/>
-    <mergeCell ref="B53:B54"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="D44:D45"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="D49:D50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3844,61 +3852,61 @@
       <c r="D2" s="63" t="s">
         <v>36</v>
       </c>
-      <c r="E2" s="67" t="s">
+      <c r="E2" s="55" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="3" spans="2:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="59"/>
+      <c r="B3" s="61"/>
       <c r="C3" s="7" t="s">
         <v>179</v>
       </c>
-      <c r="D3" s="59"/>
-      <c r="E3" s="67"/>
+      <c r="D3" s="61"/>
+      <c r="E3" s="55"/>
     </row>
     <row r="4" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B4" s="56">
+      <c r="B4" s="58">
         <v>93</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="56" t="s">
+      <c r="D4" s="58" t="s">
         <v>71</v>
       </c>
-      <c r="E4" s="67" t="s">
+      <c r="E4" s="55" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="5" spans="2:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="57"/>
+      <c r="B5" s="62"/>
       <c r="C5" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="D5" s="57"/>
-      <c r="E5" s="67"/>
+      <c r="D5" s="62"/>
+      <c r="E5" s="55"/>
     </row>
     <row r="6" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B6" s="58">
+      <c r="B6" s="60">
         <v>94</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="58" t="s">
+      <c r="D6" s="60" t="s">
         <v>182</v>
       </c>
-      <c r="E6" s="67" t="s">
+      <c r="E6" s="55" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="7" spans="2:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="59"/>
+      <c r="B7" s="61"/>
       <c r="C7" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="D7" s="59"/>
-      <c r="E7" s="67"/>
+      <c r="D7" s="61"/>
+      <c r="E7" s="55"/>
     </row>
     <row r="8" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="4">
@@ -3958,50 +3966,50 @@
       <c r="F11" s="47"/>
     </row>
     <row r="12" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B12" s="88">
+      <c r="B12" s="87">
         <v>99</v>
       </c>
-      <c r="C12" s="88" t="s">
+      <c r="C12" s="87" t="s">
         <v>190</v>
       </c>
       <c r="D12" s="27" t="s">
         <v>191</v>
       </c>
-      <c r="E12" s="67" t="s">
+      <c r="E12" s="55" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="13" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B13" s="62"/>
-      <c r="C13" s="62"/>
+      <c r="B13" s="59"/>
+      <c r="C13" s="59"/>
       <c r="D13" s="8" t="s">
         <v>192</v>
       </c>
-      <c r="E13" s="67"/>
+      <c r="E13" s="55"/>
     </row>
     <row r="14" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B14" s="62"/>
-      <c r="C14" s="62"/>
+      <c r="B14" s="59"/>
+      <c r="C14" s="59"/>
       <c r="D14" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="E14" s="67"/>
+      <c r="E14" s="55"/>
     </row>
     <row r="15" spans="2:6" ht="50.4" x14ac:dyDescent="0.3">
-      <c r="B15" s="62"/>
-      <c r="C15" s="62"/>
+      <c r="B15" s="59"/>
+      <c r="C15" s="59"/>
       <c r="D15" s="8" t="s">
         <v>194</v>
       </c>
-      <c r="E15" s="67"/>
+      <c r="E15" s="55"/>
     </row>
     <row r="16" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="57"/>
-      <c r="C16" s="57"/>
+      <c r="B16" s="62"/>
+      <c r="C16" s="62"/>
       <c r="D16" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="E16" s="67"/>
+      <c r="E16" s="55"/>
     </row>
     <row r="17" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="2">
@@ -4018,42 +4026,37 @@
       </c>
     </row>
     <row r="18" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B18" s="56">
+      <c r="B18" s="58">
         <v>101</v>
       </c>
-      <c r="C18" s="56" t="s">
+      <c r="C18" s="58" t="s">
         <v>198</v>
       </c>
       <c r="D18" s="8" t="s">
         <v>199</v>
       </c>
-      <c r="E18" s="67" t="s">
+      <c r="E18" s="55" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="19" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B19" s="62"/>
-      <c r="C19" s="62"/>
+      <c r="B19" s="59"/>
+      <c r="C19" s="59"/>
       <c r="D19" s="8" t="s">
         <v>200</v>
       </c>
-      <c r="E19" s="67"/>
+      <c r="E19" s="55"/>
     </row>
     <row r="20" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="57"/>
-      <c r="C20" s="57"/>
+      <c r="B20" s="62"/>
+      <c r="C20" s="62"/>
       <c r="D20" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="E20" s="67"/>
+      <c r="E20" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="E12:E16"/>
-    <mergeCell ref="E18:E20"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="B4:B5"/>
@@ -4064,6 +4067,11 @@
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="B12:B16"/>
     <mergeCell ref="C12:C16"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="E12:E16"/>
+    <mergeCell ref="E18:E20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4103,61 +4111,61 @@
       <c r="D2" s="63" t="s">
         <v>36</v>
       </c>
-      <c r="E2" s="67" t="s">
+      <c r="E2" s="55" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="3" spans="2:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="59"/>
+      <c r="B3" s="61"/>
       <c r="C3" s="7" t="s">
         <v>179</v>
       </c>
-      <c r="D3" s="59"/>
-      <c r="E3" s="67"/>
+      <c r="D3" s="61"/>
+      <c r="E3" s="55"/>
     </row>
     <row r="4" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B4" s="56">
+      <c r="B4" s="58">
         <v>103</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>202</v>
       </c>
-      <c r="D4" s="56" t="s">
+      <c r="D4" s="58" t="s">
         <v>71</v>
       </c>
-      <c r="E4" s="67" t="s">
+      <c r="E4" s="55" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="5" spans="2:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="57"/>
+      <c r="B5" s="62"/>
       <c r="C5" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="D5" s="57"/>
-      <c r="E5" s="67"/>
+      <c r="D5" s="62"/>
+      <c r="E5" s="55"/>
     </row>
     <row r="6" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B6" s="58">
+      <c r="B6" s="60">
         <v>104</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="58" t="s">
+      <c r="D6" s="60" t="s">
         <v>182</v>
       </c>
-      <c r="E6" s="67" t="s">
+      <c r="E6" s="55" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="7" spans="2:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="59"/>
+      <c r="B7" s="61"/>
       <c r="C7" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="D7" s="59"/>
-      <c r="E7" s="67"/>
+      <c r="D7" s="61"/>
+      <c r="E7" s="55"/>
     </row>
     <row r="8" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="4">
@@ -4328,24 +4336,24 @@
       </c>
     </row>
     <row r="20" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B20" s="56">
+      <c r="B20" s="58">
         <v>117</v>
       </c>
       <c r="C20" s="8" t="s">
         <v>223</v>
       </c>
-      <c r="D20" s="56" t="s">
+      <c r="D20" s="58" t="s">
         <v>56</v>
       </c>
-      <c r="E20" s="67"/>
+      <c r="E20" s="55"/>
     </row>
     <row r="21" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="57"/>
+      <c r="B21" s="62"/>
       <c r="C21" s="4" t="s">
         <v>224</v>
       </c>
-      <c r="D21" s="57"/>
-      <c r="E21" s="67"/>
+      <c r="D21" s="62"/>
+      <c r="E21" s="55"/>
     </row>
     <row r="22" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B22" s="2">
@@ -4457,13 +4465,13 @@
       </c>
     </row>
     <row r="30" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B30" s="58">
+      <c r="B30" s="60">
         <v>126</v>
       </c>
       <c r="C30" s="6" t="s">
         <v>267</v>
       </c>
-      <c r="D30" s="58" t="s">
+      <c r="D30" s="60" t="s">
         <v>241</v>
       </c>
       <c r="E30" s="39" t="s">
@@ -4471,12 +4479,18 @@
       </c>
     </row>
     <row r="31" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B31" s="59"/>
+      <c r="B31" s="61"/>
       <c r="C31" s="2"/>
-      <c r="D31" s="59"/>
+      <c r="D31" s="61"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="D20:D21"/>
     <mergeCell ref="E20:E21"/>
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="E4:E5"/>
@@ -4485,12 +4499,6 @@
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="D4:D5"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="D20:D21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Filestream and SSL for Server
</commit_message>
<xml_diff>
--- a/Checklist.xlsx
+++ b/Checklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Prashant\AziraPowershellscript\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9433CB5C-0B1E-48A8-BEAA-516010EE31C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC2019FD-0EB0-4594-B6C1-051AC1C3317F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Application" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="272">
   <si>
     <t xml:space="preserve"> Last Updated</t>
   </si>
@@ -1341,7 +1341,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1493,42 +1493,57 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1538,80 +1553,77 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="4" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="4" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="4" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="4" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2023,9 +2035,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A39" sqref="A39:XFD39"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A40" sqref="A40:XFD40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2055,11 +2067,11 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="56" t="s">
+      <c r="B2" s="64" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="65"/>
     </row>
     <row r="3" spans="1:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="12">
@@ -2090,11 +2102,11 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="65" t="s">
+      <c r="B5" s="69" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="66"/>
-      <c r="D5" s="66"/>
+      <c r="C5" s="70"/>
+      <c r="D5" s="70"/>
     </row>
     <row r="6" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B6" s="13">
@@ -2103,10 +2115,10 @@
       <c r="C6" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="63" t="s">
+      <c r="D6" s="67" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="55" t="s">
+      <c r="E6" s="71" t="s">
         <v>266</v>
       </c>
     </row>
@@ -2115,8 +2127,8 @@
       <c r="C7" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="61"/>
-      <c r="E7" s="55"/>
+      <c r="D7" s="63"/>
+      <c r="E7" s="71"/>
     </row>
     <row r="8" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A8" s="54"/>
@@ -2126,10 +2138,10 @@
       <c r="C8" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="58" t="s">
+      <c r="D8" s="60" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="55"/>
+      <c r="E8" s="71"/>
     </row>
     <row r="9" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="54"/>
@@ -2137,8 +2149,8 @@
       <c r="C9" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="62"/>
-      <c r="E9" s="55"/>
+      <c r="D9" s="61"/>
+      <c r="E9" s="71"/>
     </row>
     <row r="10" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B10" s="13">
@@ -2147,10 +2159,10 @@
       <c r="C10" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="63" t="s">
+      <c r="D10" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="55" t="s">
+      <c r="E10" s="71" t="s">
         <v>266</v>
       </c>
     </row>
@@ -2159,8 +2171,8 @@
       <c r="C11" s="16" t="s">
         <v>261</v>
       </c>
-      <c r="D11" s="64"/>
-      <c r="E11" s="55"/>
+      <c r="D11" s="68"/>
+      <c r="E11" s="71"/>
     </row>
     <row r="12" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B12" s="11">
@@ -2169,10 +2181,10 @@
       <c r="C12" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="58" t="s">
+      <c r="D12" s="60" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="55" t="s">
+      <c r="E12" s="71" t="s">
         <v>266</v>
       </c>
     </row>
@@ -2181,8 +2193,8 @@
       <c r="C13" s="17" t="s">
         <v>261</v>
       </c>
-      <c r="D13" s="59"/>
-      <c r="E13" s="55"/>
+      <c r="D13" s="66"/>
+      <c r="E13" s="71"/>
     </row>
     <row r="14" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B14" s="11">
@@ -2191,10 +2203,10 @@
       <c r="C14" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="60" t="s">
+      <c r="D14" s="62" t="s">
         <v>14</v>
       </c>
-      <c r="E14" s="55" t="s">
+      <c r="E14" s="71" t="s">
         <v>266</v>
       </c>
     </row>
@@ -2203,8 +2215,8 @@
       <c r="C15" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="61"/>
-      <c r="E15" s="55"/>
+      <c r="D15" s="63"/>
+      <c r="E15" s="71"/>
     </row>
     <row r="16" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B16" s="11">
@@ -2213,10 +2225,10 @@
       <c r="C16" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="58" t="s">
+      <c r="D16" s="60" t="s">
         <v>17</v>
       </c>
-      <c r="E16" s="55" t="s">
+      <c r="E16" s="71" t="s">
         <v>266</v>
       </c>
     </row>
@@ -2225,8 +2237,8 @@
       <c r="C17" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="62"/>
-      <c r="E17" s="55"/>
+      <c r="D17" s="61"/>
+      <c r="E17" s="71"/>
     </row>
     <row r="18" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B18" s="11">
@@ -2235,10 +2247,10 @@
       <c r="C18" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D18" s="60">
+      <c r="D18" s="62">
         <v>4</v>
       </c>
-      <c r="E18" s="55" t="s">
+      <c r="E18" s="71" t="s">
         <v>266</v>
       </c>
     </row>
@@ -2247,8 +2259,8 @@
       <c r="C19" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D19" s="61"/>
-      <c r="E19" s="55"/>
+      <c r="D19" s="63"/>
+      <c r="E19" s="71"/>
     </row>
     <row r="20" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B20" s="1">
@@ -2260,7 +2272,7 @@
       <c r="D20" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E20" s="55" t="s">
+      <c r="E20" s="71" t="s">
         <v>266</v>
       </c>
     </row>
@@ -2271,7 +2283,7 @@
       <c r="D21" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E21" s="55"/>
+      <c r="E21" s="71"/>
     </row>
     <row r="22" spans="2:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="11">
@@ -2280,10 +2292,10 @@
       <c r="C22" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D22" s="58" t="s">
+      <c r="D22" s="60" t="s">
         <v>25</v>
       </c>
-      <c r="E22" s="55" t="s">
+      <c r="E22" s="71" t="s">
         <v>266</v>
       </c>
     </row>
@@ -2292,8 +2304,8 @@
       <c r="C23" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="D23" s="62"/>
-      <c r="E23" s="55"/>
+      <c r="D23" s="61"/>
+      <c r="E23" s="71"/>
     </row>
     <row r="24" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B24" s="11">
@@ -2302,10 +2314,10 @@
       <c r="C24" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D24" s="60" t="s">
+      <c r="D24" s="62" t="s">
         <v>28</v>
       </c>
-      <c r="E24" s="55" t="s">
+      <c r="E24" s="71" t="s">
         <v>266</v>
       </c>
     </row>
@@ -2314,8 +2326,8 @@
       <c r="C25" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="D25" s="61"/>
-      <c r="E25" s="55"/>
+      <c r="D25" s="63"/>
+      <c r="E25" s="71"/>
     </row>
     <row r="26" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B26" s="11">
@@ -2324,10 +2336,10 @@
       <c r="C26" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="D26" s="58" t="s">
+      <c r="D26" s="60" t="s">
         <v>31</v>
       </c>
-      <c r="E26" s="55" t="s">
+      <c r="E26" s="71" t="s">
         <v>266</v>
       </c>
     </row>
@@ -2336,8 +2348,8 @@
       <c r="C27" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D27" s="62"/>
-      <c r="E27" s="55"/>
+      <c r="D27" s="61"/>
+      <c r="E27" s="71"/>
     </row>
     <row r="28" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="11">
@@ -2346,18 +2358,18 @@
       <c r="C28" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="D28" s="60" t="s">
+      <c r="D28" s="62" t="s">
         <v>34</v>
       </c>
-      <c r="E28" s="55"/>
+      <c r="E28" s="71"/>
     </row>
     <row r="29" spans="2:5" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B29" s="1"/>
       <c r="C29" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D29" s="61"/>
-      <c r="E29" s="55"/>
+      <c r="D29" s="63"/>
+      <c r="E29" s="71"/>
     </row>
     <row r="30" spans="2:5" ht="32.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B30" s="20">
@@ -2371,10 +2383,10 @@
       </c>
     </row>
     <row r="31" spans="2:5" s="48" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B31" s="93">
+      <c r="B31" s="58">
         <v>16</v>
       </c>
-      <c r="C31" s="94" t="s">
+      <c r="C31" s="59" t="s">
         <v>37</v>
       </c>
       <c r="D31" s="45" t="s">
@@ -2384,22 +2396,25 @@
         <v>265</v>
       </c>
     </row>
-    <row r="32" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B32" s="1">
+    <row r="32" spans="2:5" s="44" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B32" s="95">
         <v>17</v>
       </c>
-      <c r="C32" s="18" t="s">
+      <c r="C32" s="96" t="s">
         <v>39</v>
       </c>
-      <c r="D32" s="4" t="s">
+      <c r="D32" s="97" t="s">
         <v>38</v>
       </c>
+      <c r="E32" s="98" t="s">
+        <v>265</v>
+      </c>
     </row>
     <row r="33" spans="2:5" s="48" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B33" s="93">
+      <c r="B33" s="58">
         <v>18</v>
       </c>
-      <c r="C33" s="94" t="s">
+      <c r="C33" s="59" t="s">
         <v>40</v>
       </c>
       <c r="D33" s="45" t="s">
@@ -2409,22 +2424,25 @@
         <v>265</v>
       </c>
     </row>
-    <row r="34" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B34" s="1">
+    <row r="34" spans="2:5" s="44" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B34" s="95">
         <v>19</v>
       </c>
-      <c r="C34" s="18" t="s">
+      <c r="C34" s="96" t="s">
         <v>41</v>
       </c>
-      <c r="D34" s="4" t="s">
+      <c r="D34" s="97" t="s">
         <v>38</v>
       </c>
+      <c r="E34" s="98" t="s">
+        <v>265</v>
+      </c>
     </row>
     <row r="35" spans="2:5" s="48" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B35" s="93">
+      <c r="B35" s="58">
         <v>20</v>
       </c>
-      <c r="C35" s="94" t="s">
+      <c r="C35" s="59" t="s">
         <v>42</v>
       </c>
       <c r="D35" s="45" t="s">
@@ -2434,22 +2452,25 @@
         <v>265</v>
       </c>
     </row>
-    <row r="36" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B36" s="1">
+    <row r="36" spans="2:5" s="44" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B36" s="95">
         <v>21</v>
       </c>
-      <c r="C36" s="18" t="s">
+      <c r="C36" s="96" t="s">
         <v>43</v>
       </c>
-      <c r="D36" s="4" t="s">
+      <c r="D36" s="97" t="s">
         <v>38</v>
       </c>
+      <c r="E36" s="98" t="s">
+        <v>265</v>
+      </c>
     </row>
     <row r="37" spans="2:5" s="48" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B37" s="93">
+      <c r="B37" s="58">
         <v>22</v>
       </c>
-      <c r="C37" s="94" t="s">
+      <c r="C37" s="59" t="s">
         <v>44</v>
       </c>
       <c r="D37" s="45" t="s">
@@ -2459,22 +2480,25 @@
         <v>265</v>
       </c>
     </row>
-    <row r="38" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B38" s="1">
+    <row r="38" spans="2:5" s="44" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B38" s="95">
         <v>23</v>
       </c>
-      <c r="C38" s="18" t="s">
+      <c r="C38" s="96" t="s">
         <v>45</v>
       </c>
-      <c r="D38" s="4" t="s">
+      <c r="D38" s="97" t="s">
         <v>38</v>
       </c>
+      <c r="E38" s="98" t="s">
+        <v>265</v>
+      </c>
     </row>
     <row r="39" spans="2:5" s="48" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B39" s="93">
+      <c r="B39" s="58">
         <v>24</v>
       </c>
-      <c r="C39" s="94" t="s">
+      <c r="C39" s="59" t="s">
         <v>46</v>
       </c>
       <c r="D39" s="45" t="s">
@@ -2484,15 +2508,18 @@
         <v>265</v>
       </c>
     </row>
-    <row r="40" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B40" s="1">
+    <row r="40" spans="2:5" s="44" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B40" s="95">
         <v>25</v>
       </c>
-      <c r="C40" s="18" t="s">
+      <c r="C40" s="96" t="s">
         <v>47</v>
       </c>
-      <c r="D40" s="4" t="s">
+      <c r="D40" s="97" t="s">
         <v>36</v>
+      </c>
+      <c r="E40" s="98" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="41" spans="2:5" s="25" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
@@ -2503,19 +2530,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="D6:D7"/>
     <mergeCell ref="E26:E27"/>
     <mergeCell ref="E28:E29"/>
     <mergeCell ref="E12:E13"/>
@@ -2528,6 +2542,19 @@
     <mergeCell ref="E24:E25"/>
     <mergeCell ref="E16:E17"/>
     <mergeCell ref="E14:E15"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="D18:D19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2669,89 +2696,89 @@
       <c r="B9" s="49">
         <v>33</v>
       </c>
-      <c r="C9" s="67" t="s">
+      <c r="C9" s="72" t="s">
         <v>61</v>
       </c>
       <c r="D9" s="50" t="s">
         <v>62</v>
       </c>
-      <c r="E9" s="69" t="s">
+      <c r="E9" s="74" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="10" spans="2:6" s="48" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="51"/>
-      <c r="C10" s="68"/>
+      <c r="C10" s="73"/>
       <c r="D10" s="45" t="s">
         <v>63</v>
       </c>
-      <c r="E10" s="69"/>
+      <c r="E10" s="74"/>
     </row>
     <row r="11" spans="2:6" s="48" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B11" s="49">
         <v>34</v>
       </c>
-      <c r="C11" s="67" t="s">
+      <c r="C11" s="72" t="s">
         <v>64</v>
       </c>
       <c r="D11" s="50" t="s">
         <v>65</v>
       </c>
-      <c r="E11" s="69" t="s">
+      <c r="E11" s="74" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="12" spans="2:6" s="48" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="51"/>
-      <c r="C12" s="68"/>
+      <c r="C12" s="73"/>
       <c r="D12" s="45" t="s">
         <v>63</v>
       </c>
-      <c r="E12" s="69"/>
+      <c r="E12" s="74"/>
     </row>
     <row r="13" spans="2:6" s="48" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B13" s="49">
         <v>35</v>
       </c>
-      <c r="C13" s="67" t="s">
+      <c r="C13" s="72" t="s">
         <v>66</v>
       </c>
       <c r="D13" s="50" t="s">
         <v>62</v>
       </c>
-      <c r="E13" s="69" t="s">
+      <c r="E13" s="74" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="14" spans="2:6" s="48" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="51"/>
-      <c r="C14" s="68"/>
+      <c r="C14" s="73"/>
       <c r="D14" s="45" t="s">
         <v>67</v>
       </c>
-      <c r="E14" s="69"/>
+      <c r="E14" s="74"/>
     </row>
     <row r="15" spans="2:6" s="48" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B15" s="49">
         <v>36</v>
       </c>
-      <c r="C15" s="67" t="s">
+      <c r="C15" s="72" t="s">
         <v>68</v>
       </c>
       <c r="D15" s="50" t="s">
         <v>65</v>
       </c>
-      <c r="E15" s="69" t="s">
+      <c r="E15" s="74" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="16" spans="2:6" s="48" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="51"/>
-      <c r="C16" s="68"/>
+      <c r="C16" s="73"/>
       <c r="D16" s="45" t="s">
         <v>67</v>
       </c>
-      <c r="E16" s="69"/>
+      <c r="E16" s="74"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -2773,8 +2800,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B2:F80"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C49" sqref="A49:XFD54"/>
+    <sheetView tabSelected="1" topLeftCell="B68" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E75" sqref="E75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2796,313 +2823,313 @@
       </c>
     </row>
     <row r="3" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B3" s="63">
+      <c r="B3" s="67">
         <v>37</v>
       </c>
       <c r="C3" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="63" t="s">
+      <c r="D3" s="67" t="s">
         <v>71</v>
       </c>
-      <c r="E3" s="55" t="s">
+      <c r="E3" s="71" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="4" spans="2:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="61"/>
+      <c r="B4" s="63"/>
       <c r="C4" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="D4" s="61"/>
-      <c r="E4" s="55"/>
+      <c r="D4" s="63"/>
+      <c r="E4" s="71"/>
     </row>
     <row r="5" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B5" s="58">
+      <c r="B5" s="60">
         <v>38</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="58" t="s">
+      <c r="D5" s="60" t="s">
         <v>73</v>
       </c>
-      <c r="E5" s="55" t="s">
+      <c r="E5" s="71" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="6" spans="2:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="62"/>
+      <c r="B6" s="61"/>
       <c r="C6" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="D6" s="62"/>
-      <c r="E6" s="55"/>
+      <c r="D6" s="61"/>
+      <c r="E6" s="71"/>
     </row>
     <row r="7" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B7" s="60">
+      <c r="B7" s="62">
         <v>39</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="60" t="s">
+      <c r="D7" s="62" t="s">
         <v>31</v>
       </c>
-      <c r="E7" s="55" t="s">
+      <c r="E7" s="71" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="8" spans="2:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="61"/>
+      <c r="B8" s="63"/>
       <c r="C8" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="D8" s="61"/>
-      <c r="E8" s="55"/>
+      <c r="D8" s="63"/>
+      <c r="E8" s="71"/>
     </row>
     <row r="9" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B9" s="58">
+      <c r="B9" s="60">
         <v>40</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="D9" s="58" t="s">
+      <c r="D9" s="60" t="s">
         <v>77</v>
       </c>
-      <c r="E9" s="55" t="s">
+      <c r="E9" s="71" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="10" spans="2:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="62"/>
+      <c r="B10" s="61"/>
       <c r="C10" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="D10" s="62"/>
-      <c r="E10" s="55"/>
+      <c r="D10" s="61"/>
+      <c r="E10" s="71"/>
     </row>
     <row r="11" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B11" s="60">
+      <c r="B11" s="62">
         <v>41</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="D11" s="60" t="s">
+      <c r="D11" s="62" t="s">
         <v>80</v>
       </c>
-      <c r="E11" s="55" t="s">
+      <c r="E11" s="71" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="12" spans="2:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="61"/>
+      <c r="B12" s="63"/>
       <c r="C12" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="D12" s="61"/>
-      <c r="E12" s="55"/>
+      <c r="D12" s="63"/>
+      <c r="E12" s="71"/>
     </row>
     <row r="13" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B13" s="58">
+      <c r="B13" s="60">
         <v>42</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="D13" s="58" t="s">
+      <c r="D13" s="60" t="s">
         <v>83</v>
       </c>
-      <c r="E13" s="55" t="s">
+      <c r="E13" s="71" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="14" spans="2:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="62"/>
+      <c r="B14" s="61"/>
       <c r="C14" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="D14" s="62"/>
-      <c r="E14" s="55"/>
+      <c r="D14" s="61"/>
+      <c r="E14" s="71"/>
     </row>
     <row r="15" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B15" s="78">
+      <c r="B15" s="89">
         <v>43</v>
       </c>
       <c r="C15" s="29" t="s">
         <v>84</v>
       </c>
-      <c r="D15" s="78" t="s">
+      <c r="D15" s="89" t="s">
         <v>86</v>
       </c>
-      <c r="E15" s="55" t="s">
+      <c r="E15" s="71" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="16" spans="2:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="73"/>
+      <c r="B16" s="78"/>
       <c r="C16" s="30" t="s">
         <v>85</v>
       </c>
-      <c r="D16" s="73"/>
-      <c r="E16" s="55"/>
+      <c r="D16" s="78"/>
+      <c r="E16" s="71"/>
     </row>
     <row r="17" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B17" s="74">
+      <c r="B17" s="79">
         <v>44</v>
       </c>
       <c r="C17" s="31" t="s">
         <v>87</v>
       </c>
-      <c r="D17" s="79">
+      <c r="D17" s="90">
         <v>987654321</v>
       </c>
-      <c r="E17" s="55"/>
+      <c r="E17" s="71"/>
     </row>
     <row r="18" spans="2:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="75"/>
+      <c r="B18" s="80"/>
       <c r="C18" s="32" t="s">
         <v>88</v>
       </c>
-      <c r="D18" s="80"/>
-      <c r="E18" s="55"/>
+      <c r="D18" s="91"/>
+      <c r="E18" s="71"/>
     </row>
     <row r="19" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B19" s="72">
+      <c r="B19" s="77">
         <v>45</v>
       </c>
       <c r="C19" s="33" t="s">
         <v>89</v>
       </c>
-      <c r="D19" s="72">
+      <c r="D19" s="77">
         <v>1433</v>
       </c>
-      <c r="E19" s="55" t="s">
+      <c r="E19" s="71" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="20" spans="2:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="73"/>
+      <c r="B20" s="78"/>
       <c r="C20" s="30" t="s">
         <v>90</v>
       </c>
-      <c r="D20" s="73"/>
-      <c r="E20" s="55"/>
+      <c r="D20" s="78"/>
+      <c r="E20" s="71"/>
     </row>
     <row r="21" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B21" s="74">
+      <c r="B21" s="79">
         <v>46</v>
       </c>
       <c r="C21" s="31" t="s">
         <v>91</v>
       </c>
-      <c r="D21" s="76">
+      <c r="D21" s="86">
         <v>43925</v>
       </c>
-      <c r="E21" s="71" t="s">
+      <c r="E21" s="93" t="s">
         <v>269</v>
       </c>
     </row>
     <row r="22" spans="2:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="75"/>
+      <c r="B22" s="80"/>
       <c r="C22" s="32" t="s">
         <v>92</v>
       </c>
-      <c r="D22" s="77"/>
-      <c r="E22" s="55"/>
+      <c r="D22" s="88"/>
+      <c r="E22" s="71"/>
     </row>
     <row r="23" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B23" s="72">
+      <c r="B23" s="77">
         <v>47</v>
       </c>
       <c r="C23" s="33" t="s">
         <v>93</v>
       </c>
-      <c r="D23" s="81" t="s">
+      <c r="D23" s="84" t="s">
         <v>7</v>
       </c>
-      <c r="E23" s="71" t="s">
+      <c r="E23" s="93" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="24" spans="2:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="73"/>
+      <c r="B24" s="78"/>
       <c r="C24" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="D24" s="82"/>
-      <c r="E24" s="55"/>
+      <c r="D24" s="85"/>
+      <c r="E24" s="71"/>
     </row>
     <row r="25" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B25" s="74">
+      <c r="B25" s="79">
         <v>48</v>
       </c>
       <c r="C25" s="31" t="s">
         <v>94</v>
       </c>
-      <c r="D25" s="76">
+      <c r="D25" s="86">
         <v>43834</v>
       </c>
-      <c r="E25" s="71" t="s">
+      <c r="E25" s="93" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="26" spans="2:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B26" s="75"/>
+      <c r="B26" s="80"/>
       <c r="C26" s="32" t="s">
         <v>95</v>
       </c>
-      <c r="D26" s="83"/>
-      <c r="E26" s="55"/>
+      <c r="D26" s="87"/>
+      <c r="E26" s="71"/>
     </row>
     <row r="27" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B27" s="72">
+      <c r="B27" s="77">
         <v>49</v>
       </c>
       <c r="C27" s="33" t="s">
         <v>96</v>
       </c>
-      <c r="D27" s="72">
+      <c r="D27" s="77">
         <v>0</v>
       </c>
-      <c r="E27" s="71" t="s">
+      <c r="E27" s="93" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="28" spans="2:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="73"/>
+      <c r="B28" s="78"/>
       <c r="C28" s="30" t="s">
         <v>96</v>
       </c>
-      <c r="D28" s="73"/>
-      <c r="E28" s="55"/>
+      <c r="D28" s="78"/>
+      <c r="E28" s="71"/>
     </row>
     <row r="29" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B29" s="74">
+      <c r="B29" s="79">
         <v>50</v>
       </c>
       <c r="C29" s="31" t="s">
         <v>97</v>
       </c>
-      <c r="D29" s="74">
+      <c r="D29" s="79">
         <v>5</v>
       </c>
-      <c r="E29" s="71" t="s">
+      <c r="E29" s="93" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="30" spans="2:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B30" s="75"/>
+      <c r="B30" s="80"/>
       <c r="C30" s="32" t="s">
         <v>98</v>
       </c>
-      <c r="D30" s="75"/>
-      <c r="E30" s="55"/>
+      <c r="D30" s="80"/>
+      <c r="E30" s="71"/>
     </row>
     <row r="31" spans="2:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="72">
+      <c r="B31" s="77">
         <v>51</v>
       </c>
       <c r="C31" s="33" t="s">
@@ -3111,85 +3138,85 @@
       <c r="D31" s="33" t="s">
         <v>101</v>
       </c>
-      <c r="E31" s="55" t="s">
+      <c r="E31" s="71" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="32" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B32" s="73"/>
+      <c r="B32" s="78"/>
       <c r="C32" s="30" t="s">
         <v>100</v>
       </c>
       <c r="D32" s="34" t="s">
         <v>102</v>
       </c>
-      <c r="E32" s="55"/>
+      <c r="E32" s="71"/>
     </row>
     <row r="33" spans="2:5" s="44" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B33" s="85">
+      <c r="B33" s="82">
         <v>52</v>
       </c>
       <c r="C33" s="52" t="s">
         <v>103</v>
       </c>
-      <c r="D33" s="85" t="s">
+      <c r="D33" s="82" t="s">
         <v>105</v>
       </c>
-      <c r="E33" s="70" t="s">
+      <c r="E33" s="92" t="s">
         <v>265</v>
       </c>
     </row>
     <row r="34" spans="2:5" s="44" customFormat="1" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B34" s="86"/>
+      <c r="B34" s="83"/>
       <c r="C34" s="53" t="s">
         <v>104</v>
       </c>
-      <c r="D34" s="86"/>
-      <c r="E34" s="70"/>
+      <c r="D34" s="83"/>
+      <c r="E34" s="92"/>
     </row>
     <row r="35" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B35" s="72">
+      <c r="B35" s="77">
         <v>53</v>
       </c>
       <c r="C35" s="33" t="s">
         <v>106</v>
       </c>
-      <c r="D35" s="72" t="s">
+      <c r="D35" s="77" t="s">
         <v>108</v>
       </c>
-      <c r="E35" s="55" t="s">
+      <c r="E35" s="71" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="36" spans="2:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B36" s="73"/>
+      <c r="B36" s="78"/>
       <c r="C36" s="30" t="s">
         <v>107</v>
       </c>
-      <c r="D36" s="73"/>
-      <c r="E36" s="55"/>
+      <c r="D36" s="78"/>
+      <c r="E36" s="71"/>
     </row>
     <row r="37" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B37" s="74">
+      <c r="B37" s="79">
         <v>54</v>
       </c>
       <c r="C37" s="31" t="s">
         <v>109</v>
       </c>
-      <c r="D37" s="74" t="s">
+      <c r="D37" s="79" t="s">
         <v>111</v>
       </c>
-      <c r="E37" s="55" t="s">
+      <c r="E37" s="71" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="38" spans="2:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B38" s="75"/>
+      <c r="B38" s="80"/>
       <c r="C38" s="32" t="s">
         <v>110</v>
       </c>
-      <c r="D38" s="75"/>
-      <c r="E38" s="55"/>
+      <c r="D38" s="80"/>
+      <c r="E38" s="71"/>
     </row>
     <row r="39" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B39" s="34">
@@ -3234,48 +3261,48 @@
       </c>
     </row>
     <row r="42" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="84">
+      <c r="B42" s="81">
         <v>58</v>
       </c>
       <c r="C42" s="37" t="s">
         <v>117</v>
       </c>
-      <c r="D42" s="84" t="s">
+      <c r="D42" s="81" t="s">
         <v>36</v>
       </c>
-      <c r="E42" s="55" t="s">
+      <c r="E42" s="71" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="43" spans="2:5" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B43" s="75"/>
+      <c r="B43" s="80"/>
       <c r="C43" s="32" t="s">
         <v>118</v>
       </c>
-      <c r="D43" s="75"/>
-      <c r="E43" s="55"/>
+      <c r="D43" s="80"/>
+      <c r="E43" s="71"/>
     </row>
     <row r="44" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B44" s="72">
+      <c r="B44" s="77">
         <v>59</v>
       </c>
       <c r="C44" s="33" t="s">
         <v>119</v>
       </c>
-      <c r="D44" s="72" t="s">
+      <c r="D44" s="77" t="s">
         <v>36</v>
       </c>
-      <c r="E44" s="55" t="s">
+      <c r="E44" s="71" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="45" spans="2:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B45" s="73"/>
+      <c r="B45" s="78"/>
       <c r="C45" s="30" t="s">
         <v>120</v>
       </c>
-      <c r="D45" s="73"/>
-      <c r="E45" s="55"/>
+      <c r="D45" s="78"/>
+      <c r="E45" s="71"/>
     </row>
     <row r="46" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B46" s="36">
@@ -3292,13 +3319,13 @@
       </c>
     </row>
     <row r="47" spans="2:5" s="48" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B47" s="88">
+      <c r="B47" s="55">
         <v>61</v>
       </c>
-      <c r="C47" s="88" t="s">
+      <c r="C47" s="55" t="s">
         <v>123</v>
       </c>
-      <c r="D47" s="88" t="s">
+      <c r="D47" s="55" t="s">
         <v>124</v>
       </c>
       <c r="E47" s="46" t="s">
@@ -3320,70 +3347,70 @@
       </c>
     </row>
     <row r="49" spans="2:5" s="48" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B49" s="89">
+      <c r="B49" s="75">
         <v>63</v>
       </c>
-      <c r="C49" s="90" t="s">
+      <c r="C49" s="56" t="s">
         <v>126</v>
       </c>
-      <c r="D49" s="89" t="s">
+      <c r="D49" s="75" t="s">
         <v>128</v>
       </c>
-      <c r="E49" s="69" t="s">
+      <c r="E49" s="74" t="s">
         <v>265</v>
       </c>
     </row>
     <row r="50" spans="2:5" s="48" customFormat="1" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B50" s="91"/>
-      <c r="C50" s="92" t="s">
+      <c r="B50" s="76"/>
+      <c r="C50" s="57" t="s">
         <v>127</v>
       </c>
-      <c r="D50" s="91"/>
-      <c r="E50" s="69"/>
+      <c r="D50" s="76"/>
+      <c r="E50" s="74"/>
     </row>
     <row r="51" spans="2:5" s="48" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B51" s="89">
+      <c r="B51" s="75">
         <v>64</v>
       </c>
-      <c r="C51" s="90" t="s">
+      <c r="C51" s="56" t="s">
         <v>129</v>
       </c>
-      <c r="D51" s="89" t="s">
+      <c r="D51" s="75" t="s">
         <v>131</v>
       </c>
-      <c r="E51" s="69" t="s">
+      <c r="E51" s="74" t="s">
         <v>265</v>
       </c>
     </row>
     <row r="52" spans="2:5" s="48" customFormat="1" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B52" s="91"/>
-      <c r="C52" s="92" t="s">
+      <c r="B52" s="76"/>
+      <c r="C52" s="57" t="s">
         <v>130</v>
       </c>
-      <c r="D52" s="91"/>
-      <c r="E52" s="69"/>
+      <c r="D52" s="76"/>
+      <c r="E52" s="74"/>
     </row>
     <row r="53" spans="2:5" s="48" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B53" s="89">
+      <c r="B53" s="75">
         <v>65</v>
       </c>
-      <c r="C53" s="90" t="s">
+      <c r="C53" s="56" t="s">
         <v>132</v>
       </c>
-      <c r="D53" s="89" t="s">
+      <c r="D53" s="75" t="s">
         <v>134</v>
       </c>
-      <c r="E53" s="69" t="s">
+      <c r="E53" s="74" t="s">
         <v>265</v>
       </c>
     </row>
     <row r="54" spans="2:5" s="48" customFormat="1" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B54" s="91"/>
-      <c r="C54" s="92" t="s">
+      <c r="B54" s="76"/>
+      <c r="C54" s="57" t="s">
         <v>133</v>
       </c>
-      <c r="D54" s="91"/>
-      <c r="E54" s="69"/>
+      <c r="D54" s="76"/>
+      <c r="E54" s="74"/>
     </row>
     <row r="55" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B55" s="36">
@@ -3651,15 +3678,18 @@
         <v>266</v>
       </c>
     </row>
-    <row r="74" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B74" s="4">
+    <row r="74" spans="2:5" s="44" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B74" s="97">
         <v>85</v>
       </c>
-      <c r="C74" s="4" t="s">
+      <c r="C74" s="97" t="s">
         <v>165</v>
       </c>
-      <c r="D74" s="4" t="s">
+      <c r="D74" s="97" t="s">
         <v>166</v>
+      </c>
+      <c r="E74" s="98" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="75" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
@@ -3745,37 +3775,27 @@
     </row>
   </sheetData>
   <mergeCells count="68">
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="D51:D52"/>
-    <mergeCell ref="B53:B54"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="D44:D45"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="D49:D50"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="D42:D43"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E49:E50"/>
+    <mergeCell ref="E51:E52"/>
+    <mergeCell ref="E53:E54"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="E44:E45"/>
+    <mergeCell ref="E42:E43"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="E31:E32"/>
     <mergeCell ref="E33:E34"/>
     <mergeCell ref="E35:E36"/>
     <mergeCell ref="B3:B4"/>
@@ -3792,27 +3812,37 @@
     <mergeCell ref="D9:D10"/>
     <mergeCell ref="B19:B20"/>
     <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="E49:E50"/>
-    <mergeCell ref="E51:E52"/>
-    <mergeCell ref="E53:E54"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="E44:E45"/>
-    <mergeCell ref="E42:E43"/>
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="D51:D52"/>
+    <mergeCell ref="B53:B54"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="D49:D50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3843,70 +3873,70 @@
       </c>
     </row>
     <row r="2" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B2" s="63">
+      <c r="B2" s="67">
         <v>92</v>
       </c>
       <c r="C2" s="15" t="s">
         <v>178</v>
       </c>
-      <c r="D2" s="63" t="s">
+      <c r="D2" s="67" t="s">
         <v>36</v>
       </c>
-      <c r="E2" s="55" t="s">
+      <c r="E2" s="71" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="3" spans="2:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="61"/>
+      <c r="B3" s="63"/>
       <c r="C3" s="7" t="s">
         <v>179</v>
       </c>
-      <c r="D3" s="61"/>
-      <c r="E3" s="55"/>
+      <c r="D3" s="63"/>
+      <c r="E3" s="71"/>
     </row>
     <row r="4" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B4" s="58">
+      <c r="B4" s="60">
         <v>93</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="58" t="s">
+      <c r="D4" s="60" t="s">
         <v>71</v>
       </c>
-      <c r="E4" s="55" t="s">
+      <c r="E4" s="71" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="5" spans="2:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="62"/>
+      <c r="B5" s="61"/>
       <c r="C5" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="D5" s="62"/>
-      <c r="E5" s="55"/>
+      <c r="D5" s="61"/>
+      <c r="E5" s="71"/>
     </row>
     <row r="6" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B6" s="60">
+      <c r="B6" s="62">
         <v>94</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="60" t="s">
+      <c r="D6" s="62" t="s">
         <v>182</v>
       </c>
-      <c r="E6" s="55" t="s">
+      <c r="E6" s="71" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="7" spans="2:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="61"/>
+      <c r="B7" s="63"/>
       <c r="C7" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="D7" s="61"/>
-      <c r="E7" s="55"/>
+      <c r="D7" s="63"/>
+      <c r="E7" s="71"/>
     </row>
     <row r="8" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="4">
@@ -3966,50 +3996,50 @@
       <c r="F11" s="47"/>
     </row>
     <row r="12" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B12" s="87">
+      <c r="B12" s="94">
         <v>99</v>
       </c>
-      <c r="C12" s="87" t="s">
+      <c r="C12" s="94" t="s">
         <v>190</v>
       </c>
       <c r="D12" s="27" t="s">
         <v>191</v>
       </c>
-      <c r="E12" s="55" t="s">
+      <c r="E12" s="71" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="13" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B13" s="59"/>
-      <c r="C13" s="59"/>
+      <c r="B13" s="66"/>
+      <c r="C13" s="66"/>
       <c r="D13" s="8" t="s">
         <v>192</v>
       </c>
-      <c r="E13" s="55"/>
+      <c r="E13" s="71"/>
     </row>
     <row r="14" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B14" s="59"/>
-      <c r="C14" s="59"/>
+      <c r="B14" s="66"/>
+      <c r="C14" s="66"/>
       <c r="D14" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="E14" s="55"/>
+      <c r="E14" s="71"/>
     </row>
     <row r="15" spans="2:6" ht="50.4" x14ac:dyDescent="0.3">
-      <c r="B15" s="59"/>
-      <c r="C15" s="59"/>
+      <c r="B15" s="66"/>
+      <c r="C15" s="66"/>
       <c r="D15" s="8" t="s">
         <v>194</v>
       </c>
-      <c r="E15" s="55"/>
+      <c r="E15" s="71"/>
     </row>
     <row r="16" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="62"/>
-      <c r="C16" s="62"/>
+      <c r="B16" s="61"/>
+      <c r="C16" s="61"/>
       <c r="D16" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="E16" s="55"/>
+      <c r="E16" s="71"/>
     </row>
     <row r="17" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="2">
@@ -4026,37 +4056,42 @@
       </c>
     </row>
     <row r="18" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B18" s="58">
+      <c r="B18" s="60">
         <v>101</v>
       </c>
-      <c r="C18" s="58" t="s">
+      <c r="C18" s="60" t="s">
         <v>198</v>
       </c>
       <c r="D18" s="8" t="s">
         <v>199</v>
       </c>
-      <c r="E18" s="55" t="s">
+      <c r="E18" s="71" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="19" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B19" s="59"/>
-      <c r="C19" s="59"/>
+      <c r="B19" s="66"/>
+      <c r="C19" s="66"/>
       <c r="D19" s="8" t="s">
         <v>200</v>
       </c>
-      <c r="E19" s="55"/>
+      <c r="E19" s="71"/>
     </row>
     <row r="20" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="62"/>
-      <c r="C20" s="62"/>
+      <c r="B20" s="61"/>
+      <c r="C20" s="61"/>
       <c r="D20" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="E20" s="55"/>
+      <c r="E20" s="71"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="E12:E16"/>
+    <mergeCell ref="E18:E20"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="B4:B5"/>
@@ -4067,11 +4102,6 @@
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="B12:B16"/>
     <mergeCell ref="C12:C16"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="E12:E16"/>
-    <mergeCell ref="E18:E20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4102,70 +4132,70 @@
       </c>
     </row>
     <row r="2" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B2" s="63">
+      <c r="B2" s="67">
         <v>102</v>
       </c>
       <c r="C2" s="15" t="s">
         <v>178</v>
       </c>
-      <c r="D2" s="63" t="s">
+      <c r="D2" s="67" t="s">
         <v>36</v>
       </c>
-      <c r="E2" s="55" t="s">
+      <c r="E2" s="71" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="3" spans="2:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="61"/>
+      <c r="B3" s="63"/>
       <c r="C3" s="7" t="s">
         <v>179</v>
       </c>
-      <c r="D3" s="61"/>
-      <c r="E3" s="55"/>
+      <c r="D3" s="63"/>
+      <c r="E3" s="71"/>
     </row>
     <row r="4" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B4" s="58">
+      <c r="B4" s="60">
         <v>103</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>202</v>
       </c>
-      <c r="D4" s="58" t="s">
+      <c r="D4" s="60" t="s">
         <v>71</v>
       </c>
-      <c r="E4" s="55" t="s">
+      <c r="E4" s="71" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="5" spans="2:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="62"/>
+      <c r="B5" s="61"/>
       <c r="C5" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="D5" s="62"/>
-      <c r="E5" s="55"/>
+      <c r="D5" s="61"/>
+      <c r="E5" s="71"/>
     </row>
     <row r="6" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B6" s="60">
+      <c r="B6" s="62">
         <v>104</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="60" t="s">
+      <c r="D6" s="62" t="s">
         <v>182</v>
       </c>
-      <c r="E6" s="55" t="s">
+      <c r="E6" s="71" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="7" spans="2:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="61"/>
+      <c r="B7" s="63"/>
       <c r="C7" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="D7" s="61"/>
-      <c r="E7" s="55"/>
+      <c r="D7" s="63"/>
+      <c r="E7" s="71"/>
     </row>
     <row r="8" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="4">
@@ -4336,24 +4366,24 @@
       </c>
     </row>
     <row r="20" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B20" s="58">
+      <c r="B20" s="60">
         <v>117</v>
       </c>
       <c r="C20" s="8" t="s">
         <v>223</v>
       </c>
-      <c r="D20" s="58" t="s">
+      <c r="D20" s="60" t="s">
         <v>56</v>
       </c>
-      <c r="E20" s="55"/>
+      <c r="E20" s="71"/>
     </row>
     <row r="21" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="62"/>
+      <c r="B21" s="61"/>
       <c r="C21" s="4" t="s">
         <v>224</v>
       </c>
-      <c r="D21" s="62"/>
-      <c r="E21" s="55"/>
+      <c r="D21" s="61"/>
+      <c r="E21" s="71"/>
     </row>
     <row r="22" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B22" s="2">
@@ -4465,13 +4495,13 @@
       </c>
     </row>
     <row r="30" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B30" s="60">
+      <c r="B30" s="62">
         <v>126</v>
       </c>
       <c r="C30" s="6" t="s">
         <v>267</v>
       </c>
-      <c r="D30" s="60" t="s">
+      <c r="D30" s="62" t="s">
         <v>241</v>
       </c>
       <c r="E30" s="39" t="s">
@@ -4479,18 +4509,12 @@
       </c>
     </row>
     <row r="31" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B31" s="61"/>
+      <c r="B31" s="63"/>
       <c r="C31" s="2"/>
-      <c r="D31" s="61"/>
+      <c r="D31" s="63"/>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="D20:D21"/>
     <mergeCell ref="E20:E21"/>
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="E4:E5"/>
@@ -4499,6 +4523,12 @@
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="D4:D5"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="D20:D21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Feedback Sheet added in Checklist
</commit_message>
<xml_diff>
--- a/Checklist.xlsx
+++ b/Checklist.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Prashant\AziraPowershellscript\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16770B7E-7D6F-46E1-BB97-6927D972BF61}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C210AA5-96C7-4803-A802-3F6AEDA2ADCA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Application" sheetId="1" r:id="rId1"/>
-    <sheet name="IISConfiguration" sheetId="6" r:id="rId2"/>
-    <sheet name="SQL Server" sheetId="2" r:id="rId3"/>
-    <sheet name="SSAS Configuration" sheetId="3" r:id="rId4"/>
-    <sheet name="SSRS Configuration" sheetId="4" r:id="rId5"/>
-    <sheet name="SQL Server Diagnostics" sheetId="5" r:id="rId6"/>
+    <sheet name="Feedback Task" sheetId="7" r:id="rId2"/>
+    <sheet name="IISConfiguration" sheetId="6" r:id="rId3"/>
+    <sheet name="SQL Server" sheetId="2" r:id="rId4"/>
+    <sheet name="SSAS Configuration" sheetId="3" r:id="rId5"/>
+    <sheet name="SSRS Configuration" sheetId="4" r:id="rId6"/>
+    <sheet name="SQL Server Diagnostics" sheetId="5" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="278">
   <si>
     <t xml:space="preserve"> Last Updated</t>
   </si>
@@ -1024,6 +1025,24 @@
   </si>
   <si>
     <t>is this the location where db is stored?</t>
+  </si>
+  <si>
+    <t>IIS Version</t>
+  </si>
+  <si>
+    <t>Timeout setting for every script</t>
+  </si>
+  <si>
+    <t>MDF &amp; LDF File Size</t>
+  </si>
+  <si>
+    <t>Web IIS Role and Sub features - need to show all features</t>
+  </si>
+  <si>
+    <t>All webservces/site are hosted on the server</t>
+  </si>
+  <si>
+    <t>Script Name</t>
   </si>
 </sst>
 </file>
@@ -1087,7 +1106,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1115,12 +1134,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
@@ -1347,7 +1360,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="103">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1472,63 +1485,72 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1541,23 +1563,20 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1571,75 +1590,56 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="16" fontId="4" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="4" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="4" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="4" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="4" fillId="9" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="4" fillId="9" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2051,9 +2051,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E30" sqref="E30"/>
+      <selection pane="bottomLeft" activeCell="A28" sqref="A28:XFD29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2083,11 +2083,11 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="62" t="s">
+      <c r="B2" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="63"/>
-      <c r="D2" s="63"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
     </row>
     <row r="3" spans="1:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="12">
@@ -2118,11 +2118,11 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="67" t="s">
+      <c r="B5" s="70" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="68"/>
-      <c r="D5" s="68"/>
+      <c r="C5" s="71"/>
+      <c r="D5" s="71"/>
     </row>
     <row r="6" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B6" s="13">
@@ -2131,10 +2131,10 @@
       <c r="C6" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="65" t="s">
+      <c r="D6" s="68" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="69" t="s">
+      <c r="E6" s="60" t="s">
         <v>266</v>
       </c>
     </row>
@@ -2143,30 +2143,30 @@
       <c r="C7" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="61"/>
-      <c r="E7" s="69"/>
+      <c r="D7" s="66"/>
+      <c r="E7" s="60"/>
     </row>
     <row r="8" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="52"/>
+      <c r="A8" s="51"/>
       <c r="B8" s="11">
         <v>4</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="58" t="s">
+      <c r="D8" s="63" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="69"/>
+      <c r="E8" s="60"/>
     </row>
     <row r="9" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="52"/>
+      <c r="A9" s="51"/>
       <c r="B9" s="1"/>
       <c r="C9" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="59"/>
-      <c r="E9" s="69"/>
+      <c r="D9" s="67"/>
+      <c r="E9" s="60"/>
     </row>
     <row r="10" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B10" s="13">
@@ -2175,10 +2175,10 @@
       <c r="C10" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="65" t="s">
+      <c r="D10" s="68" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="69" t="s">
+      <c r="E10" s="60" t="s">
         <v>266</v>
       </c>
     </row>
@@ -2187,8 +2187,8 @@
       <c r="C11" s="16" t="s">
         <v>261</v>
       </c>
-      <c r="D11" s="66"/>
-      <c r="E11" s="69"/>
+      <c r="D11" s="69"/>
+      <c r="E11" s="60"/>
     </row>
     <row r="12" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B12" s="11">
@@ -2197,10 +2197,10 @@
       <c r="C12" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="58" t="s">
+      <c r="D12" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="69" t="s">
+      <c r="E12" s="60" t="s">
         <v>266</v>
       </c>
     </row>
@@ -2210,7 +2210,7 @@
         <v>261</v>
       </c>
       <c r="D13" s="64"/>
-      <c r="E13" s="69"/>
+      <c r="E13" s="60"/>
     </row>
     <row r="14" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B14" s="11">
@@ -2219,10 +2219,10 @@
       <c r="C14" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="60" t="s">
+      <c r="D14" s="65" t="s">
         <v>14</v>
       </c>
-      <c r="E14" s="69" t="s">
+      <c r="E14" s="60" t="s">
         <v>266</v>
       </c>
     </row>
@@ -2231,8 +2231,8 @@
       <c r="C15" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="61"/>
-      <c r="E15" s="69"/>
+      <c r="D15" s="66"/>
+      <c r="E15" s="60"/>
     </row>
     <row r="16" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B16" s="11">
@@ -2241,10 +2241,10 @@
       <c r="C16" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="58" t="s">
+      <c r="D16" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="E16" s="69" t="s">
+      <c r="E16" s="60" t="s">
         <v>266</v>
       </c>
     </row>
@@ -2253,8 +2253,8 @@
       <c r="C17" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="59"/>
-      <c r="E17" s="69"/>
+      <c r="D17" s="67"/>
+      <c r="E17" s="60"/>
     </row>
     <row r="18" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B18" s="11">
@@ -2263,10 +2263,10 @@
       <c r="C18" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D18" s="60">
+      <c r="D18" s="65">
         <v>4</v>
       </c>
-      <c r="E18" s="69" t="s">
+      <c r="E18" s="60" t="s">
         <v>266</v>
       </c>
     </row>
@@ -2275,8 +2275,8 @@
       <c r="C19" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D19" s="61"/>
-      <c r="E19" s="69"/>
+      <c r="D19" s="66"/>
+      <c r="E19" s="60"/>
     </row>
     <row r="20" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B20" s="1">
@@ -2288,7 +2288,7 @@
       <c r="D20" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E20" s="69" t="s">
+      <c r="E20" s="60" t="s">
         <v>266</v>
       </c>
     </row>
@@ -2299,7 +2299,7 @@
       <c r="D21" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E21" s="69"/>
+      <c r="E21" s="60"/>
     </row>
     <row r="22" spans="2:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="11">
@@ -2308,10 +2308,10 @@
       <c r="C22" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D22" s="58" t="s">
+      <c r="D22" s="63" t="s">
         <v>25</v>
       </c>
-      <c r="E22" s="69" t="s">
+      <c r="E22" s="60" t="s">
         <v>266</v>
       </c>
     </row>
@@ -2320,8 +2320,8 @@
       <c r="C23" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="D23" s="59"/>
-      <c r="E23" s="69"/>
+      <c r="D23" s="67"/>
+      <c r="E23" s="60"/>
     </row>
     <row r="24" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B24" s="11">
@@ -2330,10 +2330,10 @@
       <c r="C24" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D24" s="60" t="s">
+      <c r="D24" s="65" t="s">
         <v>28</v>
       </c>
-      <c r="E24" s="69" t="s">
+      <c r="E24" s="60" t="s">
         <v>266</v>
       </c>
     </row>
@@ -2342,8 +2342,8 @@
       <c r="C25" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="D25" s="61"/>
-      <c r="E25" s="69"/>
+      <c r="D25" s="66"/>
+      <c r="E25" s="60"/>
     </row>
     <row r="26" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B26" s="11">
@@ -2352,10 +2352,10 @@
       <c r="C26" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="D26" s="58" t="s">
+      <c r="D26" s="63" t="s">
         <v>31</v>
       </c>
-      <c r="E26" s="69" t="s">
+      <c r="E26" s="60" t="s">
         <v>266</v>
       </c>
     </row>
@@ -2364,30 +2364,30 @@
       <c r="C27" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D27" s="59"/>
-      <c r="E27" s="69"/>
-    </row>
-    <row r="28" spans="2:5" s="44" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="97">
+      <c r="D27" s="67"/>
+      <c r="E27" s="60"/>
+    </row>
+    <row r="28" spans="2:5" s="47" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="95">
         <v>14</v>
       </c>
-      <c r="C28" s="98" t="s">
+      <c r="C28" s="49" t="s">
         <v>32</v>
       </c>
-      <c r="D28" s="99" t="s">
+      <c r="D28" s="72" t="s">
         <v>34</v>
       </c>
-      <c r="E28" s="87" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="29" spans="2:5" s="44" customFormat="1" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B29" s="100"/>
-      <c r="C29" s="101" t="s">
+      <c r="E28" s="74" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" s="47" customFormat="1" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B29" s="55"/>
+      <c r="C29" s="96" t="s">
         <v>33</v>
       </c>
-      <c r="D29" s="102"/>
-      <c r="E29" s="87"/>
+      <c r="D29" s="73"/>
+      <c r="E29" s="74"/>
     </row>
     <row r="30" spans="2:5" ht="32.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B30" s="20">
@@ -2400,143 +2400,143 @@
         <v>36</v>
       </c>
     </row>
-    <row r="31" spans="2:5" s="48" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B31" s="56">
+    <row r="31" spans="2:5" s="47" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B31" s="55">
         <v>16</v>
       </c>
-      <c r="C31" s="57" t="s">
+      <c r="C31" s="56" t="s">
         <v>37</v>
       </c>
-      <c r="D31" s="45" t="s">
+      <c r="D31" s="44" t="s">
         <v>38</v>
       </c>
-      <c r="E31" s="46" t="s">
+      <c r="E31" s="45" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="32" spans="2:5" s="48" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B32" s="56">
+    <row r="32" spans="2:5" s="47" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B32" s="55">
         <v>17</v>
       </c>
-      <c r="C32" s="57" t="s">
+      <c r="C32" s="56" t="s">
         <v>39</v>
       </c>
-      <c r="D32" s="45" t="s">
+      <c r="D32" s="44" t="s">
         <v>38</v>
       </c>
-      <c r="E32" s="46" t="s">
+      <c r="E32" s="45" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="33" spans="2:5" s="48" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B33" s="56">
+    <row r="33" spans="2:5" s="47" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B33" s="55">
         <v>18</v>
       </c>
-      <c r="C33" s="57" t="s">
+      <c r="C33" s="56" t="s">
         <v>40</v>
       </c>
-      <c r="D33" s="45" t="s">
+      <c r="D33" s="44" t="s">
         <v>38</v>
       </c>
-      <c r="E33" s="46" t="s">
+      <c r="E33" s="45" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="34" spans="2:5" s="48" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B34" s="56">
+    <row r="34" spans="2:5" s="47" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B34" s="55">
         <v>19</v>
       </c>
-      <c r="C34" s="57" t="s">
+      <c r="C34" s="56" t="s">
         <v>41</v>
       </c>
-      <c r="D34" s="45" t="s">
+      <c r="D34" s="44" t="s">
         <v>38</v>
       </c>
-      <c r="E34" s="46" t="s">
+      <c r="E34" s="45" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="35" spans="2:5" s="48" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B35" s="56">
+    <row r="35" spans="2:5" s="47" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B35" s="55">
         <v>20</v>
       </c>
-      <c r="C35" s="57" t="s">
+      <c r="C35" s="56" t="s">
         <v>42</v>
       </c>
-      <c r="D35" s="45" t="s">
+      <c r="D35" s="44" t="s">
         <v>36</v>
       </c>
-      <c r="E35" s="46" t="s">
+      <c r="E35" s="45" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="36" spans="2:5" s="48" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B36" s="56">
+    <row r="36" spans="2:5" s="47" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B36" s="55">
         <v>21</v>
       </c>
-      <c r="C36" s="57" t="s">
+      <c r="C36" s="56" t="s">
         <v>43</v>
       </c>
-      <c r="D36" s="45" t="s">
+      <c r="D36" s="44" t="s">
         <v>38</v>
       </c>
-      <c r="E36" s="46" t="s">
+      <c r="E36" s="45" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="37" spans="2:5" s="48" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B37" s="56">
+    <row r="37" spans="2:5" s="47" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B37" s="55">
         <v>22</v>
       </c>
-      <c r="C37" s="57" t="s">
+      <c r="C37" s="56" t="s">
         <v>44</v>
       </c>
-      <c r="D37" s="45" t="s">
+      <c r="D37" s="44" t="s">
         <v>38</v>
       </c>
-      <c r="E37" s="46" t="s">
+      <c r="E37" s="45" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="38" spans="2:5" s="48" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B38" s="56">
+    <row r="38" spans="2:5" s="47" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B38" s="55">
         <v>23</v>
       </c>
-      <c r="C38" s="57" t="s">
+      <c r="C38" s="56" t="s">
         <v>45</v>
       </c>
-      <c r="D38" s="45" t="s">
+      <c r="D38" s="44" t="s">
         <v>38</v>
       </c>
-      <c r="E38" s="46" t="s">
+      <c r="E38" s="45" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="39" spans="2:5" s="48" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B39" s="56">
+    <row r="39" spans="2:5" s="47" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B39" s="55">
         <v>24</v>
       </c>
-      <c r="C39" s="57" t="s">
+      <c r="C39" s="56" t="s">
         <v>46</v>
       </c>
-      <c r="D39" s="45" t="s">
+      <c r="D39" s="44" t="s">
         <v>36</v>
       </c>
-      <c r="E39" s="46" t="s">
+      <c r="E39" s="45" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="40" spans="2:5" s="48" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B40" s="56">
+    <row r="40" spans="2:5" s="47" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B40" s="55">
         <v>25</v>
       </c>
-      <c r="C40" s="57" t="s">
+      <c r="C40" s="56" t="s">
         <v>47</v>
       </c>
-      <c r="D40" s="45" t="s">
+      <c r="D40" s="44" t="s">
         <v>36</v>
       </c>
-      <c r="E40" s="46" t="s">
+      <c r="E40" s="45" t="s">
         <v>265</v>
       </c>
     </row>
@@ -2548,6 +2548,19 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="D6:D7"/>
     <mergeCell ref="E26:E27"/>
     <mergeCell ref="E28:E29"/>
     <mergeCell ref="E12:E13"/>
@@ -2560,19 +2573,6 @@
     <mergeCell ref="E24:E25"/>
     <mergeCell ref="E16:E17"/>
     <mergeCell ref="E14:E15"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="D18:D19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2581,6 +2581,92 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{331241C8-C85E-4C97-B23E-412C2BAA38EA}">
+  <dimension ref="B1:E6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="26.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B1" s="97" t="s">
+        <v>277</v>
+      </c>
+      <c r="C1" s="97"/>
+      <c r="D1" s="97"/>
+      <c r="E1" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B2" s="97" t="s">
+        <v>272</v>
+      </c>
+      <c r="C2" s="97"/>
+      <c r="D2" s="97"/>
+      <c r="E2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B3" s="97" t="s">
+        <v>273</v>
+      </c>
+      <c r="C3" s="97"/>
+      <c r="D3" s="97"/>
+      <c r="E3" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B4" s="97" t="s">
+        <v>274</v>
+      </c>
+      <c r="C4" s="97"/>
+      <c r="D4" s="97"/>
+      <c r="E4" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B5" s="97" t="s">
+        <v>275</v>
+      </c>
+      <c r="C5" s="97"/>
+      <c r="D5" s="97"/>
+      <c r="E5" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B6" s="97" t="s">
+        <v>276</v>
+      </c>
+      <c r="C6" s="97"/>
+      <c r="D6" s="97"/>
+      <c r="E6" t="s">
+        <v>266</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B1:D1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:F16"/>
   <sheetViews>
@@ -2710,93 +2796,93 @@
       </c>
       <c r="F8" s="43"/>
     </row>
-    <row r="9" spans="2:6" s="48" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B9" s="49">
+    <row r="9" spans="2:6" s="47" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="B9" s="48">
         <v>33</v>
       </c>
-      <c r="C9" s="70" t="s">
+      <c r="C9" s="72" t="s">
         <v>61</v>
       </c>
-      <c r="D9" s="50" t="s">
+      <c r="D9" s="49" t="s">
         <v>62</v>
       </c>
-      <c r="E9" s="72" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" s="48" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="51"/>
-      <c r="C10" s="71"/>
-      <c r="D10" s="45" t="s">
+      <c r="E9" s="74" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" s="47" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="50"/>
+      <c r="C10" s="73"/>
+      <c r="D10" s="44" t="s">
         <v>63</v>
       </c>
-      <c r="E10" s="72"/>
-    </row>
-    <row r="11" spans="2:6" s="48" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B11" s="49">
+      <c r="E10" s="74"/>
+    </row>
+    <row r="11" spans="2:6" s="47" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="B11" s="48">
         <v>34</v>
       </c>
-      <c r="C11" s="70" t="s">
+      <c r="C11" s="72" t="s">
         <v>64</v>
       </c>
-      <c r="D11" s="50" t="s">
+      <c r="D11" s="49" t="s">
         <v>65</v>
       </c>
-      <c r="E11" s="72" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" s="48" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="51"/>
-      <c r="C12" s="71"/>
-      <c r="D12" s="45" t="s">
+      <c r="E11" s="74" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" s="47" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="50"/>
+      <c r="C12" s="73"/>
+      <c r="D12" s="44" t="s">
         <v>63</v>
       </c>
-      <c r="E12" s="72"/>
-    </row>
-    <row r="13" spans="2:6" s="48" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B13" s="49">
+      <c r="E12" s="74"/>
+    </row>
+    <row r="13" spans="2:6" s="47" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="B13" s="48">
         <v>35</v>
       </c>
-      <c r="C13" s="70" t="s">
+      <c r="C13" s="72" t="s">
         <v>66</v>
       </c>
-      <c r="D13" s="50" t="s">
+      <c r="D13" s="49" t="s">
         <v>62</v>
       </c>
-      <c r="E13" s="72" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" s="48" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="51"/>
-      <c r="C14" s="71"/>
-      <c r="D14" s="45" t="s">
+      <c r="E13" s="74" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" s="47" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="50"/>
+      <c r="C14" s="73"/>
+      <c r="D14" s="44" t="s">
         <v>67</v>
       </c>
-      <c r="E14" s="72"/>
-    </row>
-    <row r="15" spans="2:6" s="48" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B15" s="49">
+      <c r="E14" s="74"/>
+    </row>
+    <row r="15" spans="2:6" s="47" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="B15" s="48">
         <v>36</v>
       </c>
-      <c r="C15" s="70" t="s">
+      <c r="C15" s="72" t="s">
         <v>68</v>
       </c>
-      <c r="D15" s="50" t="s">
+      <c r="D15" s="49" t="s">
         <v>65</v>
       </c>
-      <c r="E15" s="72" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6" s="48" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="51"/>
-      <c r="C16" s="71"/>
-      <c r="D16" s="45" t="s">
+      <c r="E15" s="74" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" s="47" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="50"/>
+      <c r="C16" s="73"/>
+      <c r="D16" s="44" t="s">
         <v>67</v>
       </c>
-      <c r="E16" s="72"/>
+      <c r="E16" s="74"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -2814,7 +2900,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B2:F80"/>
   <sheetViews>
@@ -2841,315 +2927,315 @@
       </c>
     </row>
     <row r="3" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B3" s="65">
+      <c r="B3" s="68">
         <v>37</v>
       </c>
       <c r="C3" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="65" t="s">
+      <c r="D3" s="68" t="s">
         <v>71</v>
       </c>
-      <c r="E3" s="69" t="s">
+      <c r="E3" s="60" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="4" spans="2:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="61"/>
+      <c r="B4" s="66"/>
       <c r="C4" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="D4" s="61"/>
-      <c r="E4" s="69"/>
+      <c r="D4" s="66"/>
+      <c r="E4" s="60"/>
     </row>
     <row r="5" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B5" s="58">
+      <c r="B5" s="63">
         <v>38</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="58" t="s">
+      <c r="D5" s="63" t="s">
         <v>73</v>
       </c>
-      <c r="E5" s="69" t="s">
+      <c r="E5" s="60" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="6" spans="2:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="59"/>
+      <c r="B6" s="67"/>
       <c r="C6" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="D6" s="59"/>
-      <c r="E6" s="69"/>
+      <c r="D6" s="67"/>
+      <c r="E6" s="60"/>
     </row>
     <row r="7" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B7" s="60">
+      <c r="B7" s="65">
         <v>39</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="60" t="s">
+      <c r="D7" s="65" t="s">
         <v>31</v>
       </c>
-      <c r="E7" s="69" t="s">
+      <c r="E7" s="60" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="8" spans="2:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="61"/>
+      <c r="B8" s="66"/>
       <c r="C8" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="D8" s="61"/>
-      <c r="E8" s="69"/>
+      <c r="D8" s="66"/>
+      <c r="E8" s="60"/>
     </row>
     <row r="9" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B9" s="58">
+      <c r="B9" s="63">
         <v>40</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="D9" s="58" t="s">
+      <c r="D9" s="63" t="s">
         <v>77</v>
       </c>
-      <c r="E9" s="69" t="s">
+      <c r="E9" s="60" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="10" spans="2:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="59"/>
+      <c r="B10" s="67"/>
       <c r="C10" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="D10" s="59"/>
-      <c r="E10" s="69"/>
+      <c r="D10" s="67"/>
+      <c r="E10" s="60"/>
     </row>
     <row r="11" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B11" s="60">
+      <c r="B11" s="65">
         <v>41</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="D11" s="60" t="s">
+      <c r="D11" s="65" t="s">
         <v>80</v>
       </c>
-      <c r="E11" s="69" t="s">
+      <c r="E11" s="60" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="12" spans="2:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="61"/>
+      <c r="B12" s="66"/>
       <c r="C12" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="D12" s="61"/>
-      <c r="E12" s="69"/>
+      <c r="D12" s="66"/>
+      <c r="E12" s="60"/>
     </row>
     <row r="13" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B13" s="58">
+      <c r="B13" s="63">
         <v>42</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="D13" s="58" t="s">
+      <c r="D13" s="63" t="s">
         <v>83</v>
       </c>
-      <c r="E13" s="69" t="s">
+      <c r="E13" s="60" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="14" spans="2:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="59"/>
+      <c r="B14" s="67"/>
       <c r="C14" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="D14" s="59"/>
-      <c r="E14" s="69"/>
+      <c r="D14" s="67"/>
+      <c r="E14" s="60"/>
     </row>
     <row r="15" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B15" s="85">
+      <c r="B15" s="83">
         <v>43</v>
       </c>
       <c r="C15" s="29" t="s">
         <v>84</v>
       </c>
-      <c r="D15" s="85" t="s">
+      <c r="D15" s="83" t="s">
         <v>86</v>
       </c>
-      <c r="E15" s="69" t="s">
+      <c r="E15" s="60" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="16" spans="2:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="76"/>
+      <c r="B16" s="78"/>
       <c r="C16" s="30" t="s">
         <v>85</v>
       </c>
-      <c r="D16" s="76"/>
-      <c r="E16" s="69"/>
-    </row>
-    <row r="17" spans="2:5" s="93" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B17" s="89">
+      <c r="D16" s="78"/>
+      <c r="E16" s="60"/>
+    </row>
+    <row r="17" spans="2:5" s="58" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="B17" s="84">
         <v>44</v>
       </c>
-      <c r="C17" s="90" t="s">
+      <c r="C17" s="57" t="s">
         <v>87</v>
       </c>
-      <c r="D17" s="91">
+      <c r="D17" s="86">
         <v>987654321</v>
       </c>
-      <c r="E17" s="92" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" s="93" customFormat="1" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="94"/>
-      <c r="C18" s="95" t="s">
+      <c r="E17" s="75" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" s="58" customFormat="1" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="85"/>
+      <c r="C18" s="59" t="s">
         <v>88</v>
       </c>
-      <c r="D18" s="96"/>
-      <c r="E18" s="92"/>
+      <c r="D18" s="87"/>
+      <c r="E18" s="75"/>
     </row>
     <row r="19" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B19" s="75">
+      <c r="B19" s="77">
         <v>45</v>
       </c>
       <c r="C19" s="33" t="s">
         <v>89</v>
       </c>
-      <c r="D19" s="75">
+      <c r="D19" s="77">
         <v>1433</v>
       </c>
-      <c r="E19" s="69" t="s">
+      <c r="E19" s="60" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="20" spans="2:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="76"/>
+      <c r="B20" s="78"/>
       <c r="C20" s="30" t="s">
         <v>90</v>
       </c>
-      <c r="D20" s="76"/>
-      <c r="E20" s="69"/>
+      <c r="D20" s="78"/>
+      <c r="E20" s="60"/>
     </row>
     <row r="21" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B21" s="77">
+      <c r="B21" s="79">
         <v>46</v>
       </c>
       <c r="C21" s="31" t="s">
         <v>91</v>
       </c>
-      <c r="D21" s="82">
+      <c r="D21" s="81">
         <v>43925</v>
       </c>
-      <c r="E21" s="86" t="s">
+      <c r="E21" s="76" t="s">
         <v>269</v>
       </c>
     </row>
     <row r="22" spans="2:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="78"/>
+      <c r="B22" s="80"/>
       <c r="C22" s="32" t="s">
         <v>92</v>
       </c>
-      <c r="D22" s="84"/>
-      <c r="E22" s="69"/>
+      <c r="D22" s="82"/>
+      <c r="E22" s="60"/>
     </row>
     <row r="23" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B23" s="75">
+      <c r="B23" s="77">
         <v>47</v>
       </c>
       <c r="C23" s="33" t="s">
         <v>93</v>
       </c>
-      <c r="D23" s="80" t="s">
+      <c r="D23" s="88" t="s">
         <v>7</v>
       </c>
-      <c r="E23" s="86" t="s">
+      <c r="E23" s="76" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="24" spans="2:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="76"/>
+      <c r="B24" s="78"/>
       <c r="C24" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="D24" s="81"/>
-      <c r="E24" s="69"/>
+      <c r="D24" s="89"/>
+      <c r="E24" s="60"/>
     </row>
     <row r="25" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B25" s="77">
+      <c r="B25" s="79">
         <v>48</v>
       </c>
       <c r="C25" s="31" t="s">
         <v>94</v>
       </c>
-      <c r="D25" s="82">
+      <c r="D25" s="81">
         <v>43834</v>
       </c>
-      <c r="E25" s="86" t="s">
+      <c r="E25" s="76" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="26" spans="2:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B26" s="78"/>
+      <c r="B26" s="80"/>
       <c r="C26" s="32" t="s">
         <v>95</v>
       </c>
-      <c r="D26" s="83"/>
-      <c r="E26" s="69"/>
+      <c r="D26" s="90"/>
+      <c r="E26" s="60"/>
     </row>
     <row r="27" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B27" s="75">
+      <c r="B27" s="77">
         <v>49</v>
       </c>
       <c r="C27" s="33" t="s">
         <v>96</v>
       </c>
-      <c r="D27" s="75">
+      <c r="D27" s="77">
         <v>0</v>
       </c>
-      <c r="E27" s="86" t="s">
+      <c r="E27" s="76" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="28" spans="2:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="76"/>
+      <c r="B28" s="78"/>
       <c r="C28" s="30" t="s">
         <v>96</v>
       </c>
-      <c r="D28" s="76"/>
-      <c r="E28" s="69"/>
+      <c r="D28" s="78"/>
+      <c r="E28" s="60"/>
     </row>
     <row r="29" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B29" s="77">
+      <c r="B29" s="79">
         <v>50</v>
       </c>
       <c r="C29" s="31" t="s">
         <v>97</v>
       </c>
-      <c r="D29" s="77">
+      <c r="D29" s="79">
         <v>5</v>
       </c>
-      <c r="E29" s="86" t="s">
+      <c r="E29" s="76" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="30" spans="2:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B30" s="78"/>
+      <c r="B30" s="80"/>
       <c r="C30" s="32" t="s">
         <v>98</v>
       </c>
-      <c r="D30" s="78"/>
-      <c r="E30" s="69"/>
+      <c r="D30" s="80"/>
+      <c r="E30" s="60"/>
     </row>
     <row r="31" spans="2:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="75">
+      <c r="B31" s="77">
         <v>51</v>
       </c>
       <c r="C31" s="33" t="s">
@@ -3158,85 +3244,85 @@
       <c r="D31" s="33" t="s">
         <v>101</v>
       </c>
-      <c r="E31" s="69" t="s">
+      <c r="E31" s="60" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="32" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B32" s="76"/>
+      <c r="B32" s="78"/>
       <c r="C32" s="30" t="s">
         <v>100</v>
       </c>
       <c r="D32" s="34" t="s">
         <v>102</v>
       </c>
-      <c r="E32" s="69"/>
-    </row>
-    <row r="33" spans="2:5" s="48" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B33" s="73">
+      <c r="E32" s="60"/>
+    </row>
+    <row r="33" spans="2:5" s="47" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="B33" s="92">
         <v>52</v>
       </c>
-      <c r="C33" s="54" t="s">
+      <c r="C33" s="53" t="s">
         <v>103</v>
       </c>
-      <c r="D33" s="73" t="s">
+      <c r="D33" s="92" t="s">
         <v>105</v>
       </c>
-      <c r="E33" s="72" t="s">
+      <c r="E33" s="74" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="34" spans="2:5" s="48" customFormat="1" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B34" s="74"/>
-      <c r="C34" s="55" t="s">
+    <row r="34" spans="2:5" s="47" customFormat="1" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B34" s="93"/>
+      <c r="C34" s="54" t="s">
         <v>104</v>
       </c>
-      <c r="D34" s="74"/>
-      <c r="E34" s="72"/>
+      <c r="D34" s="93"/>
+      <c r="E34" s="74"/>
     </row>
     <row r="35" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B35" s="75">
+      <c r="B35" s="77">
         <v>53</v>
       </c>
       <c r="C35" s="33" t="s">
         <v>106</v>
       </c>
-      <c r="D35" s="75" t="s">
+      <c r="D35" s="77" t="s">
         <v>108</v>
       </c>
-      <c r="E35" s="69" t="s">
+      <c r="E35" s="60" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="36" spans="2:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B36" s="76"/>
+      <c r="B36" s="78"/>
       <c r="C36" s="30" t="s">
         <v>107</v>
       </c>
-      <c r="D36" s="76"/>
-      <c r="E36" s="69"/>
+      <c r="D36" s="78"/>
+      <c r="E36" s="60"/>
     </row>
     <row r="37" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B37" s="77">
+      <c r="B37" s="79">
         <v>54</v>
       </c>
       <c r="C37" s="31" t="s">
         <v>109</v>
       </c>
-      <c r="D37" s="77" t="s">
+      <c r="D37" s="79" t="s">
         <v>111</v>
       </c>
-      <c r="E37" s="69" t="s">
+      <c r="E37" s="60" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="38" spans="2:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B38" s="78"/>
+      <c r="B38" s="80"/>
       <c r="C38" s="32" t="s">
         <v>110</v>
       </c>
-      <c r="D38" s="78"/>
-      <c r="E38" s="69"/>
+      <c r="D38" s="80"/>
+      <c r="E38" s="60"/>
     </row>
     <row r="39" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B39" s="34">
@@ -3281,48 +3367,48 @@
       </c>
     </row>
     <row r="42" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="79">
+      <c r="B42" s="91">
         <v>58</v>
       </c>
       <c r="C42" s="37" t="s">
         <v>117</v>
       </c>
-      <c r="D42" s="79" t="s">
+      <c r="D42" s="91" t="s">
         <v>36</v>
       </c>
-      <c r="E42" s="69" t="s">
+      <c r="E42" s="60" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="43" spans="2:5" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B43" s="78"/>
+      <c r="B43" s="80"/>
       <c r="C43" s="32" t="s">
         <v>118</v>
       </c>
-      <c r="D43" s="78"/>
-      <c r="E43" s="69"/>
+      <c r="D43" s="80"/>
+      <c r="E43" s="60"/>
     </row>
     <row r="44" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B44" s="75">
+      <c r="B44" s="77">
         <v>59</v>
       </c>
       <c r="C44" s="33" t="s">
         <v>119</v>
       </c>
-      <c r="D44" s="75" t="s">
+      <c r="D44" s="77" t="s">
         <v>36</v>
       </c>
-      <c r="E44" s="69" t="s">
+      <c r="E44" s="60" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="45" spans="2:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B45" s="76"/>
+      <c r="B45" s="78"/>
       <c r="C45" s="30" t="s">
         <v>120</v>
       </c>
-      <c r="D45" s="76"/>
-      <c r="E45" s="69"/>
+      <c r="D45" s="78"/>
+      <c r="E45" s="60"/>
     </row>
     <row r="46" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B46" s="36">
@@ -3338,17 +3424,17 @@
         <v>266</v>
       </c>
     </row>
-    <row r="47" spans="2:5" s="48" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B47" s="53">
+    <row r="47" spans="2:5" s="47" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B47" s="52">
         <v>61</v>
       </c>
-      <c r="C47" s="53" t="s">
+      <c r="C47" s="52" t="s">
         <v>123</v>
       </c>
-      <c r="D47" s="53" t="s">
+      <c r="D47" s="52" t="s">
         <v>124</v>
       </c>
-      <c r="E47" s="46" t="s">
+      <c r="E47" s="45" t="s">
         <v>266</v>
       </c>
     </row>
@@ -3366,71 +3452,71 @@
         <v>265</v>
       </c>
     </row>
-    <row r="49" spans="2:5" s="48" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B49" s="73">
+    <row r="49" spans="2:5" s="47" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="B49" s="92">
         <v>63</v>
       </c>
-      <c r="C49" s="54" t="s">
+      <c r="C49" s="53" t="s">
         <v>126</v>
       </c>
-      <c r="D49" s="73" t="s">
+      <c r="D49" s="92" t="s">
         <v>128</v>
       </c>
-      <c r="E49" s="72" t="s">
+      <c r="E49" s="74" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="50" spans="2:5" s="48" customFormat="1" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B50" s="74"/>
-      <c r="C50" s="55" t="s">
+    <row r="50" spans="2:5" s="47" customFormat="1" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B50" s="93"/>
+      <c r="C50" s="54" t="s">
         <v>127</v>
       </c>
-      <c r="D50" s="74"/>
-      <c r="E50" s="72"/>
-    </row>
-    <row r="51" spans="2:5" s="48" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B51" s="73">
+      <c r="D50" s="93"/>
+      <c r="E50" s="74"/>
+    </row>
+    <row r="51" spans="2:5" s="47" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="B51" s="92">
         <v>64</v>
       </c>
-      <c r="C51" s="54" t="s">
+      <c r="C51" s="53" t="s">
         <v>129</v>
       </c>
-      <c r="D51" s="73" t="s">
+      <c r="D51" s="92" t="s">
         <v>131</v>
       </c>
-      <c r="E51" s="72" t="s">
+      <c r="E51" s="74" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="52" spans="2:5" s="48" customFormat="1" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B52" s="74"/>
-      <c r="C52" s="55" t="s">
+    <row r="52" spans="2:5" s="47" customFormat="1" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B52" s="93"/>
+      <c r="C52" s="54" t="s">
         <v>130</v>
       </c>
-      <c r="D52" s="74"/>
-      <c r="E52" s="72"/>
-    </row>
-    <row r="53" spans="2:5" s="48" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B53" s="73">
+      <c r="D52" s="93"/>
+      <c r="E52" s="74"/>
+    </row>
+    <row r="53" spans="2:5" s="47" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="B53" s="92">
         <v>65</v>
       </c>
-      <c r="C53" s="54" t="s">
+      <c r="C53" s="53" t="s">
         <v>132</v>
       </c>
-      <c r="D53" s="73" t="s">
+      <c r="D53" s="92" t="s">
         <v>134</v>
       </c>
-      <c r="E53" s="72" t="s">
+      <c r="E53" s="74" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="54" spans="2:5" s="48" customFormat="1" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B54" s="74"/>
-      <c r="C54" s="55" t="s">
+    <row r="54" spans="2:5" s="47" customFormat="1" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B54" s="93"/>
+      <c r="C54" s="54" t="s">
         <v>133</v>
       </c>
-      <c r="D54" s="74"/>
-      <c r="E54" s="72"/>
+      <c r="D54" s="93"/>
+      <c r="E54" s="74"/>
     </row>
     <row r="55" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B55" s="36">
@@ -3698,17 +3784,17 @@
         <v>266</v>
       </c>
     </row>
-    <row r="74" spans="2:5" s="48" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B74" s="45">
+    <row r="74" spans="2:5" s="47" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B74" s="44">
         <v>85</v>
       </c>
-      <c r="C74" s="45" t="s">
+      <c r="C74" s="44" t="s">
         <v>165</v>
       </c>
-      <c r="D74" s="45" t="s">
+      <c r="D74" s="44" t="s">
         <v>166</v>
       </c>
-      <c r="E74" s="46" t="s">
+      <c r="E74" s="45" t="s">
         <v>266</v>
       </c>
     </row>
@@ -3795,6 +3881,58 @@
     </row>
   </sheetData>
   <mergeCells count="68">
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="D51:D52"/>
+    <mergeCell ref="B53:B54"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="D49:D50"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E33:E34"/>
+    <mergeCell ref="E35:E36"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="E31:E32"/>
     <mergeCell ref="E49:E50"/>
     <mergeCell ref="E51:E52"/>
     <mergeCell ref="E53:E54"/>
@@ -3811,64 +3949,12 @@
     <mergeCell ref="E13:E14"/>
     <mergeCell ref="E15:E16"/>
     <mergeCell ref="E21:E22"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="E33:E34"/>
-    <mergeCell ref="E35:E36"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="D42:D43"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="D51:D52"/>
-    <mergeCell ref="B53:B54"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="D44:D45"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="D49:D50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B1:F20"/>
   <sheetViews>
@@ -3893,70 +3979,70 @@
       </c>
     </row>
     <row r="2" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B2" s="65">
+      <c r="B2" s="68">
         <v>92</v>
       </c>
       <c r="C2" s="15" t="s">
         <v>178</v>
       </c>
-      <c r="D2" s="65" t="s">
+      <c r="D2" s="68" t="s">
         <v>36</v>
       </c>
-      <c r="E2" s="69" t="s">
+      <c r="E2" s="60" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="3" spans="2:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="61"/>
+      <c r="B3" s="66"/>
       <c r="C3" s="7" t="s">
         <v>179</v>
       </c>
-      <c r="D3" s="61"/>
-      <c r="E3" s="69"/>
+      <c r="D3" s="66"/>
+      <c r="E3" s="60"/>
     </row>
     <row r="4" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B4" s="58">
+      <c r="B4" s="63">
         <v>93</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="58" t="s">
+      <c r="D4" s="63" t="s">
         <v>71</v>
       </c>
-      <c r="E4" s="69" t="s">
+      <c r="E4" s="60" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="5" spans="2:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="59"/>
+      <c r="B5" s="67"/>
       <c r="C5" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="D5" s="59"/>
-      <c r="E5" s="69"/>
+      <c r="D5" s="67"/>
+      <c r="E5" s="60"/>
     </row>
     <row r="6" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B6" s="60">
+      <c r="B6" s="65">
         <v>94</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="60" t="s">
+      <c r="D6" s="65" t="s">
         <v>182</v>
       </c>
-      <c r="E6" s="69" t="s">
+      <c r="E6" s="60" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="7" spans="2:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="61"/>
+      <c r="B7" s="66"/>
       <c r="C7" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="D7" s="61"/>
-      <c r="E7" s="69"/>
+      <c r="D7" s="66"/>
+      <c r="E7" s="60"/>
     </row>
     <row r="8" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="4">
@@ -4000,32 +4086,32 @@
         <v>266</v>
       </c>
     </row>
-    <row r="11" spans="2:6" s="48" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="45">
+    <row r="11" spans="2:6" s="47" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="44">
         <v>98</v>
       </c>
-      <c r="C11" s="45" t="s">
+      <c r="C11" s="44" t="s">
         <v>188</v>
       </c>
-      <c r="D11" s="45" t="s">
+      <c r="D11" s="44" t="s">
         <v>189</v>
       </c>
-      <c r="E11" s="46" t="s">
-        <v>266</v>
-      </c>
-      <c r="F11" s="47"/>
+      <c r="E11" s="45" t="s">
+        <v>266</v>
+      </c>
+      <c r="F11" s="46"/>
     </row>
     <row r="12" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B12" s="88">
+      <c r="B12" s="94">
         <v>99</v>
       </c>
-      <c r="C12" s="88" t="s">
+      <c r="C12" s="94" t="s">
         <v>190</v>
       </c>
       <c r="D12" s="27" t="s">
         <v>191</v>
       </c>
-      <c r="E12" s="69" t="s">
+      <c r="E12" s="60" t="s">
         <v>266</v>
       </c>
     </row>
@@ -4035,7 +4121,7 @@
       <c r="D13" s="8" t="s">
         <v>192</v>
       </c>
-      <c r="E13" s="69"/>
+      <c r="E13" s="60"/>
     </row>
     <row r="14" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B14" s="64"/>
@@ -4043,7 +4129,7 @@
       <c r="D14" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="E14" s="69"/>
+      <c r="E14" s="60"/>
     </row>
     <row r="15" spans="2:6" ht="50.4" x14ac:dyDescent="0.3">
       <c r="B15" s="64"/>
@@ -4051,15 +4137,15 @@
       <c r="D15" s="8" t="s">
         <v>194</v>
       </c>
-      <c r="E15" s="69"/>
+      <c r="E15" s="60"/>
     </row>
     <row r="16" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="59"/>
-      <c r="C16" s="59"/>
+      <c r="B16" s="67"/>
+      <c r="C16" s="67"/>
       <c r="D16" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="E16" s="69"/>
+      <c r="E16" s="60"/>
     </row>
     <row r="17" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="2">
@@ -4076,16 +4162,16 @@
       </c>
     </row>
     <row r="18" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B18" s="58">
+      <c r="B18" s="63">
         <v>101</v>
       </c>
-      <c r="C18" s="58" t="s">
+      <c r="C18" s="63" t="s">
         <v>198</v>
       </c>
       <c r="D18" s="8" t="s">
         <v>199</v>
       </c>
-      <c r="E18" s="69" t="s">
+      <c r="E18" s="60" t="s">
         <v>266</v>
       </c>
     </row>
@@ -4095,23 +4181,18 @@
       <c r="D19" s="8" t="s">
         <v>200</v>
       </c>
-      <c r="E19" s="69"/>
+      <c r="E19" s="60"/>
     </row>
     <row r="20" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="59"/>
-      <c r="C20" s="59"/>
+      <c r="B20" s="67"/>
+      <c r="C20" s="67"/>
       <c r="D20" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="E20" s="69"/>
+      <c r="E20" s="60"/>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="E12:E16"/>
-    <mergeCell ref="E18:E20"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="B4:B5"/>
@@ -4122,12 +4203,17 @@
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="B12:B16"/>
     <mergeCell ref="C12:C16"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="E12:E16"/>
+    <mergeCell ref="E18:E20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B1:F31"/>
   <sheetViews>
@@ -4152,70 +4238,70 @@
       </c>
     </row>
     <row r="2" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B2" s="65">
+      <c r="B2" s="68">
         <v>102</v>
       </c>
       <c r="C2" s="15" t="s">
         <v>178</v>
       </c>
-      <c r="D2" s="65" t="s">
+      <c r="D2" s="68" t="s">
         <v>36</v>
       </c>
-      <c r="E2" s="69" t="s">
+      <c r="E2" s="60" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="3" spans="2:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="61"/>
+      <c r="B3" s="66"/>
       <c r="C3" s="7" t="s">
         <v>179</v>
       </c>
-      <c r="D3" s="61"/>
-      <c r="E3" s="69"/>
+      <c r="D3" s="66"/>
+      <c r="E3" s="60"/>
     </row>
     <row r="4" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B4" s="58">
+      <c r="B4" s="63">
         <v>103</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>202</v>
       </c>
-      <c r="D4" s="58" t="s">
+      <c r="D4" s="63" t="s">
         <v>71</v>
       </c>
-      <c r="E4" s="69" t="s">
+      <c r="E4" s="60" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="5" spans="2:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="59"/>
+      <c r="B5" s="67"/>
       <c r="C5" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="D5" s="59"/>
-      <c r="E5" s="69"/>
+      <c r="D5" s="67"/>
+      <c r="E5" s="60"/>
     </row>
     <row r="6" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B6" s="60">
+      <c r="B6" s="65">
         <v>104</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="60" t="s">
+      <c r="D6" s="65" t="s">
         <v>182</v>
       </c>
-      <c r="E6" s="69" t="s">
+      <c r="E6" s="60" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="7" spans="2:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="61"/>
+      <c r="B7" s="66"/>
       <c r="C7" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="D7" s="61"/>
-      <c r="E7" s="69"/>
+      <c r="D7" s="66"/>
+      <c r="E7" s="60"/>
     </row>
     <row r="8" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="4">
@@ -4273,45 +4359,45 @@
         <v>271</v>
       </c>
     </row>
-    <row r="12" spans="2:6" s="48" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="45">
+    <row r="12" spans="2:6" s="47" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="44">
         <v>109</v>
       </c>
-      <c r="C12" s="45" t="s">
+      <c r="C12" s="44" t="s">
         <v>210</v>
       </c>
-      <c r="D12" s="45" t="s">
+      <c r="D12" s="44" t="s">
         <v>211</v>
       </c>
-      <c r="E12" s="46" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" s="48" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="45">
+      <c r="E12" s="45" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" s="47" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="44">
         <v>110</v>
       </c>
-      <c r="C13" s="45" t="s">
+      <c r="C13" s="44" t="s">
         <v>212</v>
       </c>
-      <c r="D13" s="45" t="s">
+      <c r="D13" s="44" t="s">
         <v>213</v>
       </c>
-      <c r="E13" s="46" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" s="48" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="45">
+      <c r="E13" s="45" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" s="47" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="44">
         <v>111</v>
       </c>
-      <c r="C14" s="45" t="s">
+      <c r="C14" s="44" t="s">
         <v>214</v>
       </c>
-      <c r="D14" s="45">
+      <c r="D14" s="44">
         <v>0</v>
       </c>
-      <c r="E14" s="46" t="s">
+      <c r="E14" s="45" t="s">
         <v>266</v>
       </c>
     </row>
@@ -4343,17 +4429,17 @@
         <v>266</v>
       </c>
     </row>
-    <row r="17" spans="2:5" s="48" customFormat="1" ht="34.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="45">
+    <row r="17" spans="2:5" s="47" customFormat="1" ht="34.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="44">
         <v>114</v>
       </c>
-      <c r="C17" s="45" t="s">
+      <c r="C17" s="44" t="s">
         <v>217</v>
       </c>
-      <c r="D17" s="45" t="s">
+      <c r="D17" s="44" t="s">
         <v>218</v>
       </c>
-      <c r="E17" s="46" t="s">
+      <c r="E17" s="45" t="s">
         <v>266</v>
       </c>
     </row>
@@ -4371,39 +4457,39 @@
         <v>266</v>
       </c>
     </row>
-    <row r="19" spans="2:5" s="48" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="45">
+    <row r="19" spans="2:5" s="47" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B19" s="44">
         <v>116</v>
       </c>
-      <c r="C19" s="45" t="s">
+      <c r="C19" s="44" t="s">
         <v>221</v>
       </c>
-      <c r="D19" s="45" t="s">
+      <c r="D19" s="44" t="s">
         <v>222</v>
       </c>
-      <c r="E19" s="46" t="s">
+      <c r="E19" s="45" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="20" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B20" s="58">
+      <c r="B20" s="63">
         <v>117</v>
       </c>
       <c r="C20" s="8" t="s">
         <v>223</v>
       </c>
-      <c r="D20" s="58" t="s">
+      <c r="D20" s="63" t="s">
         <v>56</v>
       </c>
-      <c r="E20" s="69"/>
+      <c r="E20" s="60"/>
     </row>
     <row r="21" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="59"/>
+      <c r="B21" s="67"/>
       <c r="C21" s="4" t="s">
         <v>224</v>
       </c>
-      <c r="D21" s="59"/>
-      <c r="E21" s="69"/>
+      <c r="D21" s="67"/>
+      <c r="E21" s="60"/>
     </row>
     <row r="22" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B22" s="2">
@@ -4515,13 +4601,13 @@
       </c>
     </row>
     <row r="30" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B30" s="60">
+      <c r="B30" s="65">
         <v>126</v>
       </c>
       <c r="C30" s="6" t="s">
         <v>267</v>
       </c>
-      <c r="D30" s="60" t="s">
+      <c r="D30" s="65" t="s">
         <v>241</v>
       </c>
       <c r="E30" s="39" t="s">
@@ -4529,12 +4615,18 @@
       </c>
     </row>
     <row r="31" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B31" s="61"/>
+      <c r="B31" s="66"/>
       <c r="C31" s="2"/>
-      <c r="D31" s="61"/>
+      <c r="D31" s="66"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="D20:D21"/>
     <mergeCell ref="E20:E21"/>
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="E4:E5"/>
@@ -4543,23 +4635,17 @@
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="D4:D5"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="D20:D21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="B1:F12"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
updated ssas, ssrs, sql server, diagnostic files for output object and params changes to support the windows and user pwd
</commit_message>
<xml_diff>
--- a/Checklist.xlsx
+++ b/Checklist.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Prashant\AziraPowershellscript\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MO\Powershell\Project\AziraPowershellscript2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C77E1A7-F7C0-42AE-AB50-F1755C18966A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" firstSheet="3" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Application" sheetId="1" r:id="rId1"/>
@@ -21,7 +20,7 @@
     <sheet name="SSRS Configuration" sheetId="4" r:id="rId6"/>
     <sheet name="SQL Server Diagnostics" sheetId="5" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1048,7 +1047,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1106,7 +1105,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1151,6 +1150,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1360,7 +1365,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1639,6 +1644,27 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1679,7 +1705,7 @@
         <xdr:cNvPr id="14" name="Picture 92361">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000E000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1740,7 +1766,7 @@
         <xdr:cNvPr id="15" name="Picture 92362">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000F000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2048,7 +2074,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2056,16 +2082,16 @@
       <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="51" customWidth="1"/>
-    <col min="4" max="4" width="74.44140625" customWidth="1"/>
-    <col min="5" max="5" width="9.109375" style="39"/>
-    <col min="6" max="6" width="11.44140625" customWidth="1"/>
+    <col min="4" max="4" width="74.42578125" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="39"/>
+    <col min="6" max="6" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="38" t="s">
         <v>264</v>
       </c>
@@ -2082,14 +2108,14 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="68" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="69"/>
       <c r="D2" s="69"/>
     </row>
-    <row r="3" spans="1:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="12">
         <v>1</v>
       </c>
@@ -2103,7 +2129,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="10">
         <v>2</v>
       </c>
@@ -2117,14 +2143,14 @@
         <v>266</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="73" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="74"/>
       <c r="D5" s="74"/>
     </row>
-    <row r="6" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B6" s="13">
         <v>3</v>
       </c>
@@ -2138,7 +2164,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="1"/>
       <c r="C7" s="7" t="s">
         <v>6</v>
@@ -2146,7 +2172,7 @@
       <c r="D7" s="67"/>
       <c r="E7" s="75"/>
     </row>
-    <row r="8" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A8" s="51"/>
       <c r="B8" s="11">
         <v>4</v>
@@ -2159,7 +2185,7 @@
       </c>
       <c r="E8" s="75"/>
     </row>
-    <row r="9" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="51"/>
       <c r="B9" s="1"/>
       <c r="C9" s="9" t="s">
@@ -2168,7 +2194,7 @@
       <c r="D9" s="63"/>
       <c r="E9" s="75"/>
     </row>
-    <row r="10" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B10" s="13">
         <v>5</v>
       </c>
@@ -2182,7 +2208,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="5"/>
       <c r="C11" s="16" t="s">
         <v>261</v>
@@ -2190,7 +2216,7 @@
       <c r="D11" s="72"/>
       <c r="E11" s="75"/>
     </row>
-    <row r="12" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B12" s="11">
         <v>6</v>
       </c>
@@ -2204,7 +2230,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="5"/>
       <c r="C13" s="17" t="s">
         <v>261</v>
@@ -2212,7 +2238,7 @@
       <c r="D13" s="70"/>
       <c r="E13" s="75"/>
     </row>
-    <row r="14" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B14" s="11">
         <v>7</v>
       </c>
@@ -2226,7 +2252,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="1"/>
       <c r="C15" s="7" t="s">
         <v>13</v>
@@ -2234,7 +2260,7 @@
       <c r="D15" s="67"/>
       <c r="E15" s="75"/>
     </row>
-    <row r="16" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B16" s="11">
         <v>8</v>
       </c>
@@ -2248,7 +2274,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="17" spans="2:5" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="1"/>
       <c r="C17" s="9" t="s">
         <v>16</v>
@@ -2256,7 +2282,7 @@
       <c r="D17" s="63"/>
       <c r="E17" s="75"/>
     </row>
-    <row r="18" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B18" s="11">
         <v>9</v>
       </c>
@@ -2270,7 +2296,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="19" spans="2:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="1"/>
       <c r="C19" s="7" t="s">
         <v>19</v>
@@ -2278,7 +2304,7 @@
       <c r="D19" s="67"/>
       <c r="E19" s="75"/>
     </row>
-    <row r="20" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="1">
         <v>10</v>
       </c>
@@ -2292,7 +2318,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="21" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C21" s="19" t="s">
         <v>22</v>
       </c>
@@ -2301,7 +2327,7 @@
       </c>
       <c r="E21" s="75"/>
     </row>
-    <row r="22" spans="2:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="11">
         <v>11</v>
       </c>
@@ -2315,7 +2341,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="23" spans="2:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="1"/>
       <c r="C23" s="9" t="s">
         <v>24</v>
@@ -2323,7 +2349,7 @@
       <c r="D23" s="63"/>
       <c r="E23" s="75"/>
     </row>
-    <row r="24" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B24" s="11">
         <v>12</v>
       </c>
@@ -2337,7 +2363,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="25" spans="2:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="1"/>
       <c r="C25" s="7" t="s">
         <v>27</v>
@@ -2345,7 +2371,7 @@
       <c r="D25" s="67"/>
       <c r="E25" s="75"/>
     </row>
-    <row r="26" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B26" s="11">
         <v>13</v>
       </c>
@@ -2359,7 +2385,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="27" spans="2:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="1"/>
       <c r="C27" s="9" t="s">
         <v>30</v>
@@ -2367,7 +2393,7 @@
       <c r="D27" s="63"/>
       <c r="E27" s="75"/>
     </row>
-    <row r="28" spans="2:5" s="47" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:5" s="47" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="60">
         <v>14</v>
       </c>
@@ -2381,7 +2407,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="29" spans="2:5" s="47" customFormat="1" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:5" s="47" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B29" s="55"/>
       <c r="C29" s="61" t="s">
         <v>33</v>
@@ -2389,7 +2415,7 @@
       <c r="D29" s="65"/>
       <c r="E29" s="76"/>
     </row>
-    <row r="30" spans="2:5" ht="32.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:5" ht="31.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B30" s="20">
         <v>15</v>
       </c>
@@ -2400,7 +2426,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="31" spans="2:5" s="47" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:5" s="47" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B31" s="55">
         <v>16</v>
       </c>
@@ -2414,7 +2440,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="32" spans="2:5" s="47" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:5" s="47" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="55">
         <v>17</v>
       </c>
@@ -2428,7 +2454,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="33" spans="2:5" s="47" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:5" s="47" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="55">
         <v>18</v>
       </c>
@@ -2442,7 +2468,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="34" spans="2:5" s="47" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:5" s="47" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B34" s="55">
         <v>19</v>
       </c>
@@ -2456,7 +2482,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="35" spans="2:5" s="47" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:5" s="47" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B35" s="55">
         <v>20</v>
       </c>
@@ -2470,7 +2496,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="36" spans="2:5" s="47" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:5" s="47" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="55">
         <v>21</v>
       </c>
@@ -2484,7 +2510,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="37" spans="2:5" s="47" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:5" s="47" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="55">
         <v>22</v>
       </c>
@@ -2498,7 +2524,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="38" spans="2:5" s="47" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:5" s="47" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B38" s="55">
         <v>23</v>
       </c>
@@ -2512,7 +2538,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="39" spans="2:5" s="47" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:5" s="47" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B39" s="55">
         <v>24</v>
       </c>
@@ -2526,7 +2552,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="40" spans="2:5" s="47" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:5" s="47" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B40" s="55">
         <v>25</v>
       </c>
@@ -2540,7 +2566,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="41" spans="2:5" s="25" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:5" s="25" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="C41" s="26" t="s">
         <v>69</v>
       </c>
@@ -2581,19 +2607,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{331241C8-C85E-4C97-B23E-412C2BAA38EA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="26.109375" customWidth="1"/>
+    <col min="2" max="2" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B1" s="77" t="s">
         <v>277</v>
       </c>
@@ -2603,7 +2629,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2" s="77" t="s">
         <v>272</v>
       </c>
@@ -2613,7 +2639,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" s="77" t="s">
         <v>273</v>
       </c>
@@ -2623,7 +2649,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="77" t="s">
         <v>274</v>
       </c>
@@ -2633,7 +2659,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="77" t="s">
         <v>275</v>
       </c>
@@ -2643,7 +2669,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" s="77" t="s">
         <v>276</v>
       </c>
@@ -2655,35 +2681,35 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="B6:D6"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="B4:D4"/>
     <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B6:D6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11:C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="3.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="47.44140625" customWidth="1"/>
-    <col min="4" max="4" width="93.33203125" customWidth="1"/>
-    <col min="5" max="5" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="35.6640625" customWidth="1"/>
+    <col min="2" max="2" width="3.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="47.42578125" customWidth="1"/>
+    <col min="4" max="4" width="93.28515625" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E1" s="42" t="s">
         <v>48</v>
       </c>
@@ -2691,7 +2717,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="2" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="24">
         <v>26</v>
       </c>
@@ -2706,7 +2732,7 @@
       </c>
       <c r="F2" s="43"/>
     </row>
-    <row r="3" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:6" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="4">
         <v>27</v>
       </c>
@@ -2721,7 +2747,7 @@
       </c>
       <c r="F3" s="43"/>
     </row>
-    <row r="4" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="2">
         <v>28</v>
       </c>
@@ -2736,7 +2762,7 @@
       </c>
       <c r="F4" s="43"/>
     </row>
-    <row r="5" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="4">
         <v>29</v>
       </c>
@@ -2751,7 +2777,7 @@
       </c>
       <c r="F5" s="43"/>
     </row>
-    <row r="6" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="24">
         <v>30</v>
       </c>
@@ -2766,7 +2792,7 @@
       </c>
       <c r="F6" s="43"/>
     </row>
-    <row r="7" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="4">
         <v>31</v>
       </c>
@@ -2781,7 +2807,7 @@
       </c>
       <c r="F7" s="43"/>
     </row>
-    <row r="8" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="2">
         <v>32</v>
       </c>
@@ -2796,7 +2822,7 @@
       </c>
       <c r="F8" s="43"/>
     </row>
-    <row r="9" spans="2:6" s="47" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:6" s="47" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B9" s="48">
         <v>33</v>
       </c>
@@ -2810,7 +2836,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="10" spans="2:6" s="47" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:6" s="47" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="50"/>
       <c r="C10" s="65"/>
       <c r="D10" s="44" t="s">
@@ -2818,7 +2844,7 @@
       </c>
       <c r="E10" s="76"/>
     </row>
-    <row r="11" spans="2:6" s="47" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:6" s="47" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B11" s="48">
         <v>34</v>
       </c>
@@ -2832,7 +2858,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="12" spans="2:6" s="47" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:6" s="47" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="50"/>
       <c r="C12" s="65"/>
       <c r="D12" s="44" t="s">
@@ -2840,7 +2866,7 @@
       </c>
       <c r="E12" s="76"/>
     </row>
-    <row r="13" spans="2:6" s="47" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:6" s="47" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B13" s="48">
         <v>35</v>
       </c>
@@ -2854,7 +2880,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="14" spans="2:6" s="47" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:6" s="47" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="50"/>
       <c r="C14" s="65"/>
       <c r="D14" s="44" t="s">
@@ -2862,7 +2888,7 @@
       </c>
       <c r="E14" s="76"/>
     </row>
-    <row r="15" spans="2:6" s="47" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:6" s="47" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B15" s="48">
         <v>36</v>
       </c>
@@ -2876,7 +2902,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="16" spans="2:6" s="47" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:6" s="47" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="50"/>
       <c r="C16" s="65"/>
       <c r="D16" s="44" t="s">
@@ -2901,21 +2927,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F80"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C17" sqref="A17:XFD18"/>
+    <sheetView topLeftCell="B61" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29:D30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="56" customWidth="1"/>
-    <col min="4" max="4" width="108.33203125" customWidth="1"/>
-    <col min="5" max="5" width="9.109375" style="39"/>
+    <col min="4" max="4" width="108.28515625" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="39"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>177</v>
       </c>
@@ -2926,7 +2952,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="3" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B3" s="71">
         <v>37</v>
       </c>
@@ -2940,7 +2966,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="4" spans="2:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="67"/>
       <c r="C4" s="7" t="s">
         <v>70</v>
@@ -2948,7 +2974,7 @@
       <c r="D4" s="67"/>
       <c r="E4" s="75"/>
     </row>
-    <row r="5" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B5" s="62">
         <v>38</v>
       </c>
@@ -2962,7 +2988,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="6" spans="2:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="63"/>
       <c r="C6" s="9" t="s">
         <v>72</v>
@@ -2970,7 +2996,7 @@
       <c r="D6" s="63"/>
       <c r="E6" s="75"/>
     </row>
-    <row r="7" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B7" s="66">
         <v>39</v>
       </c>
@@ -2984,7 +3010,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="8" spans="2:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="67"/>
       <c r="C8" s="7" t="s">
         <v>74</v>
@@ -2992,7 +3018,7 @@
       <c r="D8" s="67"/>
       <c r="E8" s="75"/>
     </row>
-    <row r="9" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B9" s="62">
         <v>40</v>
       </c>
@@ -3006,7 +3032,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="10" spans="2:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="63"/>
       <c r="C10" s="9" t="s">
         <v>76</v>
@@ -3014,7 +3040,7 @@
       <c r="D10" s="63"/>
       <c r="E10" s="75"/>
     </row>
-    <row r="11" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B11" s="66">
         <v>41</v>
       </c>
@@ -3028,7 +3054,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="12" spans="2:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="67"/>
       <c r="C12" s="7" t="s">
         <v>79</v>
@@ -3036,7 +3062,7 @@
       <c r="D12" s="67"/>
       <c r="E12" s="75"/>
     </row>
-    <row r="13" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B13" s="62">
         <v>42</v>
       </c>
@@ -3050,7 +3076,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="14" spans="2:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="63"/>
       <c r="C14" s="9" t="s">
         <v>82</v>
@@ -3058,7 +3084,7 @@
       <c r="D14" s="63"/>
       <c r="E14" s="75"/>
     </row>
-    <row r="15" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B15" s="90">
         <v>43</v>
       </c>
@@ -3072,7 +3098,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="16" spans="2:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="81"/>
       <c r="C16" s="30" t="s">
         <v>85</v>
@@ -3080,7 +3106,7 @@
       <c r="D16" s="81"/>
       <c r="E16" s="75"/>
     </row>
-    <row r="17" spans="2:5" s="58" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:5" s="58" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B17" s="91">
         <v>44</v>
       </c>
@@ -3094,7 +3120,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="18" spans="2:5" s="58" customFormat="1" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:5" s="58" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="92"/>
       <c r="C18" s="59" t="s">
         <v>88</v>
@@ -3102,7 +3128,7 @@
       <c r="D18" s="94"/>
       <c r="E18" s="96"/>
     </row>
-    <row r="19" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B19" s="80">
         <v>45</v>
       </c>
@@ -3116,7 +3142,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="20" spans="2:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="81"/>
       <c r="C20" s="30" t="s">
         <v>90</v>
@@ -3124,7 +3150,7 @@
       <c r="D20" s="81"/>
       <c r="E20" s="75"/>
     </row>
-    <row r="21" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B21" s="82">
         <v>46</v>
       </c>
@@ -3138,7 +3164,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="22" spans="2:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="83"/>
       <c r="C22" s="32" t="s">
         <v>92</v>
@@ -3146,7 +3172,7 @@
       <c r="D22" s="89"/>
       <c r="E22" s="75"/>
     </row>
-    <row r="23" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B23" s="80">
         <v>47</v>
       </c>
@@ -3160,7 +3186,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="24" spans="2:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="81"/>
       <c r="C24" s="30" t="s">
         <v>6</v>
@@ -3168,7 +3194,7 @@
       <c r="D24" s="86"/>
       <c r="E24" s="75"/>
     </row>
-    <row r="25" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B25" s="82">
         <v>48</v>
       </c>
@@ -3182,7 +3208,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="26" spans="2:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="83"/>
       <c r="C26" s="32" t="s">
         <v>95</v>
@@ -3190,7 +3216,7 @@
       <c r="D26" s="88"/>
       <c r="E26" s="75"/>
     </row>
-    <row r="27" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B27" s="80">
         <v>49</v>
       </c>
@@ -3204,7 +3230,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="28" spans="2:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="81"/>
       <c r="C28" s="30" t="s">
         <v>96</v>
@@ -3212,7 +3238,7 @@
       <c r="D28" s="81"/>
       <c r="E28" s="75"/>
     </row>
-    <row r="29" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B29" s="82">
         <v>50</v>
       </c>
@@ -3226,7 +3252,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="30" spans="2:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B30" s="83"/>
       <c r="C30" s="32" t="s">
         <v>98</v>
@@ -3234,7 +3260,7 @@
       <c r="D30" s="83"/>
       <c r="E30" s="75"/>
     </row>
-    <row r="31" spans="2:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="80">
         <v>51</v>
       </c>
@@ -3248,7 +3274,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="32" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="81"/>
       <c r="C32" s="30" t="s">
         <v>100</v>
@@ -3258,7 +3284,7 @@
       </c>
       <c r="E32" s="75"/>
     </row>
-    <row r="33" spans="2:5" s="47" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:5" s="47" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B33" s="78">
         <v>52</v>
       </c>
@@ -3272,7 +3298,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="34" spans="2:5" s="47" customFormat="1" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:5" s="47" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B34" s="79"/>
       <c r="C34" s="54" t="s">
         <v>104</v>
@@ -3280,7 +3306,7 @@
       <c r="D34" s="79"/>
       <c r="E34" s="76"/>
     </row>
-    <row r="35" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B35" s="80">
         <v>53</v>
       </c>
@@ -3294,7 +3320,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="36" spans="2:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="81"/>
       <c r="C36" s="30" t="s">
         <v>107</v>
@@ -3302,7 +3328,7 @@
       <c r="D36" s="81"/>
       <c r="E36" s="75"/>
     </row>
-    <row r="37" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B37" s="82">
         <v>54</v>
       </c>
@@ -3316,7 +3342,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="38" spans="2:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B38" s="83"/>
       <c r="C38" s="32" t="s">
         <v>110</v>
@@ -3324,7 +3350,7 @@
       <c r="D38" s="83"/>
       <c r="E38" s="75"/>
     </row>
-    <row r="39" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B39" s="34">
         <v>55</v>
       </c>
@@ -3338,7 +3364,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="40" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B40" s="36">
         <v>56</v>
       </c>
@@ -3352,7 +3378,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="41" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B41" s="34">
         <v>57</v>
       </c>
@@ -3366,7 +3392,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="42" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="84">
         <v>58</v>
       </c>
@@ -3380,7 +3406,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="43" spans="2:5" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:5" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B43" s="83"/>
       <c r="C43" s="32" t="s">
         <v>118</v>
@@ -3388,7 +3414,7 @@
       <c r="D43" s="83"/>
       <c r="E43" s="75"/>
     </row>
-    <row r="44" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B44" s="80">
         <v>59</v>
       </c>
@@ -3402,7 +3428,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="45" spans="2:5" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B45" s="81"/>
       <c r="C45" s="30" t="s">
         <v>120</v>
@@ -3410,7 +3436,7 @@
       <c r="D45" s="81"/>
       <c r="E45" s="75"/>
     </row>
-    <row r="46" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B46" s="36">
         <v>60</v>
       </c>
@@ -3424,7 +3450,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="47" spans="2:5" s="47" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:5" s="47" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B47" s="52">
         <v>61</v>
       </c>
@@ -3438,7 +3464,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="48" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B48" s="36">
         <v>62</v>
       </c>
@@ -3452,7 +3478,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="49" spans="2:5" s="47" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:5" s="47" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B49" s="78">
         <v>63</v>
       </c>
@@ -3466,7 +3492,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="50" spans="2:5" s="47" customFormat="1" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:5" s="47" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B50" s="79"/>
       <c r="C50" s="54" t="s">
         <v>127</v>
@@ -3474,7 +3500,7 @@
       <c r="D50" s="79"/>
       <c r="E50" s="76"/>
     </row>
-    <row r="51" spans="2:5" s="47" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:5" s="47" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B51" s="78">
         <v>64</v>
       </c>
@@ -3488,7 +3514,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="52" spans="2:5" s="47" customFormat="1" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:5" s="47" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B52" s="79"/>
       <c r="C52" s="54" t="s">
         <v>130</v>
@@ -3496,7 +3522,7 @@
       <c r="D52" s="79"/>
       <c r="E52" s="76"/>
     </row>
-    <row r="53" spans="2:5" s="47" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:5" s="47" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B53" s="78">
         <v>65</v>
       </c>
@@ -3510,7 +3536,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="54" spans="2:5" s="47" customFormat="1" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:5" s="47" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B54" s="79"/>
       <c r="C54" s="54" t="s">
         <v>133</v>
@@ -3518,7 +3544,7 @@
       <c r="D54" s="79"/>
       <c r="E54" s="76"/>
     </row>
-    <row r="55" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B55" s="36">
         <v>66</v>
       </c>
@@ -3532,7 +3558,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="56" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B56" s="34">
         <v>67</v>
       </c>
@@ -3546,7 +3572,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="57" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B57" s="36">
         <v>68</v>
       </c>
@@ -3560,7 +3586,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="58" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B58" s="34">
         <v>69</v>
       </c>
@@ -3574,7 +3600,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="59" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B59" s="36">
         <v>70</v>
       </c>
@@ -3588,7 +3614,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="60" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B60" s="34">
         <v>71</v>
       </c>
@@ -3602,7 +3628,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="61" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B61" s="36">
         <v>72</v>
       </c>
@@ -3616,7 +3642,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="62" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B62" s="34">
         <v>73</v>
       </c>
@@ -3630,7 +3656,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="63" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B63" s="36">
         <v>74</v>
       </c>
@@ -3644,7 +3670,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="64" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B64" s="24">
         <v>75</v>
       </c>
@@ -3658,7 +3684,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="65" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B65" s="4">
         <v>76</v>
       </c>
@@ -3672,7 +3698,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="66" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B66" s="2">
         <v>77</v>
       </c>
@@ -3686,7 +3712,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="67" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B67" s="2">
         <v>78</v>
       </c>
@@ -3700,7 +3726,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="68" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B68" s="4">
         <v>79</v>
       </c>
@@ -3714,7 +3740,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="69" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B69" s="2">
         <v>80</v>
       </c>
@@ -3728,7 +3754,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="70" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B70" s="4">
         <v>81</v>
       </c>
@@ -3742,7 +3768,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="71" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B71" s="2">
         <v>82</v>
       </c>
@@ -3756,7 +3782,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="72" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B72" s="4">
         <v>83</v>
       </c>
@@ -3770,7 +3796,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="73" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B73" s="2">
         <v>84</v>
       </c>
@@ -3784,7 +3810,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="74" spans="2:5" s="47" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="2:5" s="47" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B74" s="44">
         <v>85</v>
       </c>
@@ -3798,7 +3824,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="75" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B75" s="2">
         <v>86</v>
       </c>
@@ -3812,7 +3838,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="76" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B76" s="4">
         <v>87</v>
       </c>
@@ -3826,7 +3852,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="77" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B77" s="2">
         <v>88</v>
       </c>
@@ -3840,7 +3866,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="78" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B78" s="4">
         <v>89</v>
       </c>
@@ -3854,7 +3880,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="79" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B79" s="2">
         <v>90</v>
       </c>
@@ -3865,7 +3891,7 @@
         <v>43178</v>
       </c>
     </row>
-    <row r="80" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B80" s="4">
         <v>91</v>
       </c>
@@ -3955,22 +3981,22 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F20"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="7.88671875" customWidth="1"/>
-    <col min="3" max="3" width="56.88671875" customWidth="1"/>
+    <col min="2" max="2" width="7.85546875" customWidth="1"/>
+    <col min="3" max="3" width="56.85546875" customWidth="1"/>
     <col min="4" max="4" width="100" customWidth="1"/>
-    <col min="5" max="5" width="9.109375" style="39"/>
+    <col min="5" max="5" width="9.140625" style="39"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E1" s="39" t="s">
         <v>259</v>
       </c>
@@ -3978,7 +4004,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="2" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B2" s="71">
         <v>92</v>
       </c>
@@ -3992,7 +4018,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="3" spans="2:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="67"/>
       <c r="C3" s="7" t="s">
         <v>179</v>
@@ -4000,11 +4026,11 @@
       <c r="D3" s="67"/>
       <c r="E3" s="75"/>
     </row>
-    <row r="4" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B4" s="62">
         <v>93</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="98" t="s">
         <v>12</v>
       </c>
       <c r="D4" s="62" t="s">
@@ -4014,7 +4040,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="5" spans="2:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="63"/>
       <c r="C5" s="9" t="s">
         <v>180</v>
@@ -4022,11 +4048,11 @@
       <c r="D5" s="63"/>
       <c r="E5" s="75"/>
     </row>
-    <row r="6" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B6" s="66">
         <v>94</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="98" t="s">
         <v>15</v>
       </c>
       <c r="D6" s="66" t="s">
@@ -4036,7 +4062,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="7" spans="2:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="67"/>
       <c r="C7" s="7" t="s">
         <v>181</v>
@@ -4044,7 +4070,7 @@
       <c r="D7" s="67"/>
       <c r="E7" s="75"/>
     </row>
-    <row r="8" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="4">
         <v>95</v>
       </c>
@@ -4058,11 +4084,11 @@
         <v>266</v>
       </c>
     </row>
-    <row r="9" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="2">
         <v>96</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="99" t="s">
         <v>184</v>
       </c>
       <c r="D9" s="2" t="s">
@@ -4072,11 +4098,11 @@
         <v>266</v>
       </c>
     </row>
-    <row r="10" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="4">
         <v>97</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="99" t="s">
         <v>186</v>
       </c>
       <c r="D10" s="4" t="s">
@@ -4086,11 +4112,11 @@
         <v>266</v>
       </c>
     </row>
-    <row r="11" spans="2:6" s="47" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:6" s="47" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="44">
         <v>98</v>
       </c>
-      <c r="C11" s="44" t="s">
+      <c r="C11" s="99" t="s">
         <v>188</v>
       </c>
       <c r="D11" s="44" t="s">
@@ -4101,11 +4127,11 @@
       </c>
       <c r="F11" s="46"/>
     </row>
-    <row r="12" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B12" s="97">
         <v>99</v>
       </c>
-      <c r="C12" s="97" t="s">
+      <c r="C12" s="101" t="s">
         <v>190</v>
       </c>
       <c r="D12" s="27" t="s">
@@ -4115,43 +4141,43 @@
         <v>266</v>
       </c>
     </row>
-    <row r="13" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B13" s="70"/>
-      <c r="C13" s="70"/>
+      <c r="C13" s="102"/>
       <c r="D13" s="8" t="s">
         <v>192</v>
       </c>
       <c r="E13" s="75"/>
     </row>
-    <row r="14" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:6" ht="33" x14ac:dyDescent="0.25">
       <c r="B14" s="70"/>
-      <c r="C14" s="70"/>
+      <c r="C14" s="102"/>
       <c r="D14" s="8" t="s">
         <v>193</v>
       </c>
       <c r="E14" s="75"/>
     </row>
-    <row r="15" spans="2:6" ht="50.4" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:6" ht="49.5" x14ac:dyDescent="0.25">
       <c r="B15" s="70"/>
-      <c r="C15" s="70"/>
+      <c r="C15" s="102"/>
       <c r="D15" s="8" t="s">
         <v>194</v>
       </c>
       <c r="E15" s="75"/>
     </row>
-    <row r="16" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="63"/>
-      <c r="C16" s="63"/>
+      <c r="C16" s="103"/>
       <c r="D16" s="4" t="s">
         <v>195</v>
       </c>
       <c r="E16" s="75"/>
     </row>
-    <row r="17" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="2">
         <v>100</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="99" t="s">
         <v>196</v>
       </c>
       <c r="D17" s="2" t="s">
@@ -4161,11 +4187,11 @@
         <v>266</v>
       </c>
     </row>
-    <row r="18" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B18" s="62">
         <v>101</v>
       </c>
-      <c r="C18" s="62" t="s">
+      <c r="C18" s="104" t="s">
         <v>198</v>
       </c>
       <c r="D18" s="8" t="s">
@@ -4175,17 +4201,17 @@
         <v>266</v>
       </c>
     </row>
-    <row r="19" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B19" s="70"/>
-      <c r="C19" s="70"/>
+      <c r="C19" s="102"/>
       <c r="D19" s="8" t="s">
         <v>200</v>
       </c>
       <c r="E19" s="75"/>
     </row>
-    <row r="20" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="63"/>
-      <c r="C20" s="63"/>
+      <c r="C20" s="103"/>
       <c r="D20" s="4" t="s">
         <v>201</v>
       </c>
@@ -4214,22 +4240,22 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20:E21"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="4.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="59" customWidth="1"/>
-    <col min="4" max="4" width="52.6640625" customWidth="1"/>
-    <col min="5" max="5" width="9.109375" style="39"/>
+    <col min="4" max="4" width="52.7109375" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="39"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E1" s="39" t="s">
         <v>48</v>
       </c>
@@ -4237,7 +4263,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="2" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B2" s="71">
         <v>102</v>
       </c>
@@ -4251,7 +4277,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="3" spans="2:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="67"/>
       <c r="C3" s="7" t="s">
         <v>179</v>
@@ -4259,11 +4285,11 @@
       <c r="D3" s="67"/>
       <c r="E3" s="75"/>
     </row>
-    <row r="4" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B4" s="62">
         <v>103</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="98" t="s">
         <v>202</v>
       </c>
       <c r="D4" s="62" t="s">
@@ -4273,7 +4299,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="5" spans="2:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="63"/>
       <c r="C5" s="9" t="s">
         <v>180</v>
@@ -4281,11 +4307,11 @@
       <c r="D5" s="63"/>
       <c r="E5" s="75"/>
     </row>
-    <row r="6" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B6" s="66">
         <v>104</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="98" t="s">
         <v>15</v>
       </c>
       <c r="D6" s="66" t="s">
@@ -4295,7 +4321,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="7" spans="2:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="67"/>
       <c r="C7" s="7" t="s">
         <v>181</v>
@@ -4303,11 +4329,11 @@
       <c r="D7" s="67"/>
       <c r="E7" s="75"/>
     </row>
-    <row r="8" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="4">
         <v>105</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="99" t="s">
         <v>203</v>
       </c>
       <c r="D8" s="4" t="s">
@@ -4317,11 +4343,11 @@
         <v>266</v>
       </c>
     </row>
-    <row r="9" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="2">
         <v>106</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="99" t="s">
         <v>205</v>
       </c>
       <c r="D9" s="2" t="s">
@@ -4331,11 +4357,11 @@
         <v>266</v>
       </c>
     </row>
-    <row r="10" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="4">
         <v>107</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="99" t="s">
         <v>207</v>
       </c>
       <c r="D10" s="4" t="s">
@@ -4345,11 +4371,11 @@
         <v>266</v>
       </c>
     </row>
-    <row r="11" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="2">
         <v>108</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="99" t="s">
         <v>209</v>
       </c>
       <c r="D11" s="2" t="s">
@@ -4359,11 +4385,11 @@
         <v>271</v>
       </c>
     </row>
-    <row r="12" spans="2:6" s="47" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:6" s="47" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="44">
         <v>109</v>
       </c>
-      <c r="C12" s="44" t="s">
+      <c r="C12" s="99" t="s">
         <v>210</v>
       </c>
       <c r="D12" s="44" t="s">
@@ -4373,11 +4399,11 @@
         <v>266</v>
       </c>
     </row>
-    <row r="13" spans="2:6" s="47" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:6" s="47" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="44">
         <v>110</v>
       </c>
-      <c r="C13" s="44" t="s">
+      <c r="C13" s="99" t="s">
         <v>212</v>
       </c>
       <c r="D13" s="44" t="s">
@@ -4387,11 +4413,11 @@
         <v>266</v>
       </c>
     </row>
-    <row r="14" spans="2:6" s="47" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:6" s="47" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="44">
         <v>111</v>
       </c>
-      <c r="C14" s="44" t="s">
+      <c r="C14" s="99" t="s">
         <v>214</v>
       </c>
       <c r="D14" s="44">
@@ -4401,11 +4427,11 @@
         <v>266</v>
       </c>
     </row>
-    <row r="15" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="24">
         <v>112</v>
       </c>
-      <c r="C15" s="24" t="s">
+      <c r="C15" s="100" t="s">
         <v>78</v>
       </c>
       <c r="D15" s="24" t="s">
@@ -4415,11 +4441,11 @@
         <v>266</v>
       </c>
     </row>
-    <row r="16" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="4">
         <v>113</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="99" t="s">
         <v>215</v>
       </c>
       <c r="D16" s="4" t="s">
@@ -4429,11 +4455,11 @@
         <v>266</v>
       </c>
     </row>
-    <row r="17" spans="2:5" s="47" customFormat="1" ht="34.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:5" s="47" customFormat="1" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="44">
         <v>114</v>
       </c>
-      <c r="C17" s="44" t="s">
+      <c r="C17" s="99" t="s">
         <v>217</v>
       </c>
       <c r="D17" s="44" t="s">
@@ -4443,11 +4469,11 @@
         <v>266</v>
       </c>
     </row>
-    <row r="18" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="4">
         <v>115</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="99" t="s">
         <v>219</v>
       </c>
       <c r="D18" s="4" t="s">
@@ -4457,11 +4483,11 @@
         <v>266</v>
       </c>
     </row>
-    <row r="19" spans="2:5" s="47" customFormat="1" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:5" s="47" customFormat="1" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="44">
         <v>116</v>
       </c>
-      <c r="C19" s="44" t="s">
+      <c r="C19" s="99" t="s">
         <v>221</v>
       </c>
       <c r="D19" s="44" t="s">
@@ -4471,7 +4497,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="20" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B20" s="62">
         <v>117</v>
       </c>
@@ -4483,7 +4509,7 @@
       </c>
       <c r="E20" s="75"/>
     </row>
-    <row r="21" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="63"/>
       <c r="C21" s="4" t="s">
         <v>224</v>
@@ -4491,7 +4517,7 @@
       <c r="D21" s="63"/>
       <c r="E21" s="75"/>
     </row>
-    <row r="22" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="2">
         <v>118</v>
       </c>
@@ -4502,11 +4528,11 @@
         <v>226</v>
       </c>
     </row>
-    <row r="23" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="4">
         <v>119</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C23" s="99" t="s">
         <v>227</v>
       </c>
       <c r="D23" s="4" t="s">
@@ -4516,11 +4542,11 @@
         <v>266</v>
       </c>
     </row>
-    <row r="24" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="2">
         <v>120</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C24" s="99" t="s">
         <v>229</v>
       </c>
       <c r="D24" s="2" t="s">
@@ -4530,11 +4556,11 @@
         <v>266</v>
       </c>
     </row>
-    <row r="25" spans="2:5" ht="34.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:5" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="4">
         <v>121</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C25" s="99" t="s">
         <v>231</v>
       </c>
       <c r="D25" s="4" t="s">
@@ -4544,11 +4570,11 @@
         <v>266</v>
       </c>
     </row>
-    <row r="26" spans="2:5" ht="34.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:5" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="2">
         <v>122</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C26" s="99" t="s">
         <v>233</v>
       </c>
       <c r="D26" s="2" t="s">
@@ -4558,11 +4584,11 @@
         <v>266</v>
       </c>
     </row>
-    <row r="27" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="4">
         <v>123</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="C27" s="99" t="s">
         <v>235</v>
       </c>
       <c r="D27" s="4" t="s">
@@ -4572,11 +4598,11 @@
         <v>266</v>
       </c>
     </row>
-    <row r="28" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="2">
         <v>124</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C28" s="99" t="s">
         <v>237</v>
       </c>
       <c r="D28" s="2" t="s">
@@ -4586,11 +4612,11 @@
         <v>266</v>
       </c>
     </row>
-    <row r="29" spans="2:5" ht="34.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:5" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B29" s="4">
         <v>125</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="C29" s="99" t="s">
         <v>239</v>
       </c>
       <c r="D29" s="4" t="s">
@@ -4600,11 +4626,11 @@
         <v>266</v>
       </c>
     </row>
-    <row r="30" spans="2:5" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B30" s="66">
         <v>126</v>
       </c>
-      <c r="C30" s="6" t="s">
+      <c r="C30" s="98" t="s">
         <v>267</v>
       </c>
       <c r="D30" s="66" t="s">
@@ -4614,7 +4640,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="31" spans="2:5" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B31" s="67"/>
       <c r="C31" s="2"/>
       <c r="D31" s="67"/>
@@ -4641,20 +4667,20 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="42.44140625" customWidth="1"/>
-    <col min="4" max="4" width="74.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.42578125" customWidth="1"/>
+    <col min="4" max="4" width="74.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E1" t="s">
         <v>259</v>
       </c>
@@ -4662,7 +4688,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="2" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="24">
         <v>127</v>
       </c>
@@ -4673,7 +4699,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="3" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="4">
         <v>128</v>
       </c>
@@ -4687,7 +4713,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="4" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="24">
         <v>129</v>
       </c>
@@ -4701,7 +4727,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="5" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="4">
         <v>130</v>
       </c>
@@ -4715,7 +4741,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="6" spans="2:6" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="2">
         <v>131</v>
       </c>
@@ -4729,11 +4755,11 @@
         <v>266</v>
       </c>
     </row>
-    <row r="7" spans="2:6" ht="34.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:6" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="4">
         <v>132</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="99" t="s">
         <v>249</v>
       </c>
       <c r="D7" s="4" t="s">
@@ -4743,11 +4769,11 @@
         <v>266</v>
       </c>
     </row>
-    <row r="8" spans="2:6" ht="34.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:6" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="2">
         <v>133</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="99" t="s">
         <v>251</v>
       </c>
       <c r="D8" s="2" t="s">
@@ -4757,11 +4783,11 @@
         <v>266</v>
       </c>
     </row>
-    <row r="9" spans="2:6" ht="34.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:6" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="4">
         <v>134</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="99" t="s">
         <v>252</v>
       </c>
       <c r="D9" s="4" t="s">
@@ -4771,11 +4797,11 @@
         <v>266</v>
       </c>
     </row>
-    <row r="10" spans="2:6" ht="51" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:6" ht="50.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="2">
         <v>135</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="99" t="s">
         <v>253</v>
       </c>
       <c r="D10" s="2" t="s">
@@ -4785,11 +4811,11 @@
         <v>266</v>
       </c>
     </row>
-    <row r="11" spans="2:6" ht="34.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:6" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="4">
         <v>136</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="99" t="s">
         <v>255</v>
       </c>
       <c r="D11" s="4" t="s">
@@ -4799,11 +4825,11 @@
         <v>266</v>
       </c>
     </row>
-    <row r="12" spans="2:6" ht="34.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:6" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="2">
         <v>137</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="99" t="s">
         <v>257</v>
       </c>
       <c r="D12" s="2" t="s">

</xml_diff>

<commit_message>
Updated checklist tally track record
</commit_message>
<xml_diff>
--- a/Checklist.xlsx
+++ b/Checklist.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" firstSheet="3" activeTab="4"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Application" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="278">
   <si>
     <t xml:space="preserve"> Last Updated</t>
   </si>
@@ -170,21 +170,6 @@
     <t>600 Second(s)</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Security [Fips Algorithm Policy] </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color rgb="FF515967"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t>Is Fips Algorithm Policy Enabled?</t>
-    </r>
-  </si>
-  <si>
     <t>Enabled</t>
   </si>
   <si>
@@ -1043,12 +1028,27 @@
   <si>
     <t>Script Name</t>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Security [Fips Algorithm Policy] </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="0"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>Is Fips Algorithm Policy Enabled?</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1104,8 +1104,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1156,6 +1170,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1365,7 +1391,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="105">
+  <cellXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1412,26 +1438,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1449,9 +1460,6 @@
     <xf numFmtId="14" fontId="4" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1471,9 +1479,6 @@
       <alignment horizontal="justify" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="1"/>
@@ -1513,17 +1518,8 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1535,26 +1531,20 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
@@ -1562,7 +1552,19 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1577,95 +1579,125 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="4" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="4" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="4" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="4" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="4" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="4" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1705,7 +1737,7 @@
         <xdr:cNvPr id="14" name="Picture 92361">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000E000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1766,7 +1798,7 @@
         <xdr:cNvPr id="15" name="Picture 92362">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000F000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2079,7 +2111,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
+      <selection pane="bottomLeft" activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2087,493 +2119,506 @@
     <col min="2" max="2" width="3.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="51" customWidth="1"/>
     <col min="4" max="4" width="74.42578125" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="39"/>
+    <col min="5" max="5" width="9.140625" style="32"/>
     <col min="6" max="6" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="38" t="s">
-        <v>264</v>
-      </c>
-      <c r="C1" s="38" t="s">
+      <c r="B1" s="31" t="s">
+        <v>263</v>
+      </c>
+      <c r="C1" s="31" t="s">
+        <v>261</v>
+      </c>
+      <c r="D1" s="31" t="s">
         <v>262</v>
       </c>
-      <c r="D1" s="38" t="s">
-        <v>263</v>
-      </c>
-      <c r="E1" s="40" t="s">
+      <c r="E1" s="33" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="F1" s="38" t="s">
-        <v>49</v>
-      </c>
     </row>
     <row r="2" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="68" t="s">
+      <c r="B2" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
     </row>
     <row r="3" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="12">
         <v>1</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="52" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="14">
         <v>44102</v>
       </c>
-      <c r="E3" s="39" t="s">
-        <v>266</v>
+      <c r="E3" s="32" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="10">
         <v>2</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="23" t="s">
+      <c r="D4" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="39" t="s">
-        <v>266</v>
+      <c r="E4" s="32" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="73" t="s">
+      <c r="B5" s="65" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="74"/>
-      <c r="D5" s="74"/>
+      <c r="C5" s="66"/>
+      <c r="D5" s="66"/>
     </row>
     <row r="6" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B6" s="13">
         <v>3</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="71" t="s">
+      <c r="D6" s="63" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="75" t="s">
-        <v>266</v>
+      <c r="E6" s="54" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="1"/>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="97" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="67"/>
-      <c r="E7" s="75"/>
+      <c r="D7" s="61"/>
+      <c r="E7" s="54"/>
     </row>
     <row r="8" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="51"/>
+      <c r="A8" s="44"/>
       <c r="B8" s="11">
         <v>4</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="96" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="62" t="s">
+      <c r="D8" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="75"/>
+      <c r="E8" s="54"/>
     </row>
     <row r="9" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="51"/>
+      <c r="A9" s="44"/>
       <c r="B9" s="1"/>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="99" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="63"/>
-      <c r="E9" s="75"/>
+      <c r="D9" s="62"/>
+      <c r="E9" s="54"/>
     </row>
     <row r="10" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B10" s="13">
         <v>5</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="C10" s="95" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="71" t="s">
+      <c r="D10" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="75" t="s">
-        <v>266</v>
+      <c r="E10" s="54" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="5"/>
-      <c r="C11" s="16" t="s">
-        <v>261</v>
-      </c>
-      <c r="D11" s="72"/>
-      <c r="E11" s="75"/>
+      <c r="C11" s="98" t="s">
+        <v>260</v>
+      </c>
+      <c r="D11" s="64"/>
+      <c r="E11" s="54"/>
     </row>
     <row r="12" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B12" s="11">
         <v>6</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="62" t="s">
+      <c r="D12" s="58" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="75" t="s">
-        <v>266</v>
+      <c r="E12" s="54" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="5"/>
-      <c r="C13" s="17" t="s">
-        <v>261</v>
-      </c>
-      <c r="D13" s="70"/>
-      <c r="E13" s="75"/>
+      <c r="C13" s="98" t="s">
+        <v>260</v>
+      </c>
+      <c r="D13" s="59"/>
+      <c r="E13" s="54"/>
     </row>
     <row r="14" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B14" s="11">
         <v>7</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="51" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="66" t="s">
+      <c r="D14" s="60" t="s">
         <v>14</v>
       </c>
-      <c r="E14" s="75" t="s">
-        <v>266</v>
+      <c r="E14" s="54" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="1"/>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="97" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="67"/>
-      <c r="E15" s="75"/>
+      <c r="D15" s="61"/>
+      <c r="E15" s="54"/>
     </row>
     <row r="16" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B16" s="11">
         <v>8</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="62" t="s">
+      <c r="D16" s="58" t="s">
         <v>17</v>
       </c>
-      <c r="E16" s="75" t="s">
-        <v>266</v>
+      <c r="E16" s="54" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="17" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="1"/>
-      <c r="C17" s="9" t="s">
+      <c r="C17" s="97" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="63"/>
-      <c r="E17" s="75"/>
+      <c r="D17" s="62"/>
+      <c r="E17" s="54"/>
     </row>
     <row r="18" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B18" s="11">
         <v>9</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="D18" s="66">
+      <c r="D18" s="60">
         <v>4</v>
       </c>
-      <c r="E18" s="75" t="s">
-        <v>266</v>
+      <c r="E18" s="54" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="19" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="1"/>
-      <c r="C19" s="7" t="s">
+      <c r="C19" s="97" t="s">
         <v>19</v>
       </c>
-      <c r="D19" s="67"/>
-      <c r="E19" s="75"/>
+      <c r="D19" s="61"/>
+      <c r="E19" s="54"/>
     </row>
     <row r="20" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="1">
         <v>10</v>
       </c>
-      <c r="C20" s="18" t="s">
+      <c r="C20" s="94" t="s">
         <v>20</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E20" s="75" t="s">
-        <v>266</v>
+      <c r="E20" s="54" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="21" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C21" s="19" t="s">
+      <c r="C21" s="94" t="s">
         <v>22</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E21" s="75"/>
+      <c r="E21" s="54"/>
     </row>
     <row r="22" spans="2:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="11">
         <v>11</v>
       </c>
-      <c r="C22" s="8" t="s">
+      <c r="C22" s="51" t="s">
         <v>23</v>
       </c>
-      <c r="D22" s="62" t="s">
+      <c r="D22" s="58" t="s">
         <v>25</v>
       </c>
-      <c r="E22" s="75" t="s">
-        <v>266</v>
+      <c r="E22" s="54" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="23" spans="2:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="1"/>
-      <c r="C23" s="9" t="s">
+      <c r="C23" s="97" t="s">
         <v>24</v>
       </c>
-      <c r="D23" s="63"/>
-      <c r="E23" s="75"/>
+      <c r="D23" s="62"/>
+      <c r="E23" s="54"/>
     </row>
     <row r="24" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B24" s="11">
         <v>12</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="C24" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="D24" s="66" t="s">
+      <c r="D24" s="60" t="s">
         <v>28</v>
       </c>
-      <c r="E24" s="75" t="s">
-        <v>266</v>
+      <c r="E24" s="54" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="25" spans="2:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="1"/>
-      <c r="C25" s="7" t="s">
+      <c r="C25" s="97" t="s">
         <v>27</v>
       </c>
-      <c r="D25" s="67"/>
-      <c r="E25" s="75"/>
+      <c r="D25" s="61"/>
+      <c r="E25" s="54"/>
     </row>
     <row r="26" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B26" s="11">
         <v>13</v>
       </c>
-      <c r="C26" s="8" t="s">
+      <c r="C26" s="51" t="s">
         <v>29</v>
       </c>
-      <c r="D26" s="62" t="s">
+      <c r="D26" s="58" t="s">
         <v>31</v>
       </c>
-      <c r="E26" s="75" t="s">
-        <v>266</v>
+      <c r="E26" s="54" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="27" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="1"/>
-      <c r="C27" s="9" t="s">
+      <c r="C27" s="97" t="s">
         <v>30</v>
       </c>
-      <c r="D27" s="63"/>
-      <c r="E27" s="75"/>
-    </row>
-    <row r="28" spans="2:5" s="47" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="60">
+      <c r="D27" s="62"/>
+      <c r="E27" s="54"/>
+    </row>
+    <row r="28" spans="2:5" s="40" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="50">
         <v>14</v>
       </c>
-      <c r="C28" s="49" t="s">
+      <c r="C28" s="51" t="s">
         <v>32</v>
       </c>
-      <c r="D28" s="64" t="s">
+      <c r="D28" s="67" t="s">
         <v>34</v>
       </c>
-      <c r="E28" s="76" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="29" spans="2:5" s="47" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="55"/>
-      <c r="C29" s="61" t="s">
+      <c r="E28" s="55" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" s="40" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="46"/>
+      <c r="C29" s="97" t="s">
         <v>33</v>
       </c>
-      <c r="D29" s="65"/>
-      <c r="E29" s="76"/>
+      <c r="D29" s="68"/>
+      <c r="E29" s="55"/>
     </row>
     <row r="30" spans="2:5" ht="31.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="20">
+      <c r="B30" s="16">
         <v>15</v>
       </c>
-      <c r="C30" s="22" t="s">
+      <c r="C30" s="96" t="s">
+        <v>277</v>
+      </c>
+      <c r="D30" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="D30" s="21" t="s">
+    </row>
+    <row r="31" spans="2:5" s="40" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="46">
+        <v>16</v>
+      </c>
+      <c r="C31" s="94" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="31" spans="2:5" s="47" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="55">
-        <v>16</v>
-      </c>
-      <c r="C31" s="56" t="s">
+      <c r="D31" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="D31" s="44" t="s">
+      <c r="E31" s="38" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" s="40" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="46">
+        <v>17</v>
+      </c>
+      <c r="C32" s="94" t="s">
         <v>38</v>
       </c>
-      <c r="E31" s="45" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="32" spans="2:5" s="47" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="55">
-        <v>17</v>
-      </c>
-      <c r="C32" s="56" t="s">
+      <c r="D32" s="37" t="s">
+        <v>37</v>
+      </c>
+      <c r="E32" s="38" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" s="40" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="46">
+        <v>18</v>
+      </c>
+      <c r="C33" s="94" t="s">
         <v>39</v>
       </c>
-      <c r="D32" s="44" t="s">
-        <v>38</v>
-      </c>
-      <c r="E32" s="45" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="33" spans="2:5" s="47" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="55">
-        <v>18</v>
-      </c>
-      <c r="C33" s="56" t="s">
+      <c r="D33" s="37" t="s">
+        <v>37</v>
+      </c>
+      <c r="E33" s="38" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" s="40" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="46">
+        <v>19</v>
+      </c>
+      <c r="C34" s="94" t="s">
         <v>40</v>
       </c>
-      <c r="D33" s="44" t="s">
-        <v>38</v>
-      </c>
-      <c r="E33" s="45" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="34" spans="2:5" s="47" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="55">
-        <v>19</v>
-      </c>
-      <c r="C34" s="56" t="s">
+      <c r="D34" s="37" t="s">
+        <v>37</v>
+      </c>
+      <c r="E34" s="38" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" s="40" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="46">
+        <v>20</v>
+      </c>
+      <c r="C35" s="94" t="s">
         <v>41</v>
       </c>
-      <c r="D34" s="44" t="s">
-        <v>38</v>
-      </c>
-      <c r="E34" s="45" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="35" spans="2:5" s="47" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="55">
-        <v>20</v>
-      </c>
-      <c r="C35" s="56" t="s">
+      <c r="D35" s="37" t="s">
+        <v>35</v>
+      </c>
+      <c r="E35" s="38" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" s="40" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="46">
+        <v>21</v>
+      </c>
+      <c r="C36" s="94" t="s">
         <v>42</v>
       </c>
-      <c r="D35" s="44" t="s">
-        <v>36</v>
-      </c>
-      <c r="E35" s="45" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="36" spans="2:5" s="47" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="55">
-        <v>21</v>
-      </c>
-      <c r="C36" s="56" t="s">
+      <c r="D36" s="37" t="s">
+        <v>37</v>
+      </c>
+      <c r="E36" s="38" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" s="40" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="46">
+        <v>22</v>
+      </c>
+      <c r="C37" s="94" t="s">
         <v>43</v>
       </c>
-      <c r="D36" s="44" t="s">
-        <v>38</v>
-      </c>
-      <c r="E36" s="45" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="37" spans="2:5" s="47" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="55">
-        <v>22</v>
-      </c>
-      <c r="C37" s="56" t="s">
+      <c r="D37" s="37" t="s">
+        <v>37</v>
+      </c>
+      <c r="E37" s="38" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" s="40" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="46">
+        <v>23</v>
+      </c>
+      <c r="C38" s="94" t="s">
         <v>44</v>
       </c>
-      <c r="D37" s="44" t="s">
-        <v>38</v>
-      </c>
-      <c r="E37" s="45" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="38" spans="2:5" s="47" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="55">
-        <v>23</v>
-      </c>
-      <c r="C38" s="56" t="s">
+      <c r="D38" s="37" t="s">
+        <v>37</v>
+      </c>
+      <c r="E38" s="38" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" s="40" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="46">
+        <v>24</v>
+      </c>
+      <c r="C39" s="94" t="s">
         <v>45</v>
       </c>
-      <c r="D38" s="44" t="s">
-        <v>38</v>
-      </c>
-      <c r="E38" s="45" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="39" spans="2:5" s="47" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="55">
-        <v>24</v>
-      </c>
-      <c r="C39" s="56" t="s">
+      <c r="D39" s="37" t="s">
+        <v>35</v>
+      </c>
+      <c r="E39" s="38" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" s="40" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="46">
+        <v>25</v>
+      </c>
+      <c r="C40" s="94" t="s">
         <v>46</v>
       </c>
-      <c r="D39" s="44" t="s">
-        <v>36</v>
-      </c>
-      <c r="E39" s="45" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="40" spans="2:5" s="47" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="55">
-        <v>25</v>
-      </c>
-      <c r="C40" s="56" t="s">
-        <v>47</v>
-      </c>
-      <c r="D40" s="44" t="s">
-        <v>36</v>
-      </c>
-      <c r="E40" s="45" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="41" spans="2:5" s="25" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="C41" s="26" t="s">
-        <v>69</v>
-      </c>
-      <c r="E41" s="41"/>
+      <c r="D40" s="37" t="s">
+        <v>35</v>
+      </c>
+      <c r="E40" s="38" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" s="20" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="C41" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="E41" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="D6:D7"/>
     <mergeCell ref="E26:E27"/>
     <mergeCell ref="E28:E29"/>
     <mergeCell ref="E12:E13"/>
@@ -2586,19 +2631,6 @@
     <mergeCell ref="E24:E25"/>
     <mergeCell ref="E16:E17"/>
     <mergeCell ref="E14:E15"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="D18:D19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2620,63 +2652,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B1" s="77" t="s">
-        <v>277</v>
-      </c>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
+      <c r="B1" s="69" t="s">
+        <v>276</v>
+      </c>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
       <c r="E1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="77" t="s">
+      <c r="B2" s="69" t="s">
+        <v>271</v>
+      </c>
+      <c r="C2" s="69"/>
+      <c r="D2" s="69"/>
+      <c r="E2" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="69" t="s">
         <v>272</v>
       </c>
-      <c r="C2" s="77"/>
-      <c r="D2" s="77"/>
-      <c r="E2" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="77" t="s">
+      <c r="C3" s="69"/>
+      <c r="D3" s="69"/>
+      <c r="E3" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="69" t="s">
         <v>273</v>
       </c>
-      <c r="C3" s="77"/>
-      <c r="D3" s="77"/>
-      <c r="E3" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="77" t="s">
+      <c r="C4" s="69"/>
+      <c r="D4" s="69"/>
+      <c r="E4" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="69" t="s">
         <v>274</v>
       </c>
-      <c r="C4" s="77"/>
-      <c r="D4" s="77"/>
-      <c r="E4" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="77" t="s">
+      <c r="C5" s="69"/>
+      <c r="D5" s="69"/>
+      <c r="E5" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="69" t="s">
         <v>275</v>
       </c>
-      <c r="C5" s="77"/>
-      <c r="D5" s="77"/>
-      <c r="E5" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="77" t="s">
-        <v>276</v>
-      </c>
-      <c r="C6" s="77"/>
-      <c r="D6" s="77"/>
+      <c r="C6" s="69"/>
+      <c r="D6" s="69"/>
       <c r="E6" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
   </sheetData>
@@ -2697,7 +2729,7 @@
   <dimension ref="B1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11:C12"/>
+      <selection activeCell="C9" sqref="C9:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2710,205 +2742,202 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E1" s="42" t="s">
-        <v>48</v>
-      </c>
-      <c r="F1" s="42" t="s">
-        <v>268</v>
+      <c r="E1" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" s="35" t="s">
+        <v>267</v>
       </c>
     </row>
     <row r="2" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="24">
+      <c r="B2" s="19">
         <v>26</v>
       </c>
-      <c r="C2" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="D2" s="24" t="s">
+      <c r="C2" s="53" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" s="19" t="s">
         <v>14</v>
       </c>
       <c r="E2" t="s">
-        <v>266</v>
-      </c>
-      <c r="F2" s="43"/>
+        <v>265</v>
+      </c>
+      <c r="F2" s="36"/>
     </row>
     <row r="3" spans="2:6" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="4">
         <v>27</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="52" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>52</v>
-      </c>
       <c r="E3" t="s">
-        <v>266</v>
-      </c>
-      <c r="F3" s="43"/>
+        <v>265</v>
+      </c>
+      <c r="F3" s="36"/>
     </row>
     <row r="4" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="2">
         <v>28</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="52" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>54</v>
-      </c>
       <c r="E4" t="s">
-        <v>266</v>
-      </c>
-      <c r="F4" s="43"/>
+        <v>265</v>
+      </c>
+      <c r="F4" s="36"/>
     </row>
     <row r="5" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="4">
         <v>29</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="52" t="s">
+        <v>54</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="E5" t="s">
+        <v>265</v>
+      </c>
+      <c r="F5" s="36"/>
+    </row>
+    <row r="6" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="19">
+        <v>30</v>
+      </c>
+      <c r="C6" s="53" t="s">
         <v>56</v>
       </c>
-      <c r="E5" t="s">
-        <v>266</v>
-      </c>
-      <c r="F5" s="43"/>
-    </row>
-    <row r="6" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="24">
-        <v>30</v>
-      </c>
-      <c r="C6" s="24" t="s">
-        <v>57</v>
-      </c>
-      <c r="D6" s="24" t="s">
-        <v>56</v>
+      <c r="D6" s="19" t="s">
+        <v>55</v>
       </c>
       <c r="E6" t="s">
-        <v>266</v>
-      </c>
-      <c r="F6" s="43"/>
+        <v>265</v>
+      </c>
+      <c r="F6" s="36"/>
     </row>
     <row r="7" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="4">
         <v>31</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>58</v>
+      <c r="C7" s="52" t="s">
+        <v>57</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E7" t="s">
-        <v>266</v>
-      </c>
-      <c r="F7" s="43"/>
+        <v>265</v>
+      </c>
+      <c r="F7" s="36"/>
     </row>
     <row r="8" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="2">
         <v>32</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="F8" s="36"/>
+    </row>
+    <row r="9" spans="2:6" s="40" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B9" s="41">
+        <v>33</v>
+      </c>
+      <c r="C9" s="89" t="s">
         <v>60</v>
       </c>
-      <c r="E8" t="s">
-        <v>266</v>
-      </c>
-      <c r="F8" s="43"/>
-    </row>
-    <row r="9" spans="2:6" s="47" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B9" s="48">
-        <v>33</v>
-      </c>
-      <c r="C9" s="64" t="s">
+      <c r="D9" s="42" t="s">
         <v>61</v>
       </c>
-      <c r="D9" s="49" t="s">
+      <c r="E9" s="55" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" s="40" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="43"/>
+      <c r="C10" s="91"/>
+      <c r="D10" s="37" t="s">
         <v>62</v>
       </c>
-      <c r="E9" s="76" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" s="47" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="50"/>
-      <c r="C10" s="65"/>
-      <c r="D10" s="44" t="s">
+      <c r="E10" s="55"/>
+    </row>
+    <row r="11" spans="2:6" s="40" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B11" s="41">
+        <v>34</v>
+      </c>
+      <c r="C11" s="89" t="s">
         <v>63</v>
       </c>
-      <c r="E10" s="76"/>
-    </row>
-    <row r="11" spans="2:6" s="47" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B11" s="48">
-        <v>34</v>
-      </c>
-      <c r="C11" s="64" t="s">
+      <c r="D11" s="42" t="s">
         <v>64</v>
       </c>
-      <c r="D11" s="49" t="s">
+      <c r="E11" s="55" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" s="40" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="43"/>
+      <c r="C12" s="91"/>
+      <c r="D12" s="37" t="s">
+        <v>62</v>
+      </c>
+      <c r="E12" s="55"/>
+    </row>
+    <row r="13" spans="2:6" s="40" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B13" s="41">
+        <v>35</v>
+      </c>
+      <c r="C13" s="89" t="s">
         <v>65</v>
       </c>
-      <c r="E11" s="76" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" s="47" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="50"/>
-      <c r="C12" s="65"/>
-      <c r="D12" s="44" t="s">
-        <v>63</v>
-      </c>
-      <c r="E12" s="76"/>
-    </row>
-    <row r="13" spans="2:6" s="47" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B13" s="48">
-        <v>35</v>
-      </c>
-      <c r="C13" s="64" t="s">
+      <c r="D13" s="42" t="s">
+        <v>61</v>
+      </c>
+      <c r="E13" s="55" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" s="40" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="43"/>
+      <c r="C14" s="91"/>
+      <c r="D14" s="37" t="s">
         <v>66</v>
       </c>
-      <c r="D13" s="49" t="s">
-        <v>62</v>
-      </c>
-      <c r="E13" s="76" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" s="47" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="50"/>
-      <c r="C14" s="65"/>
-      <c r="D14" s="44" t="s">
+      <c r="E14" s="55"/>
+    </row>
+    <row r="15" spans="2:6" s="40" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B15" s="41">
+        <v>36</v>
+      </c>
+      <c r="C15" s="89" t="s">
         <v>67</v>
       </c>
-      <c r="E14" s="76"/>
-    </row>
-    <row r="15" spans="2:6" s="47" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B15" s="48">
-        <v>36</v>
-      </c>
-      <c r="C15" s="64" t="s">
-        <v>68</v>
-      </c>
-      <c r="D15" s="49" t="s">
-        <v>65</v>
-      </c>
-      <c r="E15" s="76" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6" s="47" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="50"/>
-      <c r="C16" s="65"/>
-      <c r="D16" s="44" t="s">
-        <v>67</v>
-      </c>
-      <c r="E16" s="76"/>
+      <c r="D15" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="E15" s="55" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" s="40" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="43"/>
+      <c r="C16" s="91"/>
+      <c r="D16" s="37" t="s">
+        <v>66</v>
+      </c>
+      <c r="E16" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -2930,758 +2959,758 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F80"/>
   <sheetViews>
-    <sheetView topLeftCell="B61" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29:D30"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C34" activeCellId="1" sqref="C33 C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="56" customWidth="1"/>
     <col min="4" max="4" width="108.28515625" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="39"/>
+    <col min="5" max="5" width="9.140625" style="32"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>177</v>
-      </c>
-      <c r="E2" s="39" t="s">
+        <v>176</v>
+      </c>
+      <c r="E2" s="32" t="s">
+        <v>258</v>
+      </c>
+      <c r="F2" t="s">
         <v>259</v>
       </c>
-      <c r="F2" t="s">
-        <v>260</v>
-      </c>
     </row>
     <row r="3" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B3" s="71">
+      <c r="B3" s="63">
         <v>37</v>
       </c>
       <c r="C3" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="71" t="s">
-        <v>71</v>
-      </c>
-      <c r="E3" s="75" t="s">
-        <v>266</v>
+      <c r="D3" s="63" t="s">
+        <v>70</v>
+      </c>
+      <c r="E3" s="54" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="4" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="67"/>
+      <c r="B4" s="61"/>
       <c r="C4" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="D4" s="67"/>
-      <c r="E4" s="75"/>
+        <v>69</v>
+      </c>
+      <c r="D4" s="61"/>
+      <c r="E4" s="54"/>
     </row>
     <row r="5" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B5" s="62">
+      <c r="B5" s="58">
         <v>38</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="62" t="s">
-        <v>73</v>
-      </c>
-      <c r="E5" s="75" t="s">
-        <v>266</v>
+      <c r="D5" s="58" t="s">
+        <v>72</v>
+      </c>
+      <c r="E5" s="54" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="6" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="63"/>
+      <c r="B6" s="62"/>
       <c r="C6" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="D6" s="63"/>
-      <c r="E6" s="75"/>
+        <v>71</v>
+      </c>
+      <c r="D6" s="62"/>
+      <c r="E6" s="54"/>
     </row>
     <row r="7" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B7" s="66">
+      <c r="B7" s="60">
         <v>39</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="66" t="s">
+      <c r="D7" s="60" t="s">
         <v>31</v>
       </c>
-      <c r="E7" s="75" t="s">
-        <v>266</v>
+      <c r="E7" s="54" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="8" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="67"/>
+      <c r="B8" s="61"/>
       <c r="C8" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D8" s="61"/>
+      <c r="E8" s="54"/>
+    </row>
+    <row r="9" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B9" s="58">
+        <v>40</v>
+      </c>
+      <c r="C9" s="51" t="s">
         <v>74</v>
       </c>
-      <c r="D8" s="67"/>
-      <c r="E8" s="75"/>
-    </row>
-    <row r="9" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B9" s="62">
-        <v>40</v>
-      </c>
-      <c r="C9" s="8" t="s">
+      <c r="D9" s="58" t="s">
+        <v>76</v>
+      </c>
+      <c r="E9" s="54" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="62"/>
+      <c r="C10" s="97" t="s">
         <v>75</v>
       </c>
-      <c r="D9" s="62" t="s">
+      <c r="D10" s="62"/>
+      <c r="E10" s="54"/>
+    </row>
+    <row r="11" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B11" s="60">
+        <v>41</v>
+      </c>
+      <c r="C11" s="51" t="s">
         <v>77</v>
       </c>
-      <c r="E9" s="75" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="63"/>
-      <c r="C10" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="D10" s="63"/>
-      <c r="E10" s="75"/>
-    </row>
-    <row r="11" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B11" s="66">
-        <v>41</v>
-      </c>
-      <c r="C11" s="6" t="s">
+      <c r="D11" s="60" t="s">
+        <v>79</v>
+      </c>
+      <c r="E11" s="54" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="61"/>
+      <c r="C12" s="97" t="s">
         <v>78</v>
       </c>
-      <c r="D11" s="66" t="s">
+      <c r="D12" s="61"/>
+      <c r="E12" s="54"/>
+    </row>
+    <row r="13" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B13" s="58">
+        <v>42</v>
+      </c>
+      <c r="C13" s="51" t="s">
         <v>80</v>
       </c>
-      <c r="E11" s="75" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="67"/>
-      <c r="C12" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="D12" s="67"/>
-      <c r="E12" s="75"/>
-    </row>
-    <row r="13" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B13" s="62">
-        <v>42</v>
-      </c>
-      <c r="C13" s="8" t="s">
+      <c r="D13" s="58" t="s">
+        <v>82</v>
+      </c>
+      <c r="E13" s="54" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="62"/>
+      <c r="C14" s="97" t="s">
         <v>81</v>
       </c>
-      <c r="D13" s="62" t="s">
+      <c r="D14" s="62"/>
+      <c r="E14" s="54"/>
+    </row>
+    <row r="15" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B15" s="78">
+        <v>43</v>
+      </c>
+      <c r="C15" s="103" t="s">
         <v>83</v>
       </c>
-      <c r="E13" s="75" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="63"/>
-      <c r="C14" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="D14" s="63"/>
-      <c r="E14" s="75"/>
-    </row>
-    <row r="15" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B15" s="90">
-        <v>43</v>
-      </c>
-      <c r="C15" s="29" t="s">
+      <c r="D15" s="78" t="s">
+        <v>85</v>
+      </c>
+      <c r="E15" s="54" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="73"/>
+      <c r="C16" s="102" t="s">
         <v>84</v>
       </c>
-      <c r="D15" s="90" t="s">
+      <c r="D16" s="73"/>
+      <c r="E16" s="54"/>
+    </row>
+    <row r="17" spans="2:5" s="48" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B17" s="79">
+        <v>44</v>
+      </c>
+      <c r="C17" s="47" t="s">
         <v>86</v>
       </c>
-      <c r="E15" s="75" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="81"/>
-      <c r="C16" s="30" t="s">
-        <v>85</v>
-      </c>
-      <c r="D16" s="81"/>
-      <c r="E16" s="75"/>
-    </row>
-    <row r="17" spans="2:5" s="58" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B17" s="91">
-        <v>44</v>
-      </c>
-      <c r="C17" s="57" t="s">
+      <c r="D17" s="81">
+        <v>987654321</v>
+      </c>
+      <c r="E17" s="70" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" s="48" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="80"/>
+      <c r="C18" s="49" t="s">
         <v>87</v>
       </c>
-      <c r="D17" s="93">
-        <v>987654321</v>
-      </c>
-      <c r="E17" s="96" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" s="58" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="92"/>
-      <c r="C18" s="59" t="s">
+      <c r="D18" s="82"/>
+      <c r="E18" s="70"/>
+    </row>
+    <row r="19" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B19" s="72">
+        <v>45</v>
+      </c>
+      <c r="C19" s="27" t="s">
         <v>88</v>
       </c>
-      <c r="D18" s="94"/>
-      <c r="E18" s="96"/>
-    </row>
-    <row r="19" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B19" s="80">
-        <v>45</v>
-      </c>
-      <c r="C19" s="33" t="s">
+      <c r="D19" s="72">
+        <v>1433</v>
+      </c>
+      <c r="E19" s="54" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="73"/>
+      <c r="C20" s="24" t="s">
         <v>89</v>
       </c>
-      <c r="D19" s="80">
-        <v>1433</v>
-      </c>
-      <c r="E19" s="75" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="81"/>
-      <c r="C20" s="30" t="s">
+      <c r="D20" s="73"/>
+      <c r="E20" s="54"/>
+    </row>
+    <row r="21" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B21" s="74">
+        <v>46</v>
+      </c>
+      <c r="C21" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="D20" s="81"/>
-      <c r="E20" s="75"/>
-    </row>
-    <row r="21" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B21" s="82">
-        <v>46</v>
-      </c>
-      <c r="C21" s="31" t="s">
+      <c r="D21" s="76">
+        <v>43925</v>
+      </c>
+      <c r="E21" s="71" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="75"/>
+      <c r="C22" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="D21" s="87">
-        <v>43925</v>
-      </c>
-      <c r="E21" s="95" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="22" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="83"/>
-      <c r="C22" s="32" t="s">
+      <c r="D22" s="77"/>
+      <c r="E22" s="54"/>
+    </row>
+    <row r="23" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B23" s="72">
+        <v>47</v>
+      </c>
+      <c r="C23" s="100" t="s">
         <v>92</v>
       </c>
-      <c r="D22" s="89"/>
-      <c r="E22" s="75"/>
-    </row>
-    <row r="23" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B23" s="80">
-        <v>47</v>
-      </c>
-      <c r="C23" s="33" t="s">
+      <c r="D23" s="83" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23" s="71" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="73"/>
+      <c r="C24" s="102" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" s="84"/>
+      <c r="E24" s="54"/>
+    </row>
+    <row r="25" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B25" s="74">
+        <v>48</v>
+      </c>
+      <c r="C25" s="100" t="s">
         <v>93</v>
       </c>
-      <c r="D23" s="85" t="s">
-        <v>7</v>
-      </c>
-      <c r="E23" s="95" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="81"/>
-      <c r="C24" s="30" t="s">
-        <v>6</v>
-      </c>
-      <c r="D24" s="86"/>
-      <c r="E24" s="75"/>
-    </row>
-    <row r="25" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B25" s="82">
-        <v>48</v>
-      </c>
-      <c r="C25" s="31" t="s">
+      <c r="D25" s="76">
+        <v>43834</v>
+      </c>
+      <c r="E25" s="71" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="75"/>
+      <c r="C26" s="102" t="s">
         <v>94</v>
       </c>
-      <c r="D25" s="87">
-        <v>43834</v>
-      </c>
-      <c r="E25" s="95" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="26" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="83"/>
-      <c r="C26" s="32" t="s">
+      <c r="D26" s="85"/>
+      <c r="E26" s="54"/>
+    </row>
+    <row r="27" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B27" s="72">
+        <v>49</v>
+      </c>
+      <c r="C27" s="100" t="s">
         <v>95</v>
       </c>
-      <c r="D26" s="88"/>
-      <c r="E26" s="75"/>
-    </row>
-    <row r="27" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B27" s="80">
-        <v>49</v>
-      </c>
-      <c r="C27" s="33" t="s">
+      <c r="D27" s="72">
+        <v>0</v>
+      </c>
+      <c r="E27" s="71" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="73"/>
+      <c r="C28" s="102" t="s">
+        <v>95</v>
+      </c>
+      <c r="D28" s="73"/>
+      <c r="E28" s="54"/>
+    </row>
+    <row r="29" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B29" s="74">
+        <v>50</v>
+      </c>
+      <c r="C29" s="100" t="s">
         <v>96</v>
       </c>
-      <c r="D27" s="80">
-        <v>0</v>
-      </c>
-      <c r="E27" s="95" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="28" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="81"/>
-      <c r="C28" s="30" t="s">
-        <v>96</v>
-      </c>
-      <c r="D28" s="81"/>
-      <c r="E28" s="75"/>
-    </row>
-    <row r="29" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B29" s="82">
-        <v>50</v>
-      </c>
-      <c r="C29" s="31" t="s">
+      <c r="D29" s="74">
+        <v>5</v>
+      </c>
+      <c r="E29" s="71" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="75"/>
+      <c r="C30" s="102" t="s">
         <v>97</v>
       </c>
-      <c r="D29" s="82">
-        <v>5</v>
-      </c>
-      <c r="E29" s="95" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="30" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="83"/>
-      <c r="C30" s="32" t="s">
+      <c r="D30" s="75"/>
+      <c r="E30" s="54"/>
+    </row>
+    <row r="31" spans="2:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="72">
+        <v>51</v>
+      </c>
+      <c r="C31" s="100" t="s">
         <v>98</v>
       </c>
-      <c r="D30" s="83"/>
-      <c r="E30" s="75"/>
-    </row>
-    <row r="31" spans="2:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="80">
-        <v>51</v>
-      </c>
-      <c r="C31" s="33" t="s">
+      <c r="D31" s="27" t="s">
+        <v>100</v>
+      </c>
+      <c r="E31" s="54" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="73"/>
+      <c r="C32" s="102" t="s">
         <v>99</v>
       </c>
-      <c r="D31" s="33" t="s">
+      <c r="D32" s="28" t="s">
         <v>101</v>
       </c>
-      <c r="E31" s="75" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="32" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="81"/>
-      <c r="C32" s="30" t="s">
-        <v>100</v>
-      </c>
-      <c r="D32" s="34" t="s">
+      <c r="E32" s="54"/>
+    </row>
+    <row r="33" spans="2:5" s="40" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B33" s="87">
+        <v>52</v>
+      </c>
+      <c r="C33" s="100" t="s">
         <v>102</v>
       </c>
-      <c r="E32" s="75"/>
-    </row>
-    <row r="33" spans="2:5" s="47" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B33" s="78">
-        <v>52</v>
-      </c>
-      <c r="C33" s="53" t="s">
+      <c r="D33" s="87" t="s">
+        <v>104</v>
+      </c>
+      <c r="E33" s="55" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" s="40" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="88"/>
+      <c r="C34" s="102" t="s">
         <v>103</v>
       </c>
-      <c r="D33" s="78" t="s">
+      <c r="D34" s="88"/>
+      <c r="E34" s="55"/>
+    </row>
+    <row r="35" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B35" s="72">
+        <v>53</v>
+      </c>
+      <c r="C35" s="27" t="s">
         <v>105</v>
       </c>
-      <c r="E33" s="76" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="34" spans="2:5" s="47" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="79"/>
-      <c r="C34" s="54" t="s">
-        <v>104</v>
-      </c>
-      <c r="D34" s="79"/>
-      <c r="E34" s="76"/>
-    </row>
-    <row r="35" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B35" s="80">
-        <v>53</v>
-      </c>
-      <c r="C35" s="33" t="s">
+      <c r="D35" s="72" t="s">
+        <v>107</v>
+      </c>
+      <c r="E35" s="54" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="73"/>
+      <c r="C36" s="24" t="s">
         <v>106</v>
       </c>
-      <c r="D35" s="80" t="s">
+      <c r="D36" s="73"/>
+      <c r="E36" s="54"/>
+    </row>
+    <row r="37" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B37" s="74">
+        <v>54</v>
+      </c>
+      <c r="C37" s="25" t="s">
         <v>108</v>
       </c>
-      <c r="E35" s="75" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="36" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="81"/>
-      <c r="C36" s="30" t="s">
-        <v>107</v>
-      </c>
-      <c r="D36" s="81"/>
-      <c r="E36" s="75"/>
-    </row>
-    <row r="37" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B37" s="82">
-        <v>54</v>
-      </c>
-      <c r="C37" s="31" t="s">
+      <c r="D37" s="74" t="s">
+        <v>110</v>
+      </c>
+      <c r="E37" s="54" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="75"/>
+      <c r="C38" s="26" t="s">
         <v>109</v>
       </c>
-      <c r="D37" s="82" t="s">
+      <c r="D38" s="75"/>
+      <c r="E38" s="54"/>
+    </row>
+    <row r="39" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="28">
+        <v>55</v>
+      </c>
+      <c r="C39" s="29" t="s">
         <v>111</v>
       </c>
-      <c r="E37" s="75" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="38" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="83"/>
-      <c r="C38" s="32" t="s">
-        <v>110</v>
-      </c>
-      <c r="D38" s="83"/>
-      <c r="E38" s="75"/>
-    </row>
-    <row r="39" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="34">
-        <v>55</v>
-      </c>
-      <c r="C39" s="35" t="s">
+      <c r="D39" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="E39" s="32" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="106">
+        <v>56</v>
+      </c>
+      <c r="C40" s="101" t="s">
         <v>112</v>
       </c>
-      <c r="D39" s="34" t="s">
-        <v>36</v>
-      </c>
-      <c r="E39" s="39" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="40" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="36">
-        <v>56</v>
-      </c>
-      <c r="C40" s="36" t="s">
+      <c r="D40" s="30" t="s">
         <v>113</v>
       </c>
-      <c r="D40" s="36" t="s">
+      <c r="E40" s="32" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="106">
+        <v>57</v>
+      </c>
+      <c r="C41" s="101" t="s">
         <v>114</v>
       </c>
-      <c r="E40" s="39" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="41" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="34">
-        <v>57</v>
-      </c>
-      <c r="C41" s="34" t="s">
+      <c r="D41" s="28" t="s">
         <v>115</v>
       </c>
-      <c r="D41" s="34" t="s">
+      <c r="E41" s="32" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="86">
+        <v>58</v>
+      </c>
+      <c r="C42" s="103" t="s">
         <v>116</v>
       </c>
-      <c r="E41" s="39" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="42" spans="2:5" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="84">
-        <v>58</v>
-      </c>
-      <c r="C42" s="37" t="s">
+      <c r="D42" s="86" t="s">
+        <v>35</v>
+      </c>
+      <c r="E42" s="54" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B43" s="75"/>
+      <c r="C43" s="102" t="s">
         <v>117</v>
       </c>
-      <c r="D42" s="84" t="s">
-        <v>36</v>
-      </c>
-      <c r="E42" s="75" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="43" spans="2:5" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="83"/>
-      <c r="C43" s="32" t="s">
+      <c r="D43" s="75"/>
+      <c r="E43" s="54"/>
+    </row>
+    <row r="44" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B44" s="104">
+        <v>59</v>
+      </c>
+      <c r="C44" s="100" t="s">
         <v>118</v>
       </c>
-      <c r="D43" s="83"/>
-      <c r="E43" s="75"/>
-    </row>
-    <row r="44" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B44" s="80">
-        <v>59</v>
-      </c>
-      <c r="C44" s="33" t="s">
+      <c r="D44" s="72" t="s">
+        <v>35</v>
+      </c>
+      <c r="E44" s="54" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B45" s="105"/>
+      <c r="C45" s="102" t="s">
         <v>119</v>
       </c>
-      <c r="D44" s="80" t="s">
-        <v>36</v>
-      </c>
-      <c r="E44" s="75" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="45" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="81"/>
-      <c r="C45" s="30" t="s">
+      <c r="D45" s="73"/>
+      <c r="E45" s="54"/>
+    </row>
+    <row r="46" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B46" s="106">
+        <v>60</v>
+      </c>
+      <c r="C46" s="101" t="s">
         <v>120</v>
       </c>
-      <c r="D45" s="81"/>
-      <c r="E45" s="75"/>
-    </row>
-    <row r="46" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="36">
-        <v>60</v>
-      </c>
-      <c r="C46" s="36" t="s">
+      <c r="D46" s="30" t="s">
         <v>121</v>
       </c>
-      <c r="D46" s="36" t="s">
+      <c r="E46" s="32" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5" s="40" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B47" s="45">
+        <v>61</v>
+      </c>
+      <c r="C47" s="101" t="s">
         <v>122</v>
       </c>
-      <c r="E46" s="39" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="47" spans="2:5" s="47" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="52">
-        <v>61</v>
-      </c>
-      <c r="C47" s="52" t="s">
+      <c r="D47" s="45" t="s">
         <v>123</v>
       </c>
-      <c r="D47" s="52" t="s">
+      <c r="E47" s="38" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="48" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B48" s="30">
+        <v>62</v>
+      </c>
+      <c r="C48" s="101" t="s">
+        <v>26</v>
+      </c>
+      <c r="D48" s="30" t="s">
         <v>124</v>
       </c>
-      <c r="E47" s="45" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="48" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="36">
-        <v>62</v>
-      </c>
-      <c r="C48" s="36" t="s">
-        <v>26</v>
-      </c>
-      <c r="D48" s="36" t="s">
+      <c r="E48" s="32" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="49" spans="2:5" s="40" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B49" s="87">
+        <v>63</v>
+      </c>
+      <c r="C49" s="100" t="s">
         <v>125</v>
       </c>
-      <c r="E48" s="39" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="49" spans="2:5" s="47" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B49" s="78">
-        <v>63</v>
-      </c>
-      <c r="C49" s="53" t="s">
+      <c r="D49" s="87" t="s">
+        <v>127</v>
+      </c>
+      <c r="E49" s="55" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="50" spans="2:5" s="40" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B50" s="88"/>
+      <c r="C50" s="102" t="s">
         <v>126</v>
       </c>
-      <c r="D49" s="78" t="s">
+      <c r="D50" s="88"/>
+      <c r="E50" s="55"/>
+    </row>
+    <row r="51" spans="2:5" s="40" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B51" s="87">
+        <v>64</v>
+      </c>
+      <c r="C51" s="100" t="s">
         <v>128</v>
       </c>
-      <c r="E49" s="76" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="50" spans="2:5" s="47" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="79"/>
-      <c r="C50" s="54" t="s">
-        <v>127</v>
-      </c>
-      <c r="D50" s="79"/>
-      <c r="E50" s="76"/>
-    </row>
-    <row r="51" spans="2:5" s="47" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B51" s="78">
-        <v>64</v>
-      </c>
-      <c r="C51" s="53" t="s">
+      <c r="D51" s="87" t="s">
+        <v>130</v>
+      </c>
+      <c r="E51" s="55" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="52" spans="2:5" s="40" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B52" s="88"/>
+      <c r="C52" s="102" t="s">
         <v>129</v>
       </c>
-      <c r="D51" s="78" t="s">
+      <c r="D52" s="88"/>
+      <c r="E52" s="55"/>
+    </row>
+    <row r="53" spans="2:5" s="40" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B53" s="87">
+        <v>65</v>
+      </c>
+      <c r="C53" s="100" t="s">
         <v>131</v>
       </c>
-      <c r="E51" s="76" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="52" spans="2:5" s="47" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="79"/>
-      <c r="C52" s="54" t="s">
-        <v>130</v>
-      </c>
-      <c r="D52" s="79"/>
-      <c r="E52" s="76"/>
-    </row>
-    <row r="53" spans="2:5" s="47" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B53" s="78">
-        <v>65</v>
-      </c>
-      <c r="C53" s="53" t="s">
+      <c r="D53" s="87" t="s">
+        <v>133</v>
+      </c>
+      <c r="E53" s="55" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="54" spans="2:5" s="40" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B54" s="88"/>
+      <c r="C54" s="102" t="s">
         <v>132</v>
       </c>
-      <c r="D53" s="78" t="s">
+      <c r="D54" s="88"/>
+      <c r="E54" s="55"/>
+    </row>
+    <row r="55" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B55" s="30">
+        <v>66</v>
+      </c>
+      <c r="C55" s="30" t="s">
         <v>134</v>
       </c>
-      <c r="E53" s="76" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="54" spans="2:5" s="47" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="79"/>
-      <c r="C54" s="54" t="s">
-        <v>133</v>
-      </c>
-      <c r="D54" s="79"/>
-      <c r="E54" s="76"/>
-    </row>
-    <row r="55" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B55" s="36">
-        <v>66</v>
-      </c>
-      <c r="C55" s="36" t="s">
+      <c r="D55" s="30" t="s">
         <v>135</v>
       </c>
-      <c r="D55" s="36" t="s">
+      <c r="E55" s="32" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="56" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B56" s="28">
+        <v>67</v>
+      </c>
+      <c r="C56" s="28" t="s">
         <v>136</v>
       </c>
-      <c r="E55" s="39" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="56" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B56" s="34">
-        <v>67</v>
-      </c>
-      <c r="C56" s="34" t="s">
+      <c r="D56" s="28" t="s">
         <v>137</v>
       </c>
-      <c r="D56" s="34" t="s">
+      <c r="E56" s="32" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="57" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B57" s="30">
+        <v>68</v>
+      </c>
+      <c r="C57" s="30" t="s">
         <v>138</v>
       </c>
-      <c r="E56" s="39" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="57" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B57" s="36">
-        <v>68</v>
-      </c>
-      <c r="C57" s="36" t="s">
+      <c r="D57" s="30" t="s">
         <v>139</v>
       </c>
-      <c r="D57" s="36" t="s">
+      <c r="E57" s="32" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="58" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B58" s="28">
+        <v>69</v>
+      </c>
+      <c r="C58" s="28" t="s">
         <v>140</v>
       </c>
-      <c r="E57" s="39" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="58" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B58" s="34">
-        <v>69</v>
-      </c>
-      <c r="C58" s="34" t="s">
+      <c r="D58" s="28" t="s">
         <v>141</v>
       </c>
-      <c r="D58" s="34" t="s">
+      <c r="E58" s="32" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="59" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B59" s="30">
+        <v>70</v>
+      </c>
+      <c r="C59" s="30" t="s">
         <v>142</v>
       </c>
-      <c r="E58" s="39" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="59" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B59" s="36">
-        <v>70</v>
-      </c>
-      <c r="C59" s="36" t="s">
+      <c r="D59" s="30" t="s">
         <v>143</v>
       </c>
-      <c r="D59" s="36" t="s">
+      <c r="E59" s="32" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="60" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B60" s="28">
+        <v>71</v>
+      </c>
+      <c r="C60" s="28" t="s">
         <v>144</v>
       </c>
-      <c r="E59" s="39" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="60" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B60" s="34">
-        <v>71</v>
-      </c>
-      <c r="C60" s="34" t="s">
+      <c r="D60" s="28" t="s">
+        <v>143</v>
+      </c>
+      <c r="E60" s="32" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="61" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B61" s="30">
+        <v>72</v>
+      </c>
+      <c r="C61" s="30" t="s">
         <v>145</v>
       </c>
-      <c r="D60" s="34" t="s">
-        <v>144</v>
-      </c>
-      <c r="E60" s="39" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="61" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B61" s="36">
-        <v>72</v>
-      </c>
-      <c r="C61" s="36" t="s">
+      <c r="D61" s="30" t="s">
+        <v>143</v>
+      </c>
+      <c r="E61" s="32" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="62" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B62" s="28">
+        <v>73</v>
+      </c>
+      <c r="C62" s="28" t="s">
         <v>146</v>
       </c>
-      <c r="D61" s="36" t="s">
-        <v>144</v>
-      </c>
-      <c r="E61" s="39" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="62" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B62" s="34">
-        <v>73</v>
-      </c>
-      <c r="C62" s="34" t="s">
+      <c r="D62" s="28" t="s">
+        <v>143</v>
+      </c>
+      <c r="E62" s="32" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="63" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B63" s="30">
+        <v>74</v>
+      </c>
+      <c r="C63" s="30" t="s">
         <v>147</v>
       </c>
-      <c r="D62" s="34" t="s">
-        <v>144</v>
-      </c>
-      <c r="E62" s="39" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="63" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B63" s="36">
-        <v>74</v>
-      </c>
-      <c r="C63" s="36" t="s">
+      <c r="D63" s="30" t="s">
+        <v>143</v>
+      </c>
+      <c r="E63" s="32" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="64" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B64" s="19">
+        <v>75</v>
+      </c>
+      <c r="C64" s="19" t="s">
         <v>148</v>
       </c>
-      <c r="D63" s="36" t="s">
-        <v>144</v>
-      </c>
-      <c r="E63" s="39" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="64" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B64" s="24">
-        <v>75</v>
-      </c>
-      <c r="C64" s="24" t="s">
-        <v>149</v>
-      </c>
-      <c r="D64" s="24" t="s">
-        <v>144</v>
-      </c>
-      <c r="E64" s="39" t="s">
-        <v>266</v>
+      <c r="D64" s="19" t="s">
+        <v>143</v>
+      </c>
+      <c r="E64" s="32" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="65" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -3689,13 +3718,13 @@
         <v>76</v>
       </c>
       <c r="C65" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="D65" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="D65" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="E65" s="39" t="s">
-        <v>266</v>
+      <c r="E65" s="32" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="66" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -3703,13 +3732,13 @@
         <v>77</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="E66" s="39" t="s">
-        <v>266</v>
+        <v>143</v>
+      </c>
+      <c r="E66" s="32" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="67" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -3717,13 +3746,13 @@
         <v>78</v>
       </c>
       <c r="C67" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="D67" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="D67" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="E67" s="39" t="s">
-        <v>266</v>
+      <c r="E67" s="32" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="68" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -3731,13 +3760,13 @@
         <v>79</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="E68" s="39" t="s">
-        <v>266</v>
+        <v>70</v>
+      </c>
+      <c r="E68" s="32" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="69" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -3745,13 +3774,13 @@
         <v>80</v>
       </c>
       <c r="C69" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D69" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="D69" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="E69" s="39" t="s">
-        <v>266</v>
+      <c r="E69" s="32" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="70" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -3759,13 +3788,13 @@
         <v>81</v>
       </c>
       <c r="C70" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="D70" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="D70" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="E70" s="39" t="s">
-        <v>266</v>
+      <c r="E70" s="32" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="71" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -3773,13 +3802,13 @@
         <v>82</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D71" s="2">
         <v>110</v>
       </c>
-      <c r="E71" s="39" t="s">
-        <v>266</v>
+      <c r="E71" s="32" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="72" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -3787,13 +3816,13 @@
         <v>83</v>
       </c>
       <c r="C72" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="D72" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="D72" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="E72" s="39" t="s">
-        <v>266</v>
+      <c r="E72" s="32" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="73" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -3801,27 +3830,27 @@
         <v>84</v>
       </c>
       <c r="C73" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="D73" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="D73" s="2" t="s">
+      <c r="E73" s="32" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="74" spans="2:5" s="40" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B74" s="37">
+        <v>85</v>
+      </c>
+      <c r="C74" s="37" t="s">
         <v>164</v>
       </c>
-      <c r="E73" s="39" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="74" spans="2:5" s="47" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B74" s="44">
-        <v>85</v>
-      </c>
-      <c r="C74" s="44" t="s">
+      <c r="D74" s="37" t="s">
         <v>165</v>
       </c>
-      <c r="D74" s="44" t="s">
-        <v>166</v>
-      </c>
-      <c r="E74" s="45" t="s">
-        <v>266</v>
+      <c r="E74" s="38" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="75" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -3829,13 +3858,13 @@
         <v>86</v>
       </c>
       <c r="C75" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="D75" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="D75" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="E75" s="39" t="s">
-        <v>266</v>
+      <c r="E75" s="32" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="76" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -3843,13 +3872,13 @@
         <v>87</v>
       </c>
       <c r="C76" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="D76" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="D76" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="E76" s="39" t="s">
-        <v>266</v>
+      <c r="E76" s="32" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="77" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -3857,13 +3886,13 @@
         <v>88</v>
       </c>
       <c r="C77" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="D77" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="D77" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="E77" s="39" t="s">
-        <v>266</v>
+      <c r="E77" s="32" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="78" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -3871,13 +3900,13 @@
         <v>89</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="D78" s="28">
+        <v>172</v>
+      </c>
+      <c r="D78" s="23">
         <v>44088</v>
       </c>
-      <c r="E78" s="39" t="s">
-        <v>266</v>
+      <c r="E78" s="32" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="79" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -3885,7 +3914,7 @@
         <v>90</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D79" s="3">
         <v>43178</v>
@@ -3896,17 +3925,69 @@
         <v>91</v>
       </c>
       <c r="C80" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="D80" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="D80" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="E80" s="39" t="s">
-        <v>266</v>
+      <c r="E80" s="32" t="s">
+        <v>265</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="68">
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="D51:D52"/>
+    <mergeCell ref="B53:B54"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="D49:D50"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E33:E34"/>
+    <mergeCell ref="E35:E36"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="E31:E32"/>
     <mergeCell ref="E49:E50"/>
     <mergeCell ref="E51:E52"/>
     <mergeCell ref="E53:E54"/>
@@ -3923,58 +4004,6 @@
     <mergeCell ref="E13:E14"/>
     <mergeCell ref="E15:E16"/>
     <mergeCell ref="E21:E22"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="E33:E34"/>
-    <mergeCell ref="E35:E36"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="D42:D43"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="D51:D52"/>
-    <mergeCell ref="B53:B54"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="D44:D45"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="D49:D50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3984,8 +4013,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView topLeftCell="B7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3993,237 +4022,232 @@
     <col min="2" max="2" width="7.85546875" customWidth="1"/>
     <col min="3" max="3" width="56.85546875" customWidth="1"/>
     <col min="4" max="4" width="100" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="39"/>
+    <col min="5" max="5" width="9.140625" style="32"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E1" s="39" t="s">
-        <v>259</v>
+      <c r="E1" s="32" t="s">
+        <v>258</v>
       </c>
       <c r="F1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="2" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B2" s="71">
+      <c r="B2" s="63">
         <v>92</v>
       </c>
       <c r="C2" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="D2" s="63" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="54" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="61"/>
+      <c r="C3" s="7" t="s">
         <v>178</v>
       </c>
-      <c r="D2" s="71" t="s">
-        <v>36</v>
-      </c>
-      <c r="E2" s="75" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="3" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="67"/>
-      <c r="C3" s="7" t="s">
+      <c r="D3" s="61"/>
+      <c r="E3" s="54"/>
+    </row>
+    <row r="4" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B4" s="58">
+        <v>93</v>
+      </c>
+      <c r="C4" s="51" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="58" t="s">
+        <v>70</v>
+      </c>
+      <c r="E4" s="54" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="62"/>
+      <c r="C5" s="97" t="s">
         <v>179</v>
       </c>
-      <c r="D3" s="67"/>
-      <c r="E3" s="75"/>
-    </row>
-    <row r="4" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B4" s="62">
-        <v>93</v>
-      </c>
-      <c r="C4" s="98" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="62" t="s">
-        <v>71</v>
-      </c>
-      <c r="E4" s="75" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="63"/>
-      <c r="C5" s="9" t="s">
+      <c r="D5" s="62"/>
+      <c r="E5" s="54"/>
+    </row>
+    <row r="6" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B6" s="60">
+        <v>94</v>
+      </c>
+      <c r="C6" s="51" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="60" t="s">
+        <v>181</v>
+      </c>
+      <c r="E6" s="54" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="61"/>
+      <c r="C7" s="97" t="s">
         <v>180</v>
       </c>
-      <c r="D5" s="63"/>
-      <c r="E5" s="75"/>
-    </row>
-    <row r="6" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B6" s="66">
-        <v>94</v>
-      </c>
-      <c r="C6" s="98" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="66" t="s">
-        <v>182</v>
-      </c>
-      <c r="E6" s="75" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="67"/>
-      <c r="C7" s="7" t="s">
-        <v>181</v>
-      </c>
-      <c r="D7" s="67"/>
-      <c r="E7" s="75"/>
+      <c r="D7" s="61"/>
+      <c r="E7" s="54"/>
     </row>
     <row r="8" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="4">
         <v>95</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="E8" s="39" t="s">
-        <v>266</v>
+        <v>70</v>
+      </c>
+      <c r="E8" s="32" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="9" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="2">
         <v>96</v>
       </c>
-      <c r="C9" s="99" t="s">
+      <c r="C9" s="52" t="s">
+        <v>183</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="E9" s="39" t="s">
-        <v>266</v>
+      <c r="E9" s="32" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="10" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="4">
         <v>97</v>
       </c>
-      <c r="C10" s="99" t="s">
+      <c r="C10" s="52" t="s">
+        <v>185</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="E10" s="32" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" s="40" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="37">
+        <v>98</v>
+      </c>
+      <c r="C11" s="52" t="s">
         <v>187</v>
       </c>
-      <c r="E10" s="39" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" s="47" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="44">
-        <v>98</v>
-      </c>
-      <c r="C11" s="99" t="s">
+      <c r="D11" s="37" t="s">
         <v>188</v>
       </c>
-      <c r="D11" s="44" t="s">
+      <c r="E11" s="38" t="s">
+        <v>265</v>
+      </c>
+      <c r="F11" s="39"/>
+    </row>
+    <row r="12" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B12" s="92">
+        <v>99</v>
+      </c>
+      <c r="C12" s="93" t="s">
         <v>189</v>
       </c>
-      <c r="E11" s="45" t="s">
-        <v>266</v>
-      </c>
-      <c r="F11" s="46"/>
-    </row>
-    <row r="12" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B12" s="97">
-        <v>99</v>
-      </c>
-      <c r="C12" s="101" t="s">
+      <c r="D12" s="22" t="s">
         <v>190</v>
       </c>
-      <c r="D12" s="27" t="s">
+      <c r="E12" s="54" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B13" s="59"/>
+      <c r="C13" s="90"/>
+      <c r="D13" s="8" t="s">
         <v>191</v>
       </c>
-      <c r="E12" s="75" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B13" s="70"/>
-      <c r="C13" s="102"/>
-      <c r="D13" s="8" t="s">
+      <c r="E13" s="54"/>
+    </row>
+    <row r="14" spans="2:6" ht="33" x14ac:dyDescent="0.25">
+      <c r="B14" s="59"/>
+      <c r="C14" s="90"/>
+      <c r="D14" s="8" t="s">
         <v>192</v>
       </c>
-      <c r="E13" s="75"/>
-    </row>
-    <row r="14" spans="2:6" ht="33" x14ac:dyDescent="0.25">
-      <c r="B14" s="70"/>
-      <c r="C14" s="102"/>
-      <c r="D14" s="8" t="s">
+      <c r="E14" s="54"/>
+    </row>
+    <row r="15" spans="2:6" ht="49.5" x14ac:dyDescent="0.25">
+      <c r="B15" s="59"/>
+      <c r="C15" s="90"/>
+      <c r="D15" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="E14" s="75"/>
-    </row>
-    <row r="15" spans="2:6" ht="49.5" x14ac:dyDescent="0.25">
-      <c r="B15" s="70"/>
-      <c r="C15" s="102"/>
-      <c r="D15" s="8" t="s">
+      <c r="E15" s="54"/>
+    </row>
+    <row r="16" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="62"/>
+      <c r="C16" s="91"/>
+      <c r="D16" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="E15" s="75"/>
-    </row>
-    <row r="16" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="63"/>
-      <c r="C16" s="103"/>
-      <c r="D16" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="E16" s="75"/>
+      <c r="E16" s="54"/>
     </row>
     <row r="17" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="2">
         <v>100</v>
       </c>
-      <c r="C17" s="99" t="s">
+      <c r="C17" s="52" t="s">
+        <v>195</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="E17" s="32" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B18" s="58">
+        <v>101</v>
+      </c>
+      <c r="C18" s="89" t="s">
         <v>197</v>
       </c>
-      <c r="E17" s="39" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B18" s="62">
-        <v>101</v>
-      </c>
-      <c r="C18" s="104" t="s">
+      <c r="D18" s="8" t="s">
         <v>198</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="E18" s="54" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B19" s="59"/>
+      <c r="C19" s="90"/>
+      <c r="D19" s="8" t="s">
         <v>199</v>
       </c>
-      <c r="E18" s="75" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B19" s="70"/>
-      <c r="C19" s="102"/>
-      <c r="D19" s="8" t="s">
+      <c r="E19" s="54"/>
+    </row>
+    <row r="20" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="62"/>
+      <c r="C20" s="91"/>
+      <c r="D20" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="E19" s="75"/>
-    </row>
-    <row r="20" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="63"/>
-      <c r="C20" s="103"/>
-      <c r="D20" s="4" t="s">
-        <v>201</v>
-      </c>
-      <c r="E20" s="75"/>
+      <c r="E20" s="54"/>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="E12:E16"/>
-    <mergeCell ref="E18:E20"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="B4:B5"/>
@@ -4234,6 +4258,11 @@
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="B12:B16"/>
     <mergeCell ref="C12:C16"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="E12:E16"/>
+    <mergeCell ref="E18:E20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4243,8 +4272,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4252,401 +4281,407 @@
     <col min="2" max="2" width="4.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="59" customWidth="1"/>
     <col min="4" max="4" width="52.7109375" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="39"/>
+    <col min="5" max="5" width="9.140625" style="32"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E1" s="39" t="s">
-        <v>48</v>
+      <c r="E1" s="32" t="s">
+        <v>47</v>
       </c>
       <c r="F1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="2" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B2" s="71">
+      <c r="B2" s="63">
         <v>102</v>
       </c>
       <c r="C2" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="D2" s="63" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="54" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="61"/>
+      <c r="C3" s="7" t="s">
         <v>178</v>
       </c>
-      <c r="D2" s="71" t="s">
-        <v>36</v>
-      </c>
-      <c r="E2" s="75" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="3" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="67"/>
-      <c r="C3" s="7" t="s">
+      <c r="D3" s="61"/>
+      <c r="E3" s="54"/>
+    </row>
+    <row r="4" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B4" s="58">
+        <v>103</v>
+      </c>
+      <c r="C4" s="51" t="s">
+        <v>201</v>
+      </c>
+      <c r="D4" s="58" t="s">
+        <v>70</v>
+      </c>
+      <c r="E4" s="54" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="62"/>
+      <c r="C5" s="97" t="s">
         <v>179</v>
       </c>
-      <c r="D3" s="67"/>
-      <c r="E3" s="75"/>
-    </row>
-    <row r="4" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B4" s="62">
-        <v>103</v>
-      </c>
-      <c r="C4" s="98" t="s">
-        <v>202</v>
-      </c>
-      <c r="D4" s="62" t="s">
-        <v>71</v>
-      </c>
-      <c r="E4" s="75" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="63"/>
-      <c r="C5" s="9" t="s">
+      <c r="D5" s="62"/>
+      <c r="E5" s="54"/>
+    </row>
+    <row r="6" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B6" s="60">
+        <v>104</v>
+      </c>
+      <c r="C6" s="51" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="60" t="s">
+        <v>181</v>
+      </c>
+      <c r="E6" s="54" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="61"/>
+      <c r="C7" s="97" t="s">
         <v>180</v>
       </c>
-      <c r="D5" s="63"/>
-      <c r="E5" s="75"/>
-    </row>
-    <row r="6" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B6" s="66">
-        <v>104</v>
-      </c>
-      <c r="C6" s="98" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="66" t="s">
-        <v>182</v>
-      </c>
-      <c r="E6" s="75" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="67"/>
-      <c r="C7" s="7" t="s">
-        <v>181</v>
-      </c>
-      <c r="D7" s="67"/>
-      <c r="E7" s="75"/>
+      <c r="D7" s="61"/>
+      <c r="E7" s="54"/>
     </row>
     <row r="8" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="4">
         <v>105</v>
       </c>
-      <c r="C8" s="99" t="s">
+      <c r="C8" s="52" t="s">
+        <v>202</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>204</v>
-      </c>
-      <c r="E8" s="39" t="s">
-        <v>266</v>
+      <c r="E8" s="32" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="9" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="2">
         <v>106</v>
       </c>
-      <c r="C9" s="99" t="s">
+      <c r="C9" s="52" t="s">
+        <v>204</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="E9" s="39" t="s">
-        <v>266</v>
+      <c r="E9" s="32" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="10" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="4">
         <v>107</v>
       </c>
-      <c r="C10" s="99" t="s">
+      <c r="C10" s="52" t="s">
+        <v>206</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>207</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>208</v>
-      </c>
-      <c r="E10" s="39" t="s">
-        <v>266</v>
+      <c r="E10" s="32" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="11" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="2">
         <v>108</v>
       </c>
-      <c r="C11" s="99" t="s">
+      <c r="C11" s="52" t="s">
+        <v>208</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F11" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" s="40" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="37">
+        <v>109</v>
+      </c>
+      <c r="C12" s="52" t="s">
         <v>209</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="F11" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" s="47" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="44">
-        <v>109</v>
-      </c>
-      <c r="C12" s="99" t="s">
+      <c r="D12" s="37" t="s">
         <v>210</v>
       </c>
-      <c r="D12" s="44" t="s">
+      <c r="E12" s="38" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" s="40" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="37">
+        <v>110</v>
+      </c>
+      <c r="C13" s="52" t="s">
         <v>211</v>
       </c>
-      <c r="E12" s="45" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" s="47" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="44">
-        <v>110</v>
-      </c>
-      <c r="C13" s="99" t="s">
+      <c r="D13" s="37" t="s">
         <v>212</v>
       </c>
-      <c r="D13" s="44" t="s">
+      <c r="E13" s="38" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" s="40" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="37">
+        <v>111</v>
+      </c>
+      <c r="C14" s="52" t="s">
         <v>213</v>
       </c>
-      <c r="E13" s="45" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" s="47" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="44">
-        <v>111</v>
-      </c>
-      <c r="C14" s="99" t="s">
-        <v>214</v>
-      </c>
-      <c r="D14" s="44">
+      <c r="D14" s="37">
         <v>0</v>
       </c>
-      <c r="E14" s="45" t="s">
-        <v>266</v>
+      <c r="E14" s="38" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="15" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="24">
+      <c r="B15" s="19">
         <v>112</v>
       </c>
-      <c r="C15" s="100" t="s">
-        <v>78</v>
-      </c>
-      <c r="D15" s="24" t="s">
-        <v>80</v>
-      </c>
-      <c r="E15" s="39" t="s">
-        <v>266</v>
+      <c r="C15" s="53" t="s">
+        <v>77</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="E15" s="32" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="16" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="4">
         <v>113</v>
       </c>
-      <c r="C16" s="99" t="s">
+      <c r="C16" s="52" t="s">
+        <v>214</v>
+      </c>
+      <c r="D16" s="4" t="s">
         <v>215</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="E16" s="32" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" s="40" customFormat="1" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="37">
+        <v>114</v>
+      </c>
+      <c r="C17" s="52" t="s">
         <v>216</v>
       </c>
-      <c r="E16" s="39" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" s="47" customFormat="1" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="44">
-        <v>114</v>
-      </c>
-      <c r="C17" s="99" t="s">
+      <c r="D17" s="37" t="s">
         <v>217</v>
       </c>
-      <c r="D17" s="44" t="s">
-        <v>218</v>
-      </c>
-      <c r="E17" s="45" t="s">
-        <v>266</v>
+      <c r="E17" s="38" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="18" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="4">
         <v>115</v>
       </c>
-      <c r="C18" s="99" t="s">
+      <c r="C18" s="52" t="s">
+        <v>218</v>
+      </c>
+      <c r="D18" s="4" t="s">
         <v>219</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="E18" s="32" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" s="40" customFormat="1" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="37">
+        <v>116</v>
+      </c>
+      <c r="C19" s="52" t="s">
         <v>220</v>
       </c>
-      <c r="E18" s="39" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" s="47" customFormat="1" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="44">
-        <v>116</v>
-      </c>
-      <c r="C19" s="99" t="s">
+      <c r="D19" s="37" t="s">
         <v>221</v>
       </c>
-      <c r="D19" s="44" t="s">
+      <c r="E19" s="38" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B20" s="58">
+        <v>117</v>
+      </c>
+      <c r="C20" s="8" t="s">
         <v>222</v>
       </c>
-      <c r="E19" s="45" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B20" s="62">
-        <v>117</v>
-      </c>
-      <c r="C20" s="8" t="s">
+      <c r="D20" s="58" t="s">
+        <v>55</v>
+      </c>
+      <c r="E20" s="54"/>
+    </row>
+    <row r="21" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="62"/>
+      <c r="C21" s="4" t="s">
         <v>223</v>
       </c>
-      <c r="D20" s="62" t="s">
-        <v>56</v>
-      </c>
-      <c r="E20" s="75"/>
-    </row>
-    <row r="21" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="63"/>
-      <c r="C21" s="4" t="s">
-        <v>224</v>
-      </c>
-      <c r="D21" s="63"/>
-      <c r="E21" s="75"/>
+      <c r="D21" s="62"/>
+      <c r="E21" s="54"/>
     </row>
     <row r="22" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="2">
         <v>118</v>
       </c>
       <c r="C22" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>225</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="23" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="4">
         <v>119</v>
       </c>
-      <c r="C23" s="99" t="s">
+      <c r="C23" s="52" t="s">
+        <v>226</v>
+      </c>
+      <c r="D23" s="4" t="s">
         <v>227</v>
       </c>
-      <c r="D23" s="4" t="s">
-        <v>228</v>
-      </c>
-      <c r="E23" s="39" t="s">
-        <v>266</v>
+      <c r="E23" s="32" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="24" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="2">
         <v>120</v>
       </c>
-      <c r="C24" s="99" t="s">
+      <c r="C24" s="52" t="s">
+        <v>228</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="D24" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="E24" s="39" t="s">
-        <v>266</v>
+      <c r="E24" s="32" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="25" spans="2:5" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="4">
         <v>121</v>
       </c>
-      <c r="C25" s="99" t="s">
+      <c r="C25" s="52" t="s">
+        <v>230</v>
+      </c>
+      <c r="D25" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="D25" s="4" t="s">
-        <v>232</v>
-      </c>
-      <c r="E25" s="39" t="s">
-        <v>266</v>
+      <c r="E25" s="32" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="26" spans="2:5" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="2">
         <v>122</v>
       </c>
-      <c r="C26" s="99" t="s">
+      <c r="C26" s="52" t="s">
+        <v>232</v>
+      </c>
+      <c r="D26" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="D26" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="E26" s="39" t="s">
-        <v>266</v>
+      <c r="E26" s="32" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="27" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="4">
         <v>123</v>
       </c>
-      <c r="C27" s="99" t="s">
+      <c r="C27" s="52" t="s">
+        <v>234</v>
+      </c>
+      <c r="D27" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="D27" s="4" t="s">
-        <v>236</v>
-      </c>
-      <c r="E27" s="39" t="s">
-        <v>266</v>
+      <c r="E27" s="32" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="28" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="2">
         <v>124</v>
       </c>
-      <c r="C28" s="99" t="s">
+      <c r="C28" s="52" t="s">
+        <v>236</v>
+      </c>
+      <c r="D28" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="D28" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="E28" s="39" t="s">
-        <v>266</v>
+      <c r="E28" s="32" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="29" spans="2:5" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B29" s="4">
         <v>125</v>
       </c>
-      <c r="C29" s="99" t="s">
+      <c r="C29" s="52" t="s">
+        <v>238</v>
+      </c>
+      <c r="D29" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="D29" s="4" t="s">
+      <c r="E29" s="32" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B30" s="60">
+        <v>126</v>
+      </c>
+      <c r="C30" s="51" t="s">
+        <v>266</v>
+      </c>
+      <c r="D30" s="60" t="s">
         <v>240</v>
       </c>
-      <c r="E29" s="39" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="30" spans="2:5" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B30" s="66">
-        <v>126</v>
-      </c>
-      <c r="C30" s="98" t="s">
-        <v>267</v>
-      </c>
-      <c r="D30" s="66" t="s">
-        <v>241</v>
-      </c>
-      <c r="E30" s="39" t="s">
-        <v>266</v>
+      <c r="E30" s="32" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="31" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="67"/>
+      <c r="B31" s="61"/>
       <c r="C31" s="2"/>
-      <c r="D31" s="67"/>
+      <c r="D31" s="61"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="D20:D21"/>
     <mergeCell ref="E20:E21"/>
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="E4:E5"/>
@@ -4655,12 +4690,6 @@
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="D4:D5"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="D20:D21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4670,7 +4699,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F12"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -4682,21 +4711,21 @@
   <sheetData>
     <row r="1" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E1" t="s">
+        <v>258</v>
+      </c>
+      <c r="F1" t="s">
         <v>259</v>
       </c>
-      <c r="F1" t="s">
-        <v>260</v>
-      </c>
     </row>
     <row r="2" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="24">
+      <c r="B2" s="19">
         <v>127</v>
       </c>
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="19" t="s">
+        <v>241</v>
+      </c>
+      <c r="D2" s="19" t="s">
         <v>242</v>
-      </c>
-      <c r="D2" s="24" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="3" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -4704,27 +4733,27 @@
         <v>128</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>244</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="19">
+        <v>129</v>
+      </c>
+      <c r="C4" s="19" t="s">
         <v>245</v>
       </c>
-      <c r="E3" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="24">
-        <v>129</v>
-      </c>
-      <c r="C4" s="24" t="s">
-        <v>246</v>
-      </c>
-      <c r="D4" s="24" t="s">
-        <v>245</v>
+      <c r="D4" s="19" t="s">
+        <v>244</v>
       </c>
       <c r="E4" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="5" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -4732,13 +4761,13 @@
         <v>130</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E5" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="6" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -4746,97 +4775,97 @@
         <v>131</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D6" s="3">
         <v>44088</v>
       </c>
       <c r="E6" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="7" spans="2:6" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="4">
         <v>132</v>
       </c>
-      <c r="C7" s="99" t="s">
+      <c r="C7" s="52" t="s">
+        <v>248</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>249</v>
       </c>
-      <c r="D7" s="4" t="s">
-        <v>250</v>
-      </c>
       <c r="E7" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="8" spans="2:6" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="2">
         <v>133</v>
       </c>
-      <c r="C8" s="99" t="s">
-        <v>251</v>
+      <c r="C8" s="52" t="s">
+        <v>250</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E8" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="9" spans="2:6" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="4">
         <v>134</v>
       </c>
-      <c r="C9" s="99" t="s">
-        <v>252</v>
+      <c r="C9" s="52" t="s">
+        <v>251</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E9" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="10" spans="2:6" ht="50.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="2">
         <v>135</v>
       </c>
-      <c r="C10" s="99" t="s">
+      <c r="C10" s="52" t="s">
+        <v>252</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>254</v>
-      </c>
       <c r="E10" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="11" spans="2:6" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="4">
         <v>136</v>
       </c>
-      <c r="C11" s="99" t="s">
+      <c r="C11" s="52" t="s">
+        <v>254</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>255</v>
       </c>
-      <c r="D11" s="4" t="s">
-        <v>256</v>
-      </c>
       <c r="E11" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="12" spans="2:6" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="2">
         <v>137</v>
       </c>
-      <c r="C12" s="99" t="s">
+      <c r="C12" s="52" t="s">
+        <v>256</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>258</v>
-      </c>
       <c r="E12" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
   </sheetData>

</xml_diff>